<commit_message>
Adjustment to $RBLX Q3 projection rev growth
</commit_message>
<xml_diff>
--- a/$RBLX.xlsx
+++ b/$RBLX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7249BD-EC2D-9D4F-85D8-0799F4FA1155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21EE986-41FE-403C-824E-0F8C29A11E1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18880" xr2:uid="{DB6ABC51-E0DE-6747-8CA5-53C172A4844D}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18885" activeTab="1" xr2:uid="{DB6ABC51-E0DE-6747-8CA5-53C172A4844D}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,22 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="218">
   <si>
     <t>Price</t>
   </si>
@@ -698,8 +688,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="10">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="#,##0.000"/>
@@ -1218,7 +1208,7 @@
     <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="239">
@@ -1344,8 +1334,8 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1429,7 +1419,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1559,7 +1549,7 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="36" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="17" fontId="37" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1666,6 +1656,21 @@
     <xf numFmtId="165" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1675,58 +1680,43 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="172" fontId="19" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="172" fontId="19" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1736,7 +1726,7 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1760,7 +1750,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3751,54 +3741,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE4A73D-2F46-7341-9C57-6E5B7A39A15C}">
   <dimension ref="B1:AI68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH11" sqref="AH11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="6"/>
-    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.375" style="6" customWidth="1"/>
     <col min="3" max="8" width="9" style="6"/>
     <col min="9" max="9" width="9" style="6" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="9.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="20" width="9.1640625" style="6" customWidth="1"/>
-    <col min="21" max="21" width="9.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="9.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="20" width="9.125" style="6" customWidth="1"/>
+    <col min="21" max="21" width="9.125" style="6" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="L1" s="236" t="s">
+    <row r="1" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="L1" s="230" t="s">
         <v>125</v>
       </c>
-      <c r="M1" s="237"/>
-      <c r="N1" s="237"/>
-      <c r="O1" s="237"/>
-      <c r="P1" s="237"/>
-      <c r="Q1" s="237"/>
-      <c r="R1" s="237"/>
-      <c r="S1" s="238"/>
-      <c r="U1" s="232" t="s">
+      <c r="M1" s="231"/>
+      <c r="N1" s="231"/>
+      <c r="O1" s="231"/>
+      <c r="P1" s="231"/>
+      <c r="Q1" s="231"/>
+      <c r="R1" s="231"/>
+      <c r="S1" s="232"/>
+      <c r="U1" s="218" t="s">
         <v>127</v>
       </c>
-      <c r="V1" s="233"/>
-      <c r="W1" s="233"/>
-      <c r="X1" s="233"/>
-      <c r="Y1" s="233"/>
-      <c r="Z1" s="233"/>
-      <c r="AA1" s="233"/>
-      <c r="AB1" s="233"/>
-      <c r="AC1" s="233"/>
-      <c r="AD1" s="233"/>
-      <c r="AE1" s="233"/>
-      <c r="AF1" s="233"/>
-      <c r="AG1" s="233"/>
-      <c r="AH1" s="233"/>
-      <c r="AI1" s="234"/>
-    </row>
-    <row r="2" spans="2:35" ht="19" x14ac:dyDescent="0.25">
+      <c r="V1" s="219"/>
+      <c r="W1" s="219"/>
+      <c r="X1" s="219"/>
+      <c r="Y1" s="219"/>
+      <c r="Z1" s="219"/>
+      <c r="AA1" s="219"/>
+      <c r="AB1" s="219"/>
+      <c r="AC1" s="219"/>
+      <c r="AD1" s="219"/>
+      <c r="AE1" s="219"/>
+      <c r="AF1" s="219"/>
+      <c r="AG1" s="219"/>
+      <c r="AH1" s="219"/>
+      <c r="AI1" s="220"/>
+    </row>
+    <row r="2" spans="2:35" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>57</v>
       </c>
@@ -3824,7 +3814,7 @@
         <v>44788</v>
       </c>
     </row>
-    <row r="3" spans="2:35" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="46" t="s">
         <v>111</v>
       </c>
@@ -3902,7 +3892,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:35" x14ac:dyDescent="0.25">
       <c r="J4" s="31" t="s">
         <v>87</v>
       </c>
@@ -3976,17 +3966,17 @@
         <v>52.2</v>
       </c>
     </row>
-    <row r="5" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B5" s="218" t="s">
+    <row r="5" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B5" s="223" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="219"/>
-      <c r="D5" s="220"/>
-      <c r="F5" s="218" t="s">
+      <c r="C5" s="224"/>
+      <c r="D5" s="225"/>
+      <c r="F5" s="223" t="s">
         <v>193</v>
       </c>
-      <c r="G5" s="219"/>
-      <c r="H5" s="220"/>
+      <c r="G5" s="224"/>
+      <c r="H5" s="225"/>
       <c r="K5" s="28" t="s">
         <v>73</v>
       </c>
@@ -4073,7 +4063,7 @@
         <v>-3.512014787430684E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B6" s="40" t="s">
         <v>0</v>
       </c>
@@ -4084,10 +4074,10 @@
       <c r="F6" s="181" t="s">
         <v>194</v>
       </c>
-      <c r="G6" s="235" t="s">
+      <c r="G6" s="226" t="s">
         <v>198</v>
       </c>
-      <c r="H6" s="224"/>
+      <c r="H6" s="222"/>
       <c r="K6" s="28" t="s">
         <v>74</v>
       </c>
@@ -4169,7 +4159,7 @@
         <v>0.20833333333333326</v>
       </c>
     </row>
-    <row r="7" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B7" s="40" t="s">
         <v>1</v>
       </c>
@@ -4182,10 +4172,10 @@
       <c r="F7" s="181" t="s">
         <v>195</v>
       </c>
-      <c r="G7" s="223">
+      <c r="G7" s="227">
         <v>2004</v>
       </c>
-      <c r="H7" s="224"/>
+      <c r="H7" s="222"/>
       <c r="K7" s="28"/>
       <c r="L7" s="61"/>
       <c r="M7" s="61"/>
@@ -4212,7 +4202,7 @@
       <c r="AH7" s="24"/>
       <c r="AI7" s="24"/>
     </row>
-    <row r="8" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B8" s="40" t="s">
         <v>2</v>
       </c>
@@ -4224,11 +4214,11 @@
       <c r="F8" s="181" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="223">
+      <c r="G8" s="227">
         <f>AI4</f>
         <v>52.2</v>
       </c>
-      <c r="H8" s="224"/>
+      <c r="H8" s="222"/>
       <c r="K8" s="28" t="s">
         <v>75</v>
       </c>
@@ -4298,7 +4288,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="9" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B9" s="40" t="s">
         <v>3</v>
       </c>
@@ -4309,8 +4299,8 @@
         <v>13</v>
       </c>
       <c r="F9" s="167"/>
-      <c r="G9" s="223"/>
-      <c r="H9" s="224"/>
+      <c r="G9" s="227"/>
+      <c r="H9" s="222"/>
       <c r="K9" s="28" t="s">
         <v>77</v>
       </c>
@@ -4393,7 +4383,7 @@
       </c>
       <c r="AI9" s="24"/>
     </row>
-    <row r="10" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B10" s="40" t="s">
         <v>4</v>
       </c>
@@ -4404,8 +4394,8 @@
         <v>13</v>
       </c>
       <c r="F10" s="167"/>
-      <c r="G10" s="223"/>
-      <c r="H10" s="224"/>
+      <c r="G10" s="227"/>
+      <c r="H10" s="222"/>
       <c r="K10" s="28" t="s">
         <v>78</v>
       </c>
@@ -4485,7 +4475,7 @@
       </c>
       <c r="AI10" s="160"/>
     </row>
-    <row r="11" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B11" s="40" t="s">
         <v>7</v>
       </c>
@@ -4499,10 +4489,10 @@
       <c r="F11" s="181" t="s">
         <v>199</v>
       </c>
-      <c r="G11" s="235" t="s">
+      <c r="G11" s="226" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="224"/>
+      <c r="H11" s="222"/>
       <c r="K11" s="28"/>
       <c r="L11" s="61"/>
       <c r="M11" s="61"/>
@@ -4518,7 +4508,7 @@
       <c r="AH11" s="161"/>
       <c r="AI11" s="161"/>
     </row>
-    <row r="12" spans="2:35" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="42" t="s">
         <v>5</v>
       </c>
@@ -4530,10 +4520,10 @@
       <c r="F12" s="182" t="s">
         <v>196</v>
       </c>
-      <c r="G12" s="227" t="s">
+      <c r="G12" s="228" t="s">
         <v>197</v>
       </c>
-      <c r="H12" s="228"/>
+      <c r="H12" s="229"/>
       <c r="K12" s="28" t="s">
         <v>76</v>
       </c>
@@ -4603,7 +4593,7 @@
         <v>28.3</v>
       </c>
     </row>
-    <row r="13" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:35" x14ac:dyDescent="0.25">
       <c r="K13" s="28" t="s">
         <v>79</v>
       </c>
@@ -4686,7 +4676,7 @@
       </c>
       <c r="AI13" s="24"/>
     </row>
-    <row r="14" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:35" x14ac:dyDescent="0.25">
       <c r="K14" s="28" t="s">
         <v>80</v>
       </c>
@@ -4766,17 +4756,17 @@
       </c>
       <c r="AI14" s="33"/>
     </row>
-    <row r="15" spans="2:35" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="218" t="s">
+    <row r="15" spans="2:35" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="223" t="s">
         <v>130</v>
       </c>
-      <c r="C15" s="219"/>
-      <c r="D15" s="220"/>
-      <c r="F15" s="218" t="s">
+      <c r="C15" s="224"/>
+      <c r="D15" s="225"/>
+      <c r="F15" s="223" t="s">
         <v>204</v>
       </c>
-      <c r="G15" s="219"/>
-      <c r="H15" s="220"/>
+      <c r="G15" s="224"/>
+      <c r="H15" s="225"/>
       <c r="K15" s="28"/>
       <c r="L15" s="63"/>
       <c r="M15" s="63"/>
@@ -4787,22 +4777,22 @@
       <c r="R15" s="63"/>
       <c r="S15" s="63"/>
     </row>
-    <row r="16" spans="2:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="93" t="s">
         <v>132</v>
       </c>
-      <c r="C16" s="231" t="s">
+      <c r="C16" s="221" t="s">
         <v>131</v>
       </c>
-      <c r="D16" s="224"/>
+      <c r="D16" s="222"/>
       <c r="F16" s="181" t="s">
         <v>205</v>
       </c>
-      <c r="G16" s="225">
+      <c r="G16" s="235">
         <f>C6/'Financial Model'!L61</f>
         <v>39.924974402465928</v>
       </c>
-      <c r="H16" s="226"/>
+      <c r="H16" s="236"/>
       <c r="J16" s="31" t="s">
         <v>86</v>
       </c>
@@ -4877,22 +4867,22 @@
         <v>11300</v>
       </c>
     </row>
-    <row r="17" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B17" s="105" t="s">
         <v>164</v>
       </c>
-      <c r="C17" s="221" t="s">
+      <c r="C17" s="233" t="s">
         <v>165</v>
       </c>
-      <c r="D17" s="222"/>
+      <c r="D17" s="234"/>
       <c r="F17" s="181" t="s">
         <v>215</v>
       </c>
-      <c r="G17" s="225">
+      <c r="G17" s="235">
         <f>C8/'Financial Model'!W3</f>
         <v>11.475129359867568</v>
       </c>
-      <c r="H17" s="226"/>
+      <c r="H17" s="236"/>
       <c r="K17" s="28" t="s">
         <v>84</v>
       </c>
@@ -4977,19 +4967,19 @@
         <v>-6.7361276179911944E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B18" s="93" t="s">
         <v>133</v>
       </c>
-      <c r="C18" s="231" t="s">
+      <c r="C18" s="221" t="s">
         <v>134</v>
       </c>
-      <c r="D18" s="224"/>
+      <c r="D18" s="222"/>
       <c r="F18" s="181" t="s">
         <v>216</v>
       </c>
-      <c r="G18" s="223"/>
-      <c r="H18" s="224"/>
+      <c r="G18" s="227"/>
+      <c r="H18" s="222"/>
       <c r="K18" s="28" t="s">
         <v>85</v>
       </c>
@@ -5071,24 +5061,24 @@
         <v>0.16040254672417342</v>
       </c>
     </row>
-    <row r="19" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B19" s="91"/>
-      <c r="C19" s="223"/>
-      <c r="D19" s="224"/>
+      <c r="C19" s="227"/>
+      <c r="D19" s="222"/>
       <c r="F19" s="181"/>
-      <c r="G19" s="223"/>
-      <c r="H19" s="224"/>
+      <c r="G19" s="227"/>
+      <c r="H19" s="222"/>
       <c r="K19" s="28"/>
       <c r="L19" s="63"/>
       <c r="M19" s="63"/>
     </row>
-    <row r="20" spans="2:35" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="92"/>
-      <c r="C20" s="229"/>
-      <c r="D20" s="230"/>
+      <c r="C20" s="237"/>
+      <c r="D20" s="238"/>
       <c r="F20" s="182"/>
-      <c r="G20" s="227"/>
-      <c r="H20" s="228"/>
+      <c r="G20" s="228"/>
+      <c r="H20" s="229"/>
       <c r="J20" s="31"/>
       <c r="K20" s="200" t="s">
         <v>214</v>
@@ -5108,30 +5098,30 @@
       <c r="AF20" s="1"/>
       <c r="AG20" s="1"/>
     </row>
-    <row r="21" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:35" x14ac:dyDescent="0.25">
       <c r="K21" s="200" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="22" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:35" x14ac:dyDescent="0.25">
       <c r="K22" s="200" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="23" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="B23" s="218" t="s">
+    <row r="23" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B23" s="223" t="s">
         <v>159</v>
       </c>
-      <c r="C23" s="219"/>
-      <c r="D23" s="219"/>
-      <c r="E23" s="219"/>
-      <c r="F23" s="219"/>
-      <c r="G23" s="220"/>
+      <c r="C23" s="224"/>
+      <c r="D23" s="224"/>
+      <c r="E23" s="224"/>
+      <c r="F23" s="224"/>
+      <c r="G23" s="225"/>
       <c r="K23" s="200" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="24" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B24" s="108" t="s">
         <v>169</v>
       </c>
@@ -5144,7 +5134,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="25" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B25" s="108" t="s">
         <v>170</v>
       </c>
@@ -5160,7 +5150,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B26" s="98"/>
       <c r="C26" s="96"/>
       <c r="D26" s="96"/>
@@ -5174,7 +5164,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="27" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B27" s="98" t="s">
         <v>149</v>
       </c>
@@ -5190,7 +5180,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="28" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B28" s="95" t="s">
         <v>162</v>
       </c>
@@ -5200,7 +5190,7 @@
       <c r="F28" s="99"/>
       <c r="G28" s="97"/>
     </row>
-    <row r="29" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B29" s="104" t="s">
         <v>163</v>
       </c>
@@ -5216,7 +5206,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="30" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B30" s="95" t="s">
         <v>161</v>
       </c>
@@ -5228,7 +5218,7 @@
       <c r="J30" s="94"/>
       <c r="K30" s="94"/>
     </row>
-    <row r="31" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B31" s="100" t="s">
         <v>150</v>
       </c>
@@ -5238,14 +5228,14 @@
       <c r="F31" s="102"/>
       <c r="G31" s="103"/>
       <c r="J31" s="7"/>
-      <c r="K31" s="218" t="s">
+      <c r="K31" s="223" t="s">
         <v>181</v>
       </c>
-      <c r="L31" s="219"/>
-      <c r="M31" s="219"/>
-      <c r="N31" s="220"/>
-    </row>
-    <row r="32" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="L31" s="224"/>
+      <c r="M31" s="224"/>
+      <c r="N31" s="225"/>
+    </row>
+    <row r="32" spans="2:35" x14ac:dyDescent="0.25">
       <c r="J32" s="7"/>
       <c r="K32" s="173" t="s">
         <v>176</v>
@@ -5254,15 +5244,15 @@
       <c r="M32" s="96"/>
       <c r="N32" s="97"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B33" s="218" t="s">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B33" s="223" t="s">
         <v>187</v>
       </c>
-      <c r="C33" s="219"/>
-      <c r="D33" s="219"/>
-      <c r="E33" s="219"/>
-      <c r="F33" s="219"/>
-      <c r="G33" s="220"/>
+      <c r="C33" s="224"/>
+      <c r="D33" s="224"/>
+      <c r="E33" s="224"/>
+      <c r="F33" s="224"/>
+      <c r="G33" s="225"/>
       <c r="J33" s="7"/>
       <c r="K33" s="173" t="s">
         <v>177</v>
@@ -5273,7 +5263,7 @@
       <c r="M33" s="170"/>
       <c r="N33" s="97"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="209">
         <v>44743</v>
       </c>
@@ -5294,7 +5284,7 @@
       <c r="M34" s="171"/>
       <c r="N34" s="97"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="167"/>
       <c r="C35" s="211" t="s">
         <v>208</v>
@@ -5315,7 +5305,7 @@
       <c r="M35" s="172"/>
       <c r="N35" s="97"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="167"/>
       <c r="C36" s="96"/>
       <c r="D36" s="96"/>
@@ -5330,7 +5320,7 @@
       <c r="M36" s="96"/>
       <c r="N36" s="97"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="167"/>
       <c r="C37" s="96"/>
       <c r="D37" s="96"/>
@@ -5345,7 +5335,7 @@
       <c r="M37" s="96"/>
       <c r="N37" s="97"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="167"/>
       <c r="C38" s="96"/>
       <c r="D38" s="96"/>
@@ -5360,7 +5350,7 @@
       <c r="M38" s="96"/>
       <c r="N38" s="97"/>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" s="167"/>
       <c r="C39" s="96"/>
       <c r="D39" s="96"/>
@@ -5375,7 +5365,7 @@
       <c r="M39" s="96"/>
       <c r="N39" s="97"/>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" s="178">
         <v>44682</v>
       </c>
@@ -5396,7 +5386,7 @@
       <c r="M40" s="96"/>
       <c r="N40" s="97"/>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" s="167"/>
       <c r="C41" s="177" t="s">
         <v>188</v>
@@ -5413,7 +5403,7 @@
       <c r="M41" s="96"/>
       <c r="N41" s="97"/>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" s="168"/>
       <c r="C42" s="101"/>
       <c r="D42" s="101"/>
@@ -5426,7 +5416,7 @@
       <c r="M42" s="96"/>
       <c r="N42" s="97"/>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J43" s="7"/>
       <c r="K43" s="180" t="s">
         <v>191</v>
@@ -5437,7 +5427,7 @@
       <c r="M43" s="96"/>
       <c r="N43" s="97"/>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J44" s="7"/>
       <c r="K44" s="174" t="s">
         <v>154</v>
@@ -5446,7 +5436,7 @@
       <c r="M44" s="96"/>
       <c r="N44" s="97"/>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B45" s="215" t="s">
         <v>217</v>
       </c>
@@ -5458,7 +5448,7 @@
       <c r="M45" s="96"/>
       <c r="N45" s="97"/>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J46" s="7"/>
       <c r="K46" s="174" t="s">
         <v>156</v>
@@ -5467,7 +5457,7 @@
       <c r="M46" s="96"/>
       <c r="N46" s="97"/>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J47" s="7"/>
       <c r="K47" s="174" t="s">
         <v>157</v>
@@ -5476,7 +5466,7 @@
       <c r="M47" s="96"/>
       <c r="N47" s="97"/>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J48" s="7"/>
       <c r="K48" s="176" t="s">
         <v>158</v>
@@ -5485,99 +5475,88 @@
       <c r="M48" s="101"/>
       <c r="N48" s="103"/>
     </row>
-    <row r="51" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K51" s="20" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K52" s="21" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K53" s="21" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K54" s="21" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="11:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="11:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K55" s="22" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="11:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="11:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K56" s="22" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="11:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="11:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K57" s="22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K58" s="90" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="61" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K61" s="106" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="62" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K62" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="63" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K63" s="87" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="64" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K64" s="94" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="65" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K65" s="94" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="66" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K66" s="94" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="67" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K67" s="94" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="68" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K68" s="94" t="s">
         <v>147</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="U1:AI1"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="L1:S1"/>
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="K31:N31"/>
     <mergeCell ref="B5:D5"/>
@@ -5593,6 +5572,17 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C16:D16"/>
+    <mergeCell ref="U1:AI1"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="L1:S1"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <hyperlinks>
@@ -5610,39 +5600,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0FDCAC-3416-844A-BCBB-390EC350CF59}">
   <dimension ref="B1:BZ73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
+      <selection pane="bottomRight" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="6" customWidth="1"/>
-    <col min="2" max="2" width="29.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="9.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.1640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="29.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.125" customWidth="1"/>
+    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="9.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.125" style="7" customWidth="1"/>
     <col min="13" max="14" width="9" style="7"/>
     <col min="15" max="16" width="9" style="6"/>
     <col min="17" max="18" width="9" style="7"/>
     <col min="19" max="21" width="9" style="6"/>
     <col min="22" max="22" width="10.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.125" style="6" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="9" style="6"/>
     <col min="25" max="25" width="9" style="6" bestFit="1" customWidth="1"/>
     <col min="26" max="40" width="9" style="6"/>
-    <col min="41" max="41" width="15.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.875" style="6" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="10" style="6" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="9" style="6"/>
-    <col min="44" max="44" width="10.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.125" style="6" bestFit="1" customWidth="1"/>
     <col min="45" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="C1" s="2" t="s">
         <v>67</v>
       </c>
@@ -5746,7 +5736,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="2:39" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:39" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C2" s="34">
         <v>43921</v>
       </c>
@@ -5844,7 +5834,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="2:39" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:39" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
@@ -5879,8 +5869,8 @@
         <v>591.20699999999999</v>
       </c>
       <c r="M3" s="118">
-        <f>I3*1.15</f>
-        <v>585.7364</v>
+        <f>I3*1.25</f>
+        <v>636.67000000000007</v>
       </c>
       <c r="N3" s="4">
         <f>J3*1.15</f>
@@ -5905,70 +5895,70 @@
       </c>
       <c r="X3" s="129">
         <f>SUM(K3:N3)</f>
-        <v>2368.1617499999998</v>
+        <v>2419.0953500000001</v>
       </c>
       <c r="Y3" s="3">
         <f>X3*1.15</f>
-        <v>2723.3860124999997</v>
+        <v>2781.9596524999997</v>
       </c>
       <c r="Z3" s="3">
         <f t="shared" ref="Z3:AK3" si="0">Y3*1.15</f>
-        <v>3131.8939143749994</v>
+        <v>3199.2536003749992</v>
       </c>
       <c r="AA3" s="3">
         <f t="shared" si="0"/>
-        <v>3601.6780015312493</v>
+        <v>3679.141640431249</v>
       </c>
       <c r="AB3" s="3">
         <f t="shared" si="0"/>
-        <v>4141.929701760936</v>
+        <v>4231.0128864959361</v>
       </c>
       <c r="AC3" s="3">
         <f t="shared" si="0"/>
-        <v>4763.2191570250761</v>
+        <v>4865.6648194703257</v>
       </c>
       <c r="AD3" s="3">
         <f t="shared" si="0"/>
-        <v>5477.7020305788374</v>
+        <v>5595.5145423908743</v>
       </c>
       <c r="AE3" s="3">
         <f t="shared" si="0"/>
-        <v>6299.3573351656623</v>
+        <v>6434.841723749505</v>
       </c>
       <c r="AF3" s="3">
         <f t="shared" si="0"/>
-        <v>7244.2609354405113</v>
+        <v>7400.0679823119299</v>
       </c>
       <c r="AG3" s="3">
         <f t="shared" si="0"/>
-        <v>8330.9000757565882</v>
+        <v>8510.078179658718</v>
       </c>
       <c r="AH3" s="3">
         <f t="shared" si="0"/>
-        <v>9580.5350871200753</v>
+        <v>9786.5899066075253</v>
       </c>
       <c r="AI3" s="3">
         <f t="shared" si="0"/>
-        <v>11017.615350188085</v>
+        <v>11254.578392598652</v>
       </c>
       <c r="AJ3" s="3">
         <f t="shared" si="0"/>
-        <v>12670.257652716296</v>
+        <v>12942.765151488449</v>
       </c>
       <c r="AK3" s="3">
         <f t="shared" si="0"/>
-        <v>14570.796300623741</v>
+        <v>14884.179924211716</v>
       </c>
       <c r="AL3" s="3">
         <f t="shared" ref="AL3:AM3" si="1">AK3*1.15</f>
-        <v>16756.415745717299</v>
+        <v>17116.806912843473</v>
       </c>
       <c r="AM3" s="3">
         <f t="shared" si="1"/>
-        <v>19269.878107574892</v>
-      </c>
-    </row>
-    <row r="4" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+        <v>19684.327949769991</v>
+      </c>
+    </row>
+    <row r="4" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>34</v>
       </c>
@@ -6004,7 +5994,7 @@
       </c>
       <c r="M4" s="119">
         <f t="shared" ref="M4:N4" si="2">M3-M5</f>
-        <v>152.29146400000002</v>
+        <v>165.5342</v>
       </c>
       <c r="N4" s="5">
         <f t="shared" si="2"/>
@@ -6029,70 +6019,70 @@
       </c>
       <c r="X4" s="130">
         <f>SUM(K4:N4)</f>
-        <v>601.14239500000008</v>
+        <v>614.385131</v>
       </c>
       <c r="Y4" s="9">
         <f>Y3-Y5</f>
-        <v>735.31422337499998</v>
+        <v>751.12910617500006</v>
       </c>
       <c r="Z4" s="9">
         <f t="shared" ref="Z4:AK4" si="3">Z3-Z5</f>
-        <v>845.61135688124978</v>
+        <v>863.7984721012499</v>
       </c>
       <c r="AA4" s="9">
         <f t="shared" si="3"/>
-        <v>972.45306041343747</v>
+        <v>993.36824291643734</v>
       </c>
       <c r="AB4" s="9">
         <f t="shared" si="3"/>
-        <v>1118.3210194754529</v>
+        <v>1142.3734793539029</v>
       </c>
       <c r="AC4" s="9">
         <f t="shared" si="3"/>
-        <v>1286.0691723967707</v>
+        <v>1313.729501256988</v>
       </c>
       <c r="AD4" s="9">
         <f t="shared" si="3"/>
-        <v>1478.9795482562863</v>
+        <v>1510.7889264455362</v>
       </c>
       <c r="AE4" s="9">
         <f t="shared" si="3"/>
-        <v>1700.8264804947294</v>
+        <v>1737.4072654123665</v>
       </c>
       <c r="AF4" s="9">
         <f t="shared" si="3"/>
-        <v>1955.9504525689381</v>
+        <v>1998.0183552242215</v>
       </c>
       <c r="AG4" s="9">
         <f t="shared" si="3"/>
-        <v>2249.3430204542792</v>
+        <v>2297.7211085078543</v>
       </c>
       <c r="AH4" s="9">
         <f t="shared" si="3"/>
-        <v>2586.7444735224208</v>
+        <v>2642.3792747840316</v>
       </c>
       <c r="AI4" s="9">
         <f t="shared" si="3"/>
-        <v>2974.7561445507836</v>
+        <v>3038.7361660016359</v>
       </c>
       <c r="AJ4" s="9">
         <f t="shared" si="3"/>
-        <v>3420.9695662333997</v>
+        <v>3494.5465909018822</v>
       </c>
       <c r="AK4" s="9">
         <f t="shared" si="3"/>
-        <v>3934.1150011684094</v>
+        <v>4018.7285795371627</v>
       </c>
       <c r="AL4" s="9">
         <f t="shared" ref="AL4" si="4">AL3-AL5</f>
-        <v>4524.2322513436702</v>
+        <v>4621.5378664677373</v>
       </c>
       <c r="AM4" s="9">
         <f t="shared" ref="AM4" si="5">AM3-AM5</f>
-        <v>5202.8670890452213</v>
-      </c>
-    </row>
-    <row r="5" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+        <v>5314.7685464378974</v>
+      </c>
+    </row>
+    <row r="5" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
@@ -6138,7 +6128,7 @@
       </c>
       <c r="M5" s="120">
         <f>M3*0.74</f>
-        <v>433.44493599999998</v>
+        <v>471.13580000000007</v>
       </c>
       <c r="N5" s="57">
         <f>N3*0.74</f>
@@ -6167,70 +6157,70 @@
       </c>
       <c r="X5" s="129">
         <f>X3-X4</f>
-        <v>1767.0193549999997</v>
+        <v>1804.7102190000001</v>
       </c>
       <c r="Y5" s="58">
         <f>Y3*0.73</f>
-        <v>1988.0717891249997</v>
+        <v>2030.8305463249997</v>
       </c>
       <c r="Z5" s="58">
         <f t="shared" ref="Z5:AK5" si="8">Z3*0.73</f>
-        <v>2286.2825574937497</v>
+        <v>2335.4551282737493</v>
       </c>
       <c r="AA5" s="58">
         <f t="shared" si="8"/>
-        <v>2629.2249411178118</v>
+        <v>2685.7733975148117</v>
       </c>
       <c r="AB5" s="58">
         <f t="shared" si="8"/>
-        <v>3023.6086822854832</v>
+        <v>3088.6394071420332</v>
       </c>
       <c r="AC5" s="58">
         <f t="shared" si="8"/>
-        <v>3477.1499846283054</v>
+        <v>3551.9353182133377</v>
       </c>
       <c r="AD5" s="58">
         <f t="shared" si="8"/>
-        <v>3998.7224823225511</v>
+        <v>4084.7256159453382</v>
       </c>
       <c r="AE5" s="58">
         <f t="shared" si="8"/>
-        <v>4598.530854670933</v>
+        <v>4697.4344583371385</v>
       </c>
       <c r="AF5" s="58">
         <f t="shared" si="8"/>
-        <v>5288.3104828715732</v>
+        <v>5402.0496270877084</v>
       </c>
       <c r="AG5" s="58">
         <f t="shared" si="8"/>
-        <v>6081.557055302309</v>
+        <v>6212.3570711508637</v>
       </c>
       <c r="AH5" s="58">
         <f t="shared" si="8"/>
-        <v>6993.7906135976546</v>
+        <v>7144.2106318234937</v>
       </c>
       <c r="AI5" s="58">
         <f t="shared" si="8"/>
-        <v>8042.8592056373018</v>
+        <v>8215.8422265970166</v>
       </c>
       <c r="AJ5" s="58">
         <f t="shared" si="8"/>
-        <v>9249.2880864828967</v>
+        <v>9448.218560586567</v>
       </c>
       <c r="AK5" s="58">
         <f t="shared" si="8"/>
-        <v>10636.681299455331</v>
+        <v>10865.451344674553</v>
       </c>
       <c r="AL5" s="58">
         <f t="shared" ref="AL5:AM5" si="9">AL3*0.73</f>
-        <v>12232.183494373628</v>
+        <v>12495.269046375735</v>
       </c>
       <c r="AM5" s="58">
         <f t="shared" si="9"/>
-        <v>14067.011018529671</v>
-      </c>
-    </row>
-    <row r="6" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+        <v>14369.559403332094</v>
+      </c>
+    </row>
+    <row r="6" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>18</v>
       </c>
@@ -6356,7 +6346,7 @@
         <v>779.38135538082281</v>
       </c>
     </row>
-    <row r="7" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>19</v>
       </c>
@@ -6481,7 +6471,7 @@
         <v>1412.9518528496542</v>
       </c>
     </row>
-    <row r="8" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>20</v>
       </c>
@@ -6606,7 +6596,7 @@
         <v>755.81141808473603</v>
       </c>
     </row>
-    <row r="9" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>21</v>
       </c>
@@ -6731,7 +6721,7 @@
         <v>254.90376657199999</v>
       </c>
     </row>
-    <row r="10" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>22</v>
       </c>
@@ -6855,7 +6845,7 @@
         <v>56.232972727291902</v>
       </c>
     </row>
-    <row r="11" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>23</v>
       </c>
@@ -6989,7 +6979,7 @@
         <v>3259.2813656145045</v>
       </c>
     </row>
-    <row r="12" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>28</v>
       </c>
@@ -7035,7 +7025,7 @@
       </c>
       <c r="M12" s="118">
         <f t="shared" si="28"/>
-        <v>-165.15242192800008</v>
+        <v>-127.46155792799999</v>
       </c>
       <c r="N12" s="4">
         <f t="shared" si="28"/>
@@ -7060,70 +7050,70 @@
       </c>
       <c r="X12" s="118">
         <f>X5-X11</f>
-        <v>-668.11633740673619</v>
+        <v>-630.42547340673582</v>
       </c>
       <c r="Y12" s="4">
         <f t="shared" ref="Y12:AK12" si="29">Y5-Y11</f>
-        <v>-484.32858564423577</v>
+        <v>-441.56982844423578</v>
       </c>
       <c r="Z12" s="4">
         <f t="shared" si="29"/>
-        <v>-225.52534013611103</v>
+        <v>-176.35276935611137</v>
       </c>
       <c r="AA12" s="4">
         <f t="shared" si="29"/>
-        <v>75.79479158486356</v>
+        <v>132.34324798186344</v>
       </c>
       <c r="AB12" s="4">
         <f t="shared" si="29"/>
-        <v>426.26462525882562</v>
+        <v>491.29535011537564</v>
       </c>
       <c r="AC12" s="4">
         <f t="shared" si="29"/>
-        <v>833.5182250304365</v>
+        <v>908.30355861546877</v>
       </c>
       <c r="AD12" s="4">
         <f t="shared" si="29"/>
-        <v>1306.3416851922539</v>
+        <v>1392.344818815041</v>
       </c>
       <c r="AE12" s="4">
         <f t="shared" si="29"/>
-        <v>1854.8465443488594</v>
+        <v>1953.750148015065</v>
       </c>
       <c r="AF12" s="4">
         <f t="shared" si="29"/>
-        <v>2490.669228341214</v>
+        <v>2604.4083725573491</v>
       </c>
       <c r="AG12" s="4">
         <f t="shared" si="29"/>
-        <v>3227.2004277593942</v>
+        <v>3358.0004436079489</v>
       </c>
       <c r="AH12" s="4">
         <f t="shared" si="29"/>
-        <v>4079.8489017875436</v>
+        <v>4230.2689200133827</v>
       </c>
       <c r="AI12" s="4">
         <f t="shared" si="29"/>
-        <v>5066.3448739316218</v>
+        <v>5239.3278948913367</v>
       </c>
       <c r="AJ12" s="4">
         <f t="shared" si="29"/>
-        <v>6207.0889600622904</v>
+        <v>6406.0194341659608</v>
       </c>
       <c r="AK12" s="4">
         <f t="shared" si="29"/>
-        <v>7525.5534603231808</v>
+        <v>7754.3235055424029</v>
       </c>
       <c r="AL12" s="4">
         <f t="shared" ref="AL12" si="30">AL5-AL11</f>
-        <v>9048.7438712445928</v>
+        <v>9311.8294232466997</v>
       </c>
       <c r="AM12" s="4">
         <f t="shared" ref="AM12" si="31">AM5-AM11</f>
-        <v>10807.729652915166</v>
-      </c>
-    </row>
-    <row r="13" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+        <v>11110.27803771759</v>
+      </c>
+    </row>
+    <row r="13" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>25</v>
       </c>
@@ -7248,7 +7238,7 @@
         <v>-6.0720532103376552</v>
       </c>
     </row>
-    <row r="14" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
         <v>93</v>
       </c>
@@ -7372,7 +7362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="39" t="s">
         <v>92</v>
       </c>
@@ -7497,7 +7487,7 @@
         <v>21.196999999999999</v>
       </c>
     </row>
-    <row r="16" spans="2:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:39" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>26</v>
       </c>
@@ -7543,7 +7533,7 @@
       </c>
       <c r="M16" s="119">
         <f t="shared" si="40"/>
-        <v>-165.8944219280001</v>
+        <v>-128.20355792799998</v>
       </c>
       <c r="N16" s="5">
         <f t="shared" si="40"/>
@@ -7568,70 +7558,70 @@
       </c>
       <c r="X16" s="119">
         <f>X12+X13+X14-X15</f>
-        <v>-694.70133740673623</v>
+        <v>-657.01047340673585</v>
       </c>
       <c r="Y16" s="5">
         <f>Y12+Y13+Y14-Y15</f>
-        <v>-510.95668964423578</v>
+        <v>-468.19793244423579</v>
       </c>
       <c r="Z16" s="5">
         <f t="shared" ref="Z16:AK16" si="42">Z12+Z13+Z14-Z15</f>
-        <v>-252.19689296811103</v>
+        <v>-203.02432218811137</v>
       </c>
       <c r="AA16" s="5">
         <f t="shared" si="42"/>
-        <v>49.079442330207556</v>
+        <v>105.62789872720744</v>
       </c>
       <c r="AB16" s="5">
         <f t="shared" si="42"/>
-        <v>399.50512921013234</v>
+        <v>464.53585406668236</v>
       </c>
       <c r="AC16" s="5">
         <f t="shared" si="42"/>
-        <v>806.7142290133537</v>
+        <v>881.49956259838598</v>
       </c>
       <c r="AD16" s="5">
         <f t="shared" si="42"/>
-        <v>1279.4928332070344</v>
+        <v>1365.4959668298216</v>
       </c>
       <c r="AE16" s="5">
         <f t="shared" si="42"/>
-        <v>1827.9524775477582</v>
+        <v>1926.8560812139638</v>
       </c>
       <c r="AF16" s="5">
         <f t="shared" si="42"/>
-        <v>2463.7295850057039</v>
+        <v>2577.4687292218391</v>
       </c>
       <c r="AG16" s="5">
         <f t="shared" si="42"/>
-        <v>3200.2148432772001</v>
+        <v>3331.0148591257548</v>
       </c>
       <c r="AH16" s="5">
         <f t="shared" si="42"/>
-        <v>4052.8170086294917</v>
+        <v>4203.2370268553314</v>
       </c>
       <c r="AI16" s="5">
         <f t="shared" si="42"/>
-        <v>5039.2663016283059</v>
+        <v>5212.2493225880207</v>
       </c>
       <c r="AJ16" s="5">
         <f t="shared" si="42"/>
-        <v>6179.9633351805478</v>
+        <v>6378.8938092842182</v>
       </c>
       <c r="AK16" s="5">
         <f t="shared" si="42"/>
-        <v>7498.3804064423839</v>
+        <v>7727.150451661606</v>
       </c>
       <c r="AL16" s="5">
         <f t="shared" ref="AL16" si="43">AL12+AL13+AL14-AL15</f>
-        <v>9021.5230089327506</v>
+        <v>9284.6085609348575</v>
       </c>
       <c r="AM16" s="5">
         <f t="shared" ref="AM16" si="44">AM12+AM13+AM14-AM15</f>
-        <v>10780.460599704829</v>
-      </c>
-    </row>
-    <row r="17" spans="2:78" ht="15" x14ac:dyDescent="0.2">
+        <v>11083.008984507253</v>
+      </c>
+    </row>
+    <row r="17" spans="2:78" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
         <v>94</v>
       </c>
@@ -7755,7 +7745,7 @@
         <v>1.1129276344999999</v>
       </c>
     </row>
-    <row r="18" spans="2:78" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:78" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>27</v>
       </c>
@@ -7801,7 +7791,7 @@
       </c>
       <c r="M18" s="118">
         <f t="shared" si="47"/>
-        <v>-166.17318882800009</v>
+        <v>-128.48232482799997</v>
       </c>
       <c r="N18" s="4">
         <f t="shared" si="47"/>
@@ -7826,226 +7816,226 @@
       </c>
       <c r="X18" s="129">
         <f>X16-X17</f>
-        <v>-695.81426504123624</v>
+        <v>-658.12340104123587</v>
       </c>
       <c r="Y18" s="3">
         <f>Y16-Y17</f>
-        <v>-512.06961727873579</v>
+        <v>-469.3108600787358</v>
       </c>
       <c r="Z18" s="3">
         <f t="shared" ref="Z18:AK18" si="49">Z16-Z17</f>
-        <v>-253.30982060261104</v>
+        <v>-204.13724982261138</v>
       </c>
       <c r="AA18" s="3">
         <f t="shared" si="49"/>
-        <v>47.966514695707559</v>
+        <v>104.51497109270744</v>
       </c>
       <c r="AB18" s="3">
         <f t="shared" si="49"/>
-        <v>398.39220157563233</v>
+        <v>463.42292643218235</v>
       </c>
       <c r="AC18" s="3">
         <f t="shared" si="49"/>
-        <v>805.60130137885369</v>
+        <v>880.38663496388597</v>
       </c>
       <c r="AD18" s="3">
         <f t="shared" si="49"/>
-        <v>1278.3799055725344</v>
+        <v>1364.3830391953215</v>
       </c>
       <c r="AE18" s="3">
         <f t="shared" si="49"/>
-        <v>1826.8395499132582</v>
+        <v>1925.7431535794638</v>
       </c>
       <c r="AF18" s="3">
         <f t="shared" si="49"/>
-        <v>2462.6166573712039</v>
+        <v>2576.3558015873391</v>
       </c>
       <c r="AG18" s="3">
         <f t="shared" si="49"/>
-        <v>3199.1019156427001</v>
+        <v>3329.9019314912548</v>
       </c>
       <c r="AH18" s="3">
         <f t="shared" si="49"/>
-        <v>4051.7040809949917</v>
+        <v>4202.1240992208313</v>
       </c>
       <c r="AI18" s="3">
         <f t="shared" si="49"/>
-        <v>5038.1533739938059</v>
+        <v>5211.1363949535207</v>
       </c>
       <c r="AJ18" s="3">
         <f t="shared" si="49"/>
-        <v>6178.8504075460478</v>
+        <v>6377.7808816497181</v>
       </c>
       <c r="AK18" s="3">
         <f t="shared" si="49"/>
-        <v>7497.2674788078839</v>
+        <v>7726.037524027106</v>
       </c>
       <c r="AL18" s="3">
         <f t="shared" ref="AL18" si="50">AL16-AL17</f>
-        <v>9020.4100812982506</v>
+        <v>9283.4956333003574</v>
       </c>
       <c r="AM18" s="3">
         <f t="shared" ref="AM18" si="51">AM16-AM17</f>
-        <v>10779.347672070329</v>
+        <v>11081.896056872753</v>
       </c>
       <c r="AN18" s="3">
         <f>AM18*(1+$AP$21)</f>
-        <v>10887.141148791032</v>
+        <v>11192.71501744148</v>
       </c>
       <c r="AO18" s="3">
         <f t="shared" ref="AO18:BZ18" si="52">AN18*(1+$AP$21)</f>
-        <v>10996.012560278943</v>
+        <v>11304.642167615895</v>
       </c>
       <c r="AP18" s="3">
         <f t="shared" si="52"/>
-        <v>11105.972685881732</v>
+        <v>11417.688589292055</v>
       </c>
       <c r="AQ18" s="3">
         <f t="shared" si="52"/>
-        <v>11217.032412740549</v>
+        <v>11531.865475184975</v>
       </c>
       <c r="AR18" s="3">
         <f t="shared" si="52"/>
-        <v>11329.202736867956</v>
+        <v>11647.184129936824</v>
       </c>
       <c r="AS18" s="3">
         <f t="shared" si="52"/>
-        <v>11442.494764236635</v>
+        <v>11763.655971236192</v>
       </c>
       <c r="AT18" s="3">
         <f t="shared" si="52"/>
-        <v>11556.919711879002</v>
+        <v>11881.292530948554</v>
       </c>
       <c r="AU18" s="3">
         <f t="shared" si="52"/>
-        <v>11672.488908997791</v>
+        <v>12000.105456258039</v>
       </c>
       <c r="AV18" s="3">
         <f t="shared" si="52"/>
-        <v>11789.213798087769</v>
+        <v>12120.10651082062</v>
       </c>
       <c r="AW18" s="3">
         <f t="shared" si="52"/>
-        <v>11907.105936068647</v>
+        <v>12241.307575928826</v>
       </c>
       <c r="AX18" s="3">
         <f t="shared" si="52"/>
-        <v>12026.176995429334</v>
+        <v>12363.720651688114</v>
       </c>
       <c r="AY18" s="3">
         <f t="shared" si="52"/>
-        <v>12146.438765383627</v>
+        <v>12487.357858204996</v>
       </c>
       <c r="AZ18" s="3">
         <f t="shared" si="52"/>
-        <v>12267.903153037463</v>
+        <v>12612.231436787046</v>
       </c>
       <c r="BA18" s="3">
         <f t="shared" si="52"/>
-        <v>12390.582184567838</v>
+        <v>12738.353751154917</v>
       </c>
       <c r="BB18" s="3">
         <f t="shared" si="52"/>
-        <v>12514.488006413518</v>
+        <v>12865.737288666465</v>
       </c>
       <c r="BC18" s="3">
         <f t="shared" si="52"/>
-        <v>12639.632886477653</v>
+        <v>12994.394661553129</v>
       </c>
       <c r="BD18" s="3">
         <f t="shared" si="52"/>
-        <v>12766.029215342431</v>
+        <v>13124.33860816866</v>
       </c>
       <c r="BE18" s="3">
         <f t="shared" si="52"/>
-        <v>12893.689507495856</v>
+        <v>13255.581994250348</v>
       </c>
       <c r="BF18" s="3">
         <f t="shared" si="52"/>
-        <v>13022.626402570815</v>
+        <v>13388.137814192851</v>
       </c>
       <c r="BG18" s="3">
         <f t="shared" si="52"/>
-        <v>13152.852666596524</v>
+        <v>13522.019192334779</v>
       </c>
       <c r="BH18" s="3">
         <f t="shared" si="52"/>
-        <v>13284.381193262489</v>
+        <v>13657.239384258128</v>
       </c>
       <c r="BI18" s="3">
         <f t="shared" si="52"/>
-        <v>13417.225005195114</v>
+        <v>13793.811778100709</v>
       </c>
       <c r="BJ18" s="3">
         <f t="shared" si="52"/>
-        <v>13551.397255247066</v>
+        <v>13931.749895881716</v>
       </c>
       <c r="BK18" s="3">
         <f t="shared" si="52"/>
-        <v>13686.911227799537</v>
+        <v>14071.067394840533</v>
       </c>
       <c r="BL18" s="3">
         <f t="shared" si="52"/>
-        <v>13823.780340077532</v>
+        <v>14211.778068788939</v>
       </c>
       <c r="BM18" s="3">
         <f t="shared" si="52"/>
-        <v>13962.018143478308</v>
+        <v>14353.895849476829</v>
       </c>
       <c r="BN18" s="3">
         <f t="shared" si="52"/>
-        <v>14101.63832491309</v>
+        <v>14497.434807971596</v>
       </c>
       <c r="BO18" s="3">
         <f t="shared" si="52"/>
-        <v>14242.654708162221</v>
+        <v>14642.409156051313</v>
       </c>
       <c r="BP18" s="3">
         <f t="shared" si="52"/>
-        <v>14385.081255243844</v>
+        <v>14788.833247611827</v>
       </c>
       <c r="BQ18" s="3">
         <f t="shared" si="52"/>
-        <v>14528.932067796282</v>
+        <v>14936.721580087946</v>
       </c>
       <c r="BR18" s="3">
         <f t="shared" si="52"/>
-        <v>14674.221388474245</v>
+        <v>15086.088795888825</v>
       </c>
       <c r="BS18" s="3">
         <f t="shared" si="52"/>
-        <v>14820.963602358988</v>
+        <v>15236.949683847713</v>
       </c>
       <c r="BT18" s="3">
         <f t="shared" si="52"/>
-        <v>14969.173238382578</v>
+        <v>15389.319180686191</v>
       </c>
       <c r="BU18" s="3">
         <f t="shared" si="52"/>
-        <v>15118.864970766404</v>
+        <v>15543.212372493053</v>
       </c>
       <c r="BV18" s="3">
         <f t="shared" si="52"/>
-        <v>15270.053620474069</v>
+        <v>15698.644496217985</v>
       </c>
       <c r="BW18" s="3">
         <f t="shared" si="52"/>
-        <v>15422.75415667881</v>
+        <v>15855.630941180165</v>
       </c>
       <c r="BX18" s="3">
         <f t="shared" si="52"/>
-        <v>15576.981698245598</v>
+        <v>16014.187250591967</v>
       </c>
       <c r="BY18" s="3">
         <f t="shared" si="52"/>
-        <v>15732.751515228054</v>
+        <v>16174.329123097887</v>
       </c>
       <c r="BZ18" s="3">
         <f t="shared" si="52"/>
-        <v>15890.079030380335</v>
-      </c>
-    </row>
-    <row r="19" spans="2:78" ht="15" x14ac:dyDescent="0.2">
+        <v>16336.072414328866</v>
+      </c>
+    </row>
+    <row r="19" spans="2:78" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>31</v>
       </c>
@@ -8090,7 +8080,7 @@
       </c>
       <c r="M19" s="124">
         <f t="shared" si="53"/>
-        <v>-0.27978675669104691</v>
+        <v>-0.21632643153378855</v>
       </c>
       <c r="N19" s="8">
         <f t="shared" si="53"/>
@@ -8115,70 +8105,70 @@
       </c>
       <c r="X19" s="124">
         <f>X18/X20</f>
-        <v>-1.1715464922368304</v>
+        <v>-1.1080861670795716</v>
       </c>
       <c r="Y19" s="35">
         <f>X19</f>
-        <v>-1.1715464922368304</v>
+        <v>-1.1080861670795716</v>
       </c>
       <c r="Z19" s="35">
         <f t="shared" ref="Z19:AK19" si="55">Y19</f>
-        <v>-1.1715464922368304</v>
+        <v>-1.1080861670795716</v>
       </c>
       <c r="AA19" s="35">
         <f t="shared" si="55"/>
-        <v>-1.1715464922368304</v>
+        <v>-1.1080861670795716</v>
       </c>
       <c r="AB19" s="35">
         <f t="shared" si="55"/>
-        <v>-1.1715464922368304</v>
+        <v>-1.1080861670795716</v>
       </c>
       <c r="AC19" s="35">
         <f t="shared" si="55"/>
-        <v>-1.1715464922368304</v>
+        <v>-1.1080861670795716</v>
       </c>
       <c r="AD19" s="35">
         <f t="shared" si="55"/>
-        <v>-1.1715464922368304</v>
+        <v>-1.1080861670795716</v>
       </c>
       <c r="AE19" s="35">
         <f t="shared" si="55"/>
-        <v>-1.1715464922368304</v>
+        <v>-1.1080861670795716</v>
       </c>
       <c r="AF19" s="35">
         <f t="shared" si="55"/>
-        <v>-1.1715464922368304</v>
+        <v>-1.1080861670795716</v>
       </c>
       <c r="AG19" s="35">
         <f t="shared" si="55"/>
-        <v>-1.1715464922368304</v>
+        <v>-1.1080861670795716</v>
       </c>
       <c r="AH19" s="35">
         <f t="shared" si="55"/>
-        <v>-1.1715464922368304</v>
+        <v>-1.1080861670795716</v>
       </c>
       <c r="AI19" s="35">
         <f t="shared" si="55"/>
-        <v>-1.1715464922368304</v>
+        <v>-1.1080861670795716</v>
       </c>
       <c r="AJ19" s="35">
         <f t="shared" si="55"/>
-        <v>-1.1715464922368304</v>
+        <v>-1.1080861670795716</v>
       </c>
       <c r="AK19" s="35">
         <f t="shared" si="55"/>
-        <v>-1.1715464922368304</v>
+        <v>-1.1080861670795716</v>
       </c>
       <c r="AL19" s="35">
         <f t="shared" ref="AL19:AM19" si="56">AK19</f>
-        <v>-1.1715464922368304</v>
+        <v>-1.1080861670795716</v>
       </c>
       <c r="AM19" s="35">
         <f t="shared" si="56"/>
-        <v>-1.1715464922368304</v>
-      </c>
-    </row>
-    <row r="20" spans="2:78" ht="15" x14ac:dyDescent="0.2">
+        <v>-1.1080861670795716</v>
+      </c>
+    </row>
+    <row r="20" spans="2:78" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>1</v>
       </c>
@@ -8300,7 +8290,7 @@
         <v>593.928</v>
       </c>
     </row>
-    <row r="21" spans="2:78" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:78" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -8317,7 +8307,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="22" spans="2:78" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:78" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>16</v>
       </c>
@@ -8388,7 +8378,7 @@
       </c>
       <c r="X22" s="126">
         <f t="shared" ref="X22:AK22" si="63">X5/X3</f>
-        <v>0.74615653048192332</v>
+        <v>0.7460269058844663</v>
       </c>
       <c r="Y22" s="10">
         <f t="shared" si="63"/>
@@ -8416,7 +8406,7 @@
       </c>
       <c r="AE22" s="10">
         <f t="shared" si="63"/>
-        <v>0.72999999999999987</v>
+        <v>0.73</v>
       </c>
       <c r="AF22" s="10">
         <f t="shared" si="63"/>
@@ -8440,7 +8430,7 @@
       </c>
       <c r="AK22" s="10">
         <f t="shared" si="63"/>
-        <v>0.73</v>
+        <v>0.73000000000000009</v>
       </c>
       <c r="AL22" s="10">
         <f t="shared" ref="AL22:AM22" si="64">AL5/AL3</f>
@@ -8458,7 +8448,7 @@
       </c>
       <c r="AR22" s="68"/>
     </row>
-    <row r="23" spans="2:78" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:78" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
         <v>24</v>
       </c>
@@ -8504,7 +8494,7 @@
       </c>
       <c r="M23" s="127">
         <f t="shared" ref="M23" si="67">M12/M3</f>
-        <v>-0.28195690404079393</v>
+        <v>-0.20020035171753023</v>
       </c>
       <c r="N23" s="14">
         <f t="shared" ref="N23" si="68">N12/N3</f>
@@ -8529,78 +8519,78 @@
       </c>
       <c r="X23" s="127">
         <f t="shared" ref="X23:AK23" si="69">X12/X3</f>
-        <v>-0.28212445260833058</v>
+        <v>-0.26060381349033462</v>
       </c>
       <c r="Y23" s="14">
         <f t="shared" si="69"/>
-        <v>-0.17784059381271272</v>
+        <v>-0.1587261799600222</v>
       </c>
       <c r="Z23" s="14">
         <f t="shared" si="69"/>
-        <v>-7.2009252644535005E-2</v>
+        <v>-5.5123097879905568E-2</v>
       </c>
       <c r="AA23" s="14">
         <f t="shared" si="69"/>
-        <v>2.1044299782667825E-2</v>
+        <v>3.597122941055101E-2</v>
       </c>
       <c r="AB23" s="14">
         <f t="shared" si="69"/>
-        <v>0.10291450023345393</v>
+        <v>0.11611766810813459</v>
       </c>
       <c r="AC23" s="14">
         <f t="shared" si="69"/>
-        <v>0.17499052585080296</v>
+        <v>0.1866761464909838</v>
       </c>
       <c r="AD23" s="14">
         <f t="shared" si="69"/>
-        <v>0.2384835242770974</v>
+        <v>0.24883231171446732</v>
       </c>
       <c r="AE23" s="14">
         <f t="shared" si="69"/>
-        <v>0.29445012334739701</v>
+        <v>0.30362054451226472</v>
       </c>
       <c r="AF23" s="14">
         <f t="shared" si="69"/>
-        <v>0.34381274370672027</v>
+        <v>0.35194384413529128</v>
       </c>
       <c r="AG23" s="14">
         <f t="shared" si="69"/>
-        <v>0.38737716194084937</v>
+        <v>0.39459102169407045</v>
       </c>
       <c r="AH23" s="14">
         <f t="shared" si="69"/>
-        <v>0.42584770732403349</v>
+        <v>0.43225157694175675</v>
       </c>
       <c r="AI23" s="14">
         <f t="shared" si="69"/>
-        <v>0.45984042035422235</v>
+        <v>0.4655285797588718</v>
       </c>
       <c r="AJ23" s="14">
         <f t="shared" si="69"/>
-        <v>0.48989445441400253</v>
+        <v>0.49494983175440321</v>
       </c>
       <c r="AK23" s="14">
         <f t="shared" si="69"/>
-        <v>0.51648196193649554</v>
+        <v>0.52097754428032961</v>
       </c>
       <c r="AL23" s="14">
         <f t="shared" ref="AL23:AM23" si="70">AL12/AL3</f>
-        <v>0.54001667233383865</v>
+        <v>0.54401673575342113</v>
       </c>
       <c r="AM23" s="14">
         <f t="shared" si="70"/>
-        <v>0.56086133978536701</v>
+        <v>0.56442252263163561</v>
       </c>
       <c r="AO23" s="146" t="s">
         <v>115</v>
       </c>
       <c r="AP23" s="141">
         <f>NPV(AP22,X18:BZ18)</f>
-        <v>96369.738915896727</v>
+        <v>99519.172695990259</v>
       </c>
       <c r="AR23" s="69"/>
     </row>
-    <row r="24" spans="2:78" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:78" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>29</v>
       </c>
@@ -8646,7 +8636,7 @@
       </c>
       <c r="M24" s="126">
         <f t="shared" ref="M24" si="73">M18/M3</f>
-        <v>-0.28369961099907753</v>
+        <v>-0.20180364211915114</v>
       </c>
       <c r="N24" s="10">
         <f t="shared" ref="N24" si="74">N18/N3</f>
@@ -8671,67 +8661,67 @@
       </c>
       <c r="X24" s="126">
         <f t="shared" ref="X24:AK24" si="75">X18/X3</f>
-        <v>-0.29382041367792394</v>
+        <v>-0.27205351828783264</v>
       </c>
       <c r="Y24" s="10">
         <f t="shared" si="75"/>
-        <v>-0.18802682209881397</v>
+        <v>-0.16869793911532505</v>
       </c>
       <c r="Z24" s="10">
         <f t="shared" si="75"/>
-        <v>-8.0880715480160681E-2</v>
+        <v>-6.3807773725310032E-2</v>
       </c>
       <c r="AA24" s="10">
         <f t="shared" si="75"/>
-        <v>1.3317824268386749E-2</v>
+        <v>2.840743339265861E-2</v>
       </c>
       <c r="AB24" s="10">
         <f t="shared" si="75"/>
-        <v>9.6185167364442811E-2</v>
+        <v>0.10953002008367375</v>
       </c>
       <c r="AC24" s="10">
         <f t="shared" si="75"/>
-        <v>0.16912958963702215</v>
+        <v>0.18093861119264776</v>
       </c>
       <c r="AD24" s="10">
         <f t="shared" si="75"/>
-        <v>0.23337886917471595</v>
+        <v>0.24383513417022457</v>
       </c>
       <c r="AE24" s="10">
         <f t="shared" si="75"/>
-        <v>0.29000411513648727</v>
+        <v>0.29926814617242153</v>
       </c>
       <c r="AF24" s="10">
         <f t="shared" si="75"/>
-        <v>0.33994035821149732</v>
+        <v>0.3481529909921765</v>
       </c>
       <c r="AG24" s="10">
         <f t="shared" si="75"/>
-        <v>0.384004355658073</v>
+        <v>0.39128922921655168</v>
       </c>
       <c r="AH24" s="10">
         <f t="shared" si="75"/>
-        <v>0.42290999867450418</v>
+        <v>0.42937572119822048</v>
       </c>
       <c r="AI24" s="10">
         <f t="shared" si="75"/>
-        <v>0.45728165431985224</v>
+        <v>0.46302368806462979</v>
       </c>
       <c r="AJ24" s="10">
         <f t="shared" si="75"/>
-        <v>0.48766572684663623</v>
+        <v>0.49276802962898991</v>
       </c>
       <c r="AK24" s="10">
         <f t="shared" si="75"/>
-        <v>0.51454068289232369</v>
+        <v>0.51907713850323445</v>
       </c>
       <c r="AL24" s="10">
         <f t="shared" ref="AL24:AM24" si="76">AL18/AL3</f>
-        <v>0.53832575045792463</v>
+        <v>0.54236141592124598</v>
       </c>
       <c r="AM24" s="10">
         <f t="shared" si="76"/>
-        <v>0.55938847209588849</v>
+        <v>0.56298066589579676</v>
       </c>
       <c r="AO24" s="146" t="s">
         <v>7</v>
@@ -8741,7 +8731,7 @@
         <v>2087.13</v>
       </c>
     </row>
-    <row r="25" spans="2:78" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:78" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
         <v>30</v>
       </c>
@@ -8787,7 +8777,7 @@
       </c>
       <c r="M25" s="126">
         <f t="shared" ref="M25" si="79">M17/M16</f>
-        <v>-1.6803874220737073E-3</v>
+        <v>-2.1744084525061108E-3</v>
       </c>
       <c r="N25" s="10">
         <f t="shared" ref="N25" si="80">N17/N16</f>
@@ -8812,77 +8802,77 @@
       </c>
       <c r="X25" s="126">
         <f t="shared" ref="X25:AK25" si="81">X17/X16</f>
-        <v>-1.6020231638742318E-3</v>
+        <v>-1.6939267782585547E-3</v>
       </c>
       <c r="Y25" s="10">
         <f t="shared" si="81"/>
-        <v>-2.1781251856686696E-3</v>
+        <v>-2.3770451712376026E-3</v>
       </c>
       <c r="Z25" s="10">
         <f t="shared" si="81"/>
-        <v>-4.4129315845327392E-3</v>
+        <v>-5.481745352011673E-3</v>
       </c>
       <c r="AA25" s="10">
         <f t="shared" si="81"/>
-        <v>2.2676044829772077E-2</v>
+        <v>1.0536303835544672E-2</v>
       </c>
       <c r="AB25" s="10">
         <f t="shared" si="81"/>
-        <v>2.7857655712716029E-3</v>
+        <v>2.395784146168927E-3</v>
       </c>
       <c r="AC25" s="10">
         <f t="shared" si="81"/>
-        <v>1.3795810145324427E-3</v>
+        <v>1.2625390660653717E-3</v>
       </c>
       <c r="AD25" s="10">
         <f t="shared" si="81"/>
-        <v>8.6981935780793647E-4</v>
+        <v>8.1503546076654306E-4</v>
       </c>
       <c r="AE25" s="10">
         <f t="shared" si="81"/>
-        <v>6.0883838511656429E-4</v>
+        <v>5.7758731715906351E-4</v>
       </c>
       <c r="AF25" s="10">
         <f t="shared" si="81"/>
-        <v>4.5172475147974619E-4</v>
+        <v>4.3179093576665919E-4</v>
       </c>
       <c r="AG25" s="10">
         <f t="shared" si="81"/>
-        <v>3.4776653724919896E-4</v>
+        <v>3.3411067844713683E-4</v>
       </c>
       <c r="AH25" s="10">
         <f t="shared" si="81"/>
-        <v>2.7460594251610426E-4</v>
+        <v>2.6477869969960773E-4</v>
       </c>
       <c r="AI25" s="10">
         <f t="shared" si="81"/>
-        <v>2.2085112551809114E-4</v>
+        <v>2.1352156537811235E-4</v>
       </c>
       <c r="AJ25" s="10">
         <f t="shared" si="81"/>
-        <v>1.8008644617104118E-4</v>
+        <v>1.7447031848691059E-4</v>
       </c>
       <c r="AK25" s="10">
         <f t="shared" si="81"/>
-        <v>1.4842240246224449E-4</v>
+        <v>1.4402820825892962E-4</v>
       </c>
       <c r="AL25" s="10">
         <f t="shared" ref="AL25:AM25" si="82">AL17/AL16</f>
-        <v>1.2336360871640227E-4</v>
+        <v>1.198680189041745E-4</v>
       </c>
       <c r="AM25" s="10">
         <f t="shared" si="82"/>
-        <v>1.0323562933205953E-4</v>
+        <v>1.0041746208594997E-4</v>
       </c>
       <c r="AO25" s="146" t="s">
         <v>116</v>
       </c>
       <c r="AP25" s="141">
         <f>AP23+AP24</f>
-        <v>98456.868915896732</v>
-      </c>
-    </row>
-    <row r="26" spans="2:78" x14ac:dyDescent="0.2">
+        <v>101606.30269599026</v>
+      </c>
+    </row>
+    <row r="26" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="M26" s="125"/>
       <c r="O26" s="7"/>
@@ -8896,11 +8886,11 @@
       </c>
       <c r="AP26" s="142">
         <f>AP25/Main!C7</f>
-        <v>165.77239819624052</v>
+        <v>171.0751180210232</v>
       </c>
       <c r="AQ26" s="68"/>
     </row>
-    <row r="27" spans="2:78" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:78" ht="15" x14ac:dyDescent="0.25">
       <c r="B27" s="16" t="s">
         <v>56</v>
       </c>
@@ -8944,12 +8934,12 @@
         <v>0.10066947912438984</v>
       </c>
       <c r="M27" s="126">
-        <f>M3/R3-1</f>
-        <v>4.868631421394598E-2</v>
+        <f t="shared" ref="M27:N27" si="84">M3/L3-1</f>
+        <v>7.6898615882423638E-2</v>
       </c>
       <c r="N27" s="10">
-        <f t="shared" ref="N27" si="84">N3/M3-1</f>
-        <v>0.11668721629729673</v>
+        <f t="shared" si="84"/>
+        <v>2.7352238993513023E-2</v>
       </c>
       <c r="O27" s="10"/>
       <c r="Q27" s="80">
@@ -8971,7 +8961,7 @@
         <v>37.08</v>
       </c>
     </row>
-    <row r="28" spans="2:78" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:78" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>35</v>
       </c>
@@ -9013,7 +9003,7 @@
       </c>
       <c r="M28" s="128">
         <f>M3/I3-1</f>
-        <v>0.14999999999999991</v>
+        <v>0.25000000000000022</v>
       </c>
       <c r="N28" s="13">
         <f>N3/J3-1</f>
@@ -9035,7 +9025,7 @@
       </c>
       <c r="X28" s="128">
         <f t="shared" ref="X28:AK28" si="86">X3/W3-1</f>
-        <v>0.23394393233363586</v>
+        <v>0.26048316964371776</v>
       </c>
       <c r="Y28" s="13">
         <f t="shared" si="86"/>
@@ -9071,7 +9061,7 @@
       </c>
       <c r="AG28" s="13">
         <f t="shared" si="86"/>
-        <v>0.15000000000000013</v>
+        <v>0.14999999999999991</v>
       </c>
       <c r="AH28" s="13">
         <f t="shared" si="86"/>
@@ -9102,10 +9092,10 @@
       </c>
       <c r="AP28" s="144">
         <f>AP26/AP27-1</f>
-        <v>3.4706687755188925</v>
-      </c>
-    </row>
-    <row r="29" spans="2:78" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+        <v>3.6136763220340669</v>
+      </c>
+    </row>
+    <row r="29" spans="2:78" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -9142,7 +9132,7 @@
       <c r="AO29" s="85"/>
       <c r="AP29" s="86"/>
     </row>
-    <row r="30" spans="2:78" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:78" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
         <v>171</v>
       </c>
@@ -9181,7 +9171,7 @@
       <c r="AM30" s="13"/>
       <c r="AO30" s="86"/>
     </row>
-    <row r="31" spans="2:78" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:78" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>122</v>
       </c>
@@ -9257,7 +9247,7 @@
       <c r="AM31" s="13"/>
       <c r="AO31" s="86"/>
     </row>
-    <row r="32" spans="2:78" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:78" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B32" s="87" t="s">
         <v>128</v>
       </c>
@@ -9338,7 +9328,7 @@
       <c r="AO32" s="85"/>
       <c r="AP32" s="86"/>
     </row>
-    <row r="33" spans="2:42" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:42" ht="15" x14ac:dyDescent="0.25">
       <c r="B33" s="87" t="s">
         <v>129</v>
       </c>
@@ -9396,11 +9386,11 @@
       </c>
       <c r="AP33" s="56"/>
     </row>
-    <row r="34" spans="2:42" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="AP34" s="56"/>
     </row>
-    <row r="35" spans="2:42" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B35" s="12" t="s">
         <v>36</v>
       </c>
@@ -9412,7 +9402,7 @@
       <c r="K35" s="107"/>
       <c r="L35" s="107"/>
     </row>
-    <row r="36" spans="2:42" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:42" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>3</v>
       </c>
@@ -9452,7 +9442,7 @@
       <c r="Q36" s="2"/>
       <c r="R36" s="13"/>
     </row>
-    <row r="37" spans="2:42" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:42" ht="15" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
         <v>37</v>
       </c>
@@ -9487,7 +9477,7 @@
         <v>186.82499999999999</v>
       </c>
     </row>
-    <row r="38" spans="2:42" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:42" ht="15" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
         <v>41</v>
       </c>
@@ -9522,7 +9512,7 @@
         <v>57.594999999999999</v>
       </c>
     </row>
-    <row r="39" spans="2:42" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:42" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
         <v>38</v>
       </c>
@@ -9557,7 +9547,7 @@
         <v>405.89100000000002</v>
       </c>
     </row>
-    <row r="40" spans="2:42" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:42" ht="15" x14ac:dyDescent="0.25">
       <c r="B40" s="11" t="s">
         <v>42</v>
       </c>
@@ -9592,7 +9582,7 @@
         <v>425.95</v>
       </c>
     </row>
-    <row r="41" spans="2:42" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:42" ht="15" x14ac:dyDescent="0.25">
       <c r="B41" s="11" t="s">
         <v>39</v>
       </c>
@@ -9627,7 +9617,7 @@
         <v>424.416</v>
       </c>
     </row>
-    <row r="42" spans="2:42" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:42" ht="15" x14ac:dyDescent="0.25">
       <c r="B42" s="11" t="s">
         <v>40</v>
       </c>
@@ -9662,7 +9652,7 @@
         <v>154.328</v>
       </c>
     </row>
-    <row r="43" spans="2:42" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:42" ht="15" x14ac:dyDescent="0.25">
       <c r="B43" s="11" t="s">
         <v>45</v>
       </c>
@@ -9704,7 +9694,7 @@
         <v>186.77</v>
       </c>
     </row>
-    <row r="44" spans="2:42" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:42" ht="15" x14ac:dyDescent="0.25">
       <c r="B44" s="11" t="s">
         <v>44</v>
       </c>
@@ -9739,7 +9729,7 @@
         <v>2.17</v>
       </c>
     </row>
-    <row r="45" spans="2:42" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:42" ht="15" x14ac:dyDescent="0.25">
       <c r="B45" s="11" t="s">
         <v>43</v>
       </c>
@@ -9781,13 +9771,13 @@
         <v>4919.420000000001</v>
       </c>
     </row>
-    <row r="46" spans="2:42" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:42" x14ac:dyDescent="0.25">
       <c r="C46" s="2"/>
       <c r="F46" s="5"/>
       <c r="K46" s="84"/>
       <c r="L46" s="84"/>
     </row>
-    <row r="47" spans="2:42" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:42" ht="15" x14ac:dyDescent="0.25">
       <c r="B47" s="11" t="s">
         <v>46</v>
       </c>
@@ -9822,7 +9812,7 @@
         <v>77.509</v>
       </c>
     </row>
-    <row r="48" spans="2:42" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:42" ht="15" x14ac:dyDescent="0.25">
       <c r="B48" s="11" t="s">
         <v>47</v>
       </c>
@@ -9857,7 +9847,7 @@
         <v>231.19900000000001</v>
       </c>
     </row>
-    <row r="49" spans="2:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B49" s="11" t="s">
         <v>48</v>
       </c>
@@ -9892,7 +9882,7 @@
         <v>147.19200000000001</v>
       </c>
     </row>
-    <row r="50" spans="2:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B50" s="11" t="s">
         <v>49</v>
       </c>
@@ -9929,7 +9919,7 @@
       <c r="Q50" s="55"/>
       <c r="R50" s="55"/>
     </row>
-    <row r="51" spans="2:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B51" s="11" t="s">
         <v>50</v>
       </c>
@@ -9964,7 +9954,7 @@
         <v>716.154</v>
       </c>
     </row>
-    <row r="52" spans="2:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B52" s="11" t="s">
         <v>51</v>
       </c>
@@ -9999,7 +9989,7 @@
         <v>399.77600000000001</v>
       </c>
     </row>
-    <row r="53" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>4</v>
       </c>
@@ -10038,7 +10028,7 @@
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
     </row>
-    <row r="54" spans="2:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B54" s="11" t="s">
         <v>52</v>
       </c>
@@ -10073,7 +10063,7 @@
         <v>1.2999999999999999E-4</v>
       </c>
     </row>
-    <row r="55" spans="2:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B55" s="11" t="s">
         <v>53</v>
       </c>
@@ -10115,7 +10105,7 @@
         <v>4367.8141299999997</v>
       </c>
     </row>
-    <row r="56" spans="2:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -10127,7 +10117,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="2:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B57" s="11" t="s">
         <v>54</v>
       </c>
@@ -10162,7 +10152,7 @@
         <v>551.59299999999996</v>
       </c>
     </row>
-    <row r="58" spans="2:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B58" s="11" t="s">
         <v>55</v>
       </c>
@@ -10203,10 +10193,10 @@
         <v>4919.4071299999996</v>
       </c>
     </row>
-    <row r="59" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F59" s="5"/>
     </row>
-    <row r="60" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B60" s="200" t="s">
         <v>200</v>
       </c>
@@ -10239,7 +10229,7 @@
         <v>551.60587000000123</v>
       </c>
     </row>
-    <row r="61" spans="2:18" s="213" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:18" s="213" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B61" s="213" t="s">
         <v>201</v>
       </c>
@@ -10285,7 +10275,7 @@
       <c r="Q61" s="214"/>
       <c r="R61" s="214"/>
     </row>
-    <row r="62" spans="2:18" s="213" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:18" s="213" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -10301,7 +10291,7 @@
       <c r="Q62" s="214"/>
       <c r="R62" s="214"/>
     </row>
-    <row r="63" spans="2:18" s="63" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:18" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="63" t="s">
         <v>3</v>
       </c>
@@ -10341,7 +10331,7 @@
       <c r="Q63" s="61"/>
       <c r="R63" s="61"/>
     </row>
-    <row r="64" spans="2:18" s="63" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:18" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="63" t="s">
         <v>4</v>
       </c>
@@ -10381,7 +10371,7 @@
       <c r="Q64" s="61"/>
       <c r="R64" s="61"/>
     </row>
-    <row r="65" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B65" s="215" t="s">
         <v>7</v>
       </c>
@@ -10414,7 +10404,7 @@
         <v>2087.13</v>
       </c>
     </row>
-    <row r="67" spans="2:18" s="63" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:18" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="63" t="s">
         <v>0</v>
       </c>
@@ -10433,7 +10423,7 @@
       <c r="Q67" s="61"/>
       <c r="R67" s="61"/>
     </row>
-    <row r="68" spans="2:18" s="63" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:18" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="63" t="s">
         <v>2</v>
       </c>
@@ -10452,7 +10442,7 @@
       <c r="Q68" s="61"/>
       <c r="R68" s="61"/>
     </row>
-    <row r="69" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B69" s="215" t="s">
         <v>5</v>
       </c>
@@ -10485,17 +10475,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B71" s="215" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="72" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B72" s="215" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B73" s="215" t="s">
         <v>216</v>
       </c>
@@ -10509,7 +10499,7 @@
   <pageSetup paperSize="119" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId2"/>
   <ignoredErrors>
     <ignoredError sqref="V3:V4 V6:V8 V9:V13 W3:W4 V17:V20 W17:W20 W6:W13 V15 W15" formulaRange="1"/>
-    <ignoredError sqref="V5 V16:W16 X5 V14:X14 X16 X21 Y16:AK16 Y18 Z18:AK20 AL13:AM18 X18:X19 M27" formula="1"/>
+    <ignoredError sqref="V5 V16:W16 X5 V14:X14 X16 X21 Y16:AK16 Y18 Z18:AK20 AL13:AM18 X18:X19" formula="1"/>
     <ignoredError sqref="W5" formula="1" formulaRange="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
@@ -10527,9 +10517,9 @@
       <selection pane="bottomRight" activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.875" style="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="17" width="9" style="23"/>
     <col min="18" max="18" width="9" style="153" customWidth="1"/>
@@ -10539,7 +10529,7 @@
     <col min="28" max="16384" width="9" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="30" t="s">
         <v>81</v>
       </c>
@@ -10622,7 +10612,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>87</v>
       </c>
@@ -10703,7 +10693,7 @@
         <v>57.591860754231618</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
         <v>73</v>
       </c>
@@ -10791,7 +10781,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
         <v>74</v>
       </c>
@@ -10879,7 +10869,7 @@
         <v>0.26506009344825054</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B5" s="28"/>
       <c r="C5" s="25"/>
       <c r="D5" s="25"/>
@@ -10901,7 +10891,7 @@
       <c r="Z5" s="37"/>
       <c r="AA5" s="154"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B6" s="28" t="s">
         <v>75</v>
       </c>
@@ -10977,7 +10967,7 @@
         <v>27.493131956981287</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B7" s="28" t="s">
         <v>77</v>
       </c>
@@ -11061,7 +11051,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B8" s="28" t="s">
         <v>78</v>
       </c>
@@ -11145,7 +11135,7 @@
         <v>0.22874332768631445</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B9" s="28"/>
       <c r="C9" s="25"/>
       <c r="P9" s="53"/>
@@ -11155,7 +11145,7 @@
       <c r="Z9" s="37"/>
       <c r="AA9" s="154"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B10" s="28" t="s">
         <v>76</v>
       </c>
@@ -11231,7 +11221,7 @@
         <v>33.805673094984186</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B11" s="28" t="s">
         <v>79</v>
       </c>
@@ -11315,7 +11305,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B12" s="28" t="s">
         <v>80</v>
       </c>
@@ -11399,7 +11389,7 @@
         <v>0.53662150431746292</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B13" s="28"/>
       <c r="P13" s="53"/>
       <c r="Q13" s="53"/>
@@ -11407,7 +11397,7 @@
       <c r="Y13" s="37"/>
       <c r="Z13" s="37"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>86</v>
       </c>
@@ -11487,7 +11477,7 @@
         <v>13334.311356202335</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B15" s="28" t="s">
         <v>84</v>
       </c>
@@ -11572,7 +11562,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B16" s="28" t="s">
         <v>85</v>
       </c>
@@ -11657,11 +11647,11 @@
         <v>0.28790373846547879</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="P17" s="53"/>
       <c r="Q17" s="53"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>173</v>
       </c>
@@ -11727,7 +11717,7 @@
       </c>
       <c r="Z18" s="137"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>175</v>
       </c>
@@ -11808,7 +11798,7 @@
       </c>
       <c r="Z19" s="137"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="31"/>
       <c r="B20" s="200" t="s">
         <v>203</v>
@@ -11877,7 +11867,7 @@
       <c r="T20" s="164"/>
       <c r="Z20" s="137"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="31"/>
       <c r="B21" s="200" t="s">
         <v>202</v>
@@ -11943,11 +11933,11 @@
       <c r="T21" s="164"/>
       <c r="Z21" s="137"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="P22" s="53"/>
       <c r="Q22" s="53"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B24" s="109"/>
       <c r="P24" s="110"/>
       <c r="Q24" s="110"/>

</xml_diff>

<commit_message>
Add Price, MC, EV, P/B history for previous Qs
</commit_message>
<xml_diff>
--- a/$RBLX.xlsx
+++ b/$RBLX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F211DF-8056-4B4C-8606-7FC2820DBD2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA99C3FC-06D7-4507-8382-84F30AF3D44D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18885" activeTab="1" xr2:uid="{DB6ABC51-E0DE-6747-8CA5-53C172A4844D}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="221">
   <si>
     <t>Price</t>
   </si>
@@ -687,6 +687,9 @@
   </si>
   <si>
     <t>R&amp;D Y/Y</t>
+  </si>
+  <si>
+    <t>EV/E</t>
   </si>
 </sst>
 </file>
@@ -705,9 +708,16 @@
     <numFmt numFmtId="171" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="172" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="42" x14ac:knownFonts="1">
+  <fonts count="43" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1218,549 +1228,549 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="252">
+  <cellXfs count="250">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="17" fontId="33" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="33" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="24" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="21" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="21" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="21" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="21" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="33" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="24" fillId="10" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="24" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="24" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="21" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="21" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="21" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="21" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="24" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="13" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="16" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="21" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="21" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="21" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="21" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="21" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="24" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="16" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="33" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="34" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="34" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="34" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="33" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="9" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="34" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="33" fillId="11" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="34" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="24" fillId="11" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="38" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="39" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="23" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="20" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="17" fontId="32" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="32" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="20" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="20" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="20" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="20" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="20" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="20" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="20" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="23" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="17" fontId="32" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="23" fillId="10" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="20" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="20" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="20" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="20" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="20" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="20" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="23" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="12" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="15" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="20" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="20" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="20" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="20" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="20" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="23" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="15" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="33" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="33" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="33" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="33" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="32" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="8" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="33" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="11" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="33" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="23" fillId="11" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="20" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="37" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="38" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="24" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="24" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="23" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="21" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="20" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="21" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="20" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="21" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="20" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="21" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="20" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="21" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="20" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="21" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="20" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="24" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="23" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="24" fillId="12" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="23" fillId="12" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="21" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="20" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="34" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="33" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="24" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="17" fontId="23" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="34" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="33" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="34" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="21" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="21" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="20" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="20" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="15" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="32" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="33" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent3" xfId="5" builtinId="38"/>
@@ -2161,10 +2171,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Metrics!$D$6:$P$6</c:f>
+              <c:f>Metrics!$D$6:$Q$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>9</c:v>
                 </c:pt>
@@ -2203,6 +2213,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2362,10 +2375,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Metrics!$D$10:$P$10</c:f>
+              <c:f>Metrics!$D$10:$Q$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>6.4</c:v>
                 </c:pt>
@@ -2404,6 +2417,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>28.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3250,7 +3266,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>85</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3300,7 +3316,7 @@
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3355,8 +3371,8 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>22225</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3371,8 +3387,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12620625" y="0"/>
-          <a:ext cx="0" cy="8013700"/>
+          <a:off x="12623800" y="0"/>
+          <a:ext cx="0" cy="10029825"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3405,8 +3421,8 @@
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3421,8 +3437,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="18770600" y="0"/>
-          <a:ext cx="0" cy="8013700"/>
+          <a:off x="18773775" y="0"/>
+          <a:ext cx="0" cy="10163175"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3784,7 +3800,7 @@
   <dimension ref="B1:AJ68"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:H8"/>
+      <selection activeCell="G16" sqref="G16:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3802,34 +3818,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="L1" s="230" t="s">
+      <c r="L1" s="245" t="s">
         <v>125</v>
       </c>
-      <c r="M1" s="231"/>
-      <c r="N1" s="231"/>
-      <c r="O1" s="231"/>
-      <c r="P1" s="231"/>
-      <c r="Q1" s="231"/>
-      <c r="R1" s="231"/>
-      <c r="S1" s="231"/>
-      <c r="T1" s="232"/>
-      <c r="V1" s="218" t="s">
+      <c r="M1" s="246"/>
+      <c r="N1" s="246"/>
+      <c r="O1" s="246"/>
+      <c r="P1" s="246"/>
+      <c r="Q1" s="246"/>
+      <c r="R1" s="246"/>
+      <c r="S1" s="246"/>
+      <c r="T1" s="247"/>
+      <c r="V1" s="241" t="s">
         <v>127</v>
       </c>
-      <c r="W1" s="219"/>
-      <c r="X1" s="219"/>
-      <c r="Y1" s="219"/>
-      <c r="Z1" s="219"/>
-      <c r="AA1" s="219"/>
-      <c r="AB1" s="219"/>
-      <c r="AC1" s="219"/>
-      <c r="AD1" s="219"/>
-      <c r="AE1" s="219"/>
-      <c r="AF1" s="219"/>
-      <c r="AG1" s="219"/>
-      <c r="AH1" s="219"/>
-      <c r="AI1" s="219"/>
-      <c r="AJ1" s="220"/>
+      <c r="W1" s="242"/>
+      <c r="X1" s="242"/>
+      <c r="Y1" s="242"/>
+      <c r="Z1" s="242"/>
+      <c r="AA1" s="242"/>
+      <c r="AB1" s="242"/>
+      <c r="AC1" s="242"/>
+      <c r="AD1" s="242"/>
+      <c r="AE1" s="242"/>
+      <c r="AF1" s="242"/>
+      <c r="AG1" s="242"/>
+      <c r="AH1" s="242"/>
+      <c r="AI1" s="242"/>
+      <c r="AJ1" s="243"/>
     </row>
     <row r="2" spans="2:36" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
@@ -4017,16 +4033,16 @@
       </c>
     </row>
     <row r="5" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B5" s="223" t="s">
+      <c r="B5" s="227" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="224"/>
-      <c r="D5" s="225"/>
-      <c r="F5" s="223" t="s">
+      <c r="C5" s="228"/>
+      <c r="D5" s="229"/>
+      <c r="F5" s="227" t="s">
         <v>193</v>
       </c>
-      <c r="G5" s="224"/>
-      <c r="H5" s="225"/>
+      <c r="G5" s="228"/>
+      <c r="H5" s="229"/>
       <c r="K5" s="28" t="s">
         <v>73</v>
       </c>
@@ -4121,16 +4137,16 @@
         <v>0</v>
       </c>
       <c r="C6" s="9">
-        <v>40.75</v>
+        <v>46.5</v>
       </c>
       <c r="D6" s="44"/>
       <c r="F6" s="181" t="s">
         <v>194</v>
       </c>
-      <c r="G6" s="226" t="s">
+      <c r="G6" s="244" t="s">
         <v>198</v>
       </c>
-      <c r="H6" s="222"/>
+      <c r="H6" s="233"/>
       <c r="K6" s="28" t="s">
         <v>74</v>
       </c>
@@ -4228,10 +4244,10 @@
       <c r="F7" s="181" t="s">
         <v>195</v>
       </c>
-      <c r="G7" s="227">
+      <c r="G7" s="232">
         <v>2004</v>
       </c>
-      <c r="H7" s="222"/>
+      <c r="H7" s="233"/>
       <c r="K7" s="28"/>
       <c r="L7" s="61"/>
       <c r="M7" s="61"/>
@@ -4265,17 +4281,17 @@
       </c>
       <c r="C8" s="9">
         <f>C6*C7</f>
-        <v>24202.565999999999</v>
+        <v>27617.651999999998</v>
       </c>
       <c r="D8" s="41"/>
       <c r="F8" s="181" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="227">
+      <c r="G8" s="232">
         <f>AJ4</f>
         <v>52.2</v>
       </c>
-      <c r="H8" s="222"/>
+      <c r="H8" s="233"/>
       <c r="K8" s="28" t="s">
         <v>75</v>
       </c>
@@ -4362,8 +4378,8 @@
         <v>13</v>
       </c>
       <c r="F9" s="167"/>
-      <c r="G9" s="227"/>
-      <c r="H9" s="222"/>
+      <c r="G9" s="232"/>
+      <c r="H9" s="233"/>
       <c r="K9" s="28" t="s">
         <v>77</v>
       </c>
@@ -4463,8 +4479,8 @@
         <v>13</v>
       </c>
       <c r="F10" s="167"/>
-      <c r="G10" s="227"/>
-      <c r="H10" s="222"/>
+      <c r="G10" s="232"/>
+      <c r="H10" s="233"/>
       <c r="K10" s="28" t="s">
         <v>78</v>
       </c>
@@ -4564,10 +4580,10 @@
       <c r="F11" s="181" t="s">
         <v>199</v>
       </c>
-      <c r="G11" s="226" t="s">
+      <c r="G11" s="244" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="222"/>
+      <c r="H11" s="233"/>
       <c r="K11" s="28"/>
       <c r="L11" s="61"/>
       <c r="M11" s="61"/>
@@ -4590,16 +4606,16 @@
       </c>
       <c r="C12" s="45">
         <f>C8-C9+C10</f>
-        <v>22115.436000000002</v>
+        <v>25530.522000000001</v>
       </c>
       <c r="D12" s="43"/>
       <c r="F12" s="182" t="s">
         <v>196</v>
       </c>
-      <c r="G12" s="228" t="s">
+      <c r="G12" s="236" t="s">
         <v>197</v>
       </c>
-      <c r="H12" s="229"/>
+      <c r="H12" s="237"/>
       <c r="K12" s="28" t="s">
         <v>76</v>
       </c>
@@ -4851,16 +4867,16 @@
       </c>
     </row>
     <row r="15" spans="2:36" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="223" t="s">
+      <c r="B15" s="227" t="s">
         <v>130</v>
       </c>
-      <c r="C15" s="224"/>
-      <c r="D15" s="225"/>
-      <c r="F15" s="223" t="s">
+      <c r="C15" s="228"/>
+      <c r="D15" s="229"/>
+      <c r="F15" s="227" t="s">
         <v>204</v>
       </c>
-      <c r="G15" s="224"/>
-      <c r="H15" s="225"/>
+      <c r="G15" s="228"/>
+      <c r="H15" s="229"/>
       <c r="K15" s="28"/>
       <c r="L15" s="63"/>
       <c r="M15" s="63"/>
@@ -4876,18 +4892,18 @@
       <c r="B16" s="93" t="s">
         <v>132</v>
       </c>
-      <c r="C16" s="221" t="s">
+      <c r="C16" s="240" t="s">
         <v>131</v>
       </c>
-      <c r="D16" s="222"/>
+      <c r="D16" s="233"/>
       <c r="F16" s="181" t="s">
         <v>205</v>
       </c>
-      <c r="G16" s="235">
+      <c r="G16" s="234">
         <f>C6/'Financial Model'!L64</f>
-        <v>43.876556281027149</v>
-      </c>
-      <c r="H16" s="236"/>
+        <v>50.067726799208891</v>
+      </c>
+      <c r="H16" s="235"/>
       <c r="J16" s="31" t="s">
         <v>86</v>
       </c>
@@ -4969,18 +4985,18 @@
       <c r="B17" s="105" t="s">
         <v>164</v>
       </c>
-      <c r="C17" s="233" t="s">
+      <c r="C17" s="230" t="s">
         <v>165</v>
       </c>
-      <c r="D17" s="234"/>
+      <c r="D17" s="231"/>
       <c r="F17" s="181" t="s">
         <v>215</v>
       </c>
-      <c r="G17" s="235">
+      <c r="G17" s="234">
         <f>C8/'Financial Model'!W3</f>
-        <v>12.610882454547017</v>
-      </c>
-      <c r="H17" s="236"/>
+        <v>14.390332126047516</v>
+      </c>
+      <c r="H17" s="235"/>
       <c r="K17" s="28" t="s">
         <v>84</v>
       </c>
@@ -5072,15 +5088,15 @@
       <c r="B18" s="93" t="s">
         <v>133</v>
       </c>
-      <c r="C18" s="221" t="s">
+      <c r="C18" s="240" t="s">
         <v>134</v>
       </c>
-      <c r="D18" s="222"/>
+      <c r="D18" s="233"/>
       <c r="F18" s="181" t="s">
         <v>216</v>
       </c>
-      <c r="G18" s="227"/>
-      <c r="H18" s="222"/>
+      <c r="G18" s="232"/>
+      <c r="H18" s="233"/>
       <c r="K18" s="28" t="s">
         <v>85</v>
       </c>
@@ -5167,22 +5183,22 @@
     </row>
     <row r="19" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B19" s="91"/>
-      <c r="C19" s="227"/>
-      <c r="D19" s="222"/>
+      <c r="C19" s="232"/>
+      <c r="D19" s="233"/>
       <c r="F19" s="181"/>
-      <c r="G19" s="227"/>
-      <c r="H19" s="222"/>
+      <c r="G19" s="232"/>
+      <c r="H19" s="233"/>
       <c r="K19" s="28"/>
       <c r="L19" s="63"/>
       <c r="M19" s="63"/>
     </row>
     <row r="20" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="92"/>
-      <c r="C20" s="237"/>
-      <c r="D20" s="238"/>
+      <c r="C20" s="238"/>
+      <c r="D20" s="239"/>
       <c r="F20" s="182"/>
-      <c r="G20" s="228"/>
-      <c r="H20" s="229"/>
+      <c r="G20" s="236"/>
+      <c r="H20" s="237"/>
       <c r="J20" s="31"/>
       <c r="K20" s="200" t="s">
         <v>214</v>
@@ -5213,14 +5229,14 @@
       </c>
     </row>
     <row r="23" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B23" s="223" t="s">
+      <c r="B23" s="227" t="s">
         <v>159</v>
       </c>
-      <c r="C23" s="224"/>
-      <c r="D23" s="224"/>
-      <c r="E23" s="224"/>
-      <c r="F23" s="224"/>
-      <c r="G23" s="225"/>
+      <c r="C23" s="228"/>
+      <c r="D23" s="228"/>
+      <c r="E23" s="228"/>
+      <c r="F23" s="228"/>
+      <c r="G23" s="229"/>
       <c r="K23" s="200" t="s">
         <v>211</v>
       </c>
@@ -5332,12 +5348,12 @@
       <c r="F31" s="102"/>
       <c r="G31" s="103"/>
       <c r="J31" s="7"/>
-      <c r="K31" s="223" t="s">
+      <c r="K31" s="227" t="s">
         <v>181</v>
       </c>
-      <c r="L31" s="224"/>
-      <c r="M31" s="224"/>
-      <c r="N31" s="225"/>
+      <c r="L31" s="228"/>
+      <c r="M31" s="228"/>
+      <c r="N31" s="229"/>
     </row>
     <row r="32" spans="2:36" x14ac:dyDescent="0.25">
       <c r="J32" s="7"/>
@@ -5349,14 +5365,14 @@
       <c r="N32" s="97"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="223" t="s">
+      <c r="B33" s="227" t="s">
         <v>187</v>
       </c>
-      <c r="C33" s="224"/>
-      <c r="D33" s="224"/>
-      <c r="E33" s="224"/>
-      <c r="F33" s="224"/>
-      <c r="G33" s="225"/>
+      <c r="C33" s="228"/>
+      <c r="D33" s="228"/>
+      <c r="E33" s="228"/>
+      <c r="F33" s="228"/>
+      <c r="G33" s="229"/>
       <c r="J33" s="7"/>
       <c r="K33" s="173" t="s">
         <v>177</v>
@@ -5661,6 +5677,17 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="V1:AJ1"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="L1:T1"/>
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="K31:N31"/>
     <mergeCell ref="B5:D5"/>
@@ -5676,19 +5703,8 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C16:D16"/>
-    <mergeCell ref="V1:AJ1"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="L1:T1"/>
   </mergeCells>
-  <phoneticPr fontId="22" type="noConversion"/>
+  <phoneticPr fontId="23" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K55" r:id="rId1" xr:uid="{F79BC045-05D5-43FB-A051-BA2031CC85A7}"/>
     <hyperlink ref="K57" r:id="rId2" xr:uid="{58004FA9-9F7A-4B71-811E-FF4EE09F281F}"/>
@@ -5702,13 +5718,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0FDCAC-3416-844A-BCBB-390EC350CF59}">
-  <dimension ref="B1:BZ76"/>
+  <dimension ref="B1:BZ77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="L15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AA3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W31" sqref="W31"/>
+      <selection pane="bottomRight" activeCell="AR26" sqref="AR26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7984,159 +8000,159 @@
       </c>
       <c r="AN18" s="3">
         <f>AM18*(1+$AP$21)</f>
-        <v>11192.71501744148</v>
+        <v>10971.077096304025</v>
       </c>
       <c r="AO18" s="3">
         <f t="shared" ref="AO18:BZ18" si="52">AN18*(1+$AP$21)</f>
-        <v>11304.642167615895</v>
+        <v>10861.366325340985</v>
       </c>
       <c r="AP18" s="3">
         <f t="shared" si="52"/>
-        <v>11417.688589292055</v>
+        <v>10752.752662087574</v>
       </c>
       <c r="AQ18" s="3">
         <f t="shared" si="52"/>
-        <v>11531.865475184975</v>
+        <v>10645.225135466699</v>
       </c>
       <c r="AR18" s="3">
         <f t="shared" si="52"/>
-        <v>11647.184129936824</v>
+        <v>10538.772884112032</v>
       </c>
       <c r="AS18" s="3">
         <f t="shared" si="52"/>
-        <v>11763.655971236192</v>
+        <v>10433.385155270911</v>
       </c>
       <c r="AT18" s="3">
         <f t="shared" si="52"/>
-        <v>11881.292530948554</v>
+        <v>10329.051303718203</v>
       </c>
       <c r="AU18" s="3">
         <f t="shared" si="52"/>
-        <v>12000.105456258039</v>
+        <v>10225.760790681021</v>
       </c>
       <c r="AV18" s="3">
         <f t="shared" si="52"/>
-        <v>12120.10651082062</v>
+        <v>10123.503182774211</v>
       </c>
       <c r="AW18" s="3">
         <f t="shared" si="52"/>
-        <v>12241.307575928826</v>
+        <v>10022.268150946469</v>
       </c>
       <c r="AX18" s="3">
         <f t="shared" si="52"/>
-        <v>12363.720651688114</v>
+        <v>9922.0454694370037</v>
       </c>
       <c r="AY18" s="3">
         <f t="shared" si="52"/>
-        <v>12487.357858204996</v>
+        <v>9822.8250147426334</v>
       </c>
       <c r="AZ18" s="3">
         <f t="shared" si="52"/>
-        <v>12612.231436787046</v>
+        <v>9724.5967645952078</v>
       </c>
       <c r="BA18" s="3">
         <f t="shared" si="52"/>
-        <v>12738.353751154917</v>
+        <v>9627.3507969492548</v>
       </c>
       <c r="BB18" s="3">
         <f t="shared" si="52"/>
-        <v>12865.737288666465</v>
+        <v>9531.0772889797627</v>
       </c>
       <c r="BC18" s="3">
         <f t="shared" si="52"/>
-        <v>12994.394661553129</v>
+        <v>9435.7665160899651</v>
       </c>
       <c r="BD18" s="3">
         <f t="shared" si="52"/>
-        <v>13124.33860816866</v>
+        <v>9341.408850929065</v>
       </c>
       <c r="BE18" s="3">
         <f t="shared" si="52"/>
-        <v>13255.581994250348</v>
+        <v>9247.9947624197739</v>
       </c>
       <c r="BF18" s="3">
         <f t="shared" si="52"/>
-        <v>13388.137814192851</v>
+        <v>9155.514814795577</v>
       </c>
       <c r="BG18" s="3">
         <f t="shared" si="52"/>
-        <v>13522.019192334779</v>
+        <v>9063.9596666476209</v>
       </c>
       <c r="BH18" s="3">
         <f t="shared" si="52"/>
-        <v>13657.239384258128</v>
+        <v>8973.3200699811441</v>
       </c>
       <c r="BI18" s="3">
         <f t="shared" si="52"/>
-        <v>13793.811778100709</v>
+        <v>8883.5868692813328</v>
       </c>
       <c r="BJ18" s="3">
         <f t="shared" si="52"/>
-        <v>13931.749895881716</v>
+        <v>8794.7510005885197</v>
       </c>
       <c r="BK18" s="3">
         <f t="shared" si="52"/>
-        <v>14071.067394840533</v>
+        <v>8706.8034905826353</v>
       </c>
       <c r="BL18" s="3">
         <f t="shared" si="52"/>
-        <v>14211.778068788939</v>
+        <v>8619.7354556768096</v>
       </c>
       <c r="BM18" s="3">
         <f t="shared" si="52"/>
-        <v>14353.895849476829</v>
+        <v>8533.5381011200407</v>
       </c>
       <c r="BN18" s="3">
         <f t="shared" si="52"/>
-        <v>14497.434807971596</v>
+        <v>8448.2027201088404</v>
       </c>
       <c r="BO18" s="3">
         <f t="shared" si="52"/>
-        <v>14642.409156051313</v>
+        <v>8363.7206929077511</v>
       </c>
       <c r="BP18" s="3">
         <f t="shared" si="52"/>
-        <v>14788.833247611827</v>
+        <v>8280.0834859786737</v>
       </c>
       <c r="BQ18" s="3">
         <f t="shared" si="52"/>
-        <v>14936.721580087946</v>
+        <v>8197.2826511188869</v>
       </c>
       <c r="BR18" s="3">
         <f t="shared" si="52"/>
-        <v>15086.088795888825</v>
+        <v>8115.3098246076979</v>
       </c>
       <c r="BS18" s="3">
         <f t="shared" si="52"/>
-        <v>15236.949683847713</v>
+        <v>8034.1567263616207</v>
       </c>
       <c r="BT18" s="3">
         <f t="shared" si="52"/>
-        <v>15389.319180686191</v>
+        <v>7953.8151590980042</v>
       </c>
       <c r="BU18" s="3">
         <f t="shared" si="52"/>
-        <v>15543.212372493053</v>
+        <v>7874.2770075070239</v>
       </c>
       <c r="BV18" s="3">
         <f t="shared" si="52"/>
-        <v>15698.644496217985</v>
+        <v>7795.5342374319534</v>
       </c>
       <c r="BW18" s="3">
         <f t="shared" si="52"/>
-        <v>15855.630941180165</v>
+        <v>7717.5788950576334</v>
       </c>
       <c r="BX18" s="3">
         <f t="shared" si="52"/>
-        <v>16014.187250591967</v>
+        <v>7640.4031061070573</v>
       </c>
       <c r="BY18" s="3">
         <f t="shared" si="52"/>
-        <v>16174.329123097887</v>
+        <v>7563.9990750459865</v>
       </c>
       <c r="BZ18" s="3">
         <f t="shared" si="52"/>
-        <v>16336.072414328866</v>
+        <v>7488.3590842955264</v>
       </c>
     </row>
     <row r="19" spans="2:78" ht="15" x14ac:dyDescent="0.25">
@@ -8408,7 +8424,7 @@
         <v>118</v>
       </c>
       <c r="AP21" s="139">
-        <v>0.01</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="22" spans="2:78" ht="15" x14ac:dyDescent="0.25">
@@ -8690,7 +8706,7 @@
       </c>
       <c r="AP23" s="141">
         <f>NPV(AP22,X18:BZ18)</f>
-        <v>99519.172695990259</v>
+        <v>82186.236313802889</v>
       </c>
       <c r="AR23" s="69"/>
     </row>
@@ -8973,7 +8989,7 @@
       </c>
       <c r="AP25" s="141">
         <f>AP23+AP24</f>
-        <v>101606.30269599026</v>
+        <v>84273.366313802893</v>
       </c>
     </row>
     <row r="26" spans="2:78" x14ac:dyDescent="0.25">
@@ -8990,9 +9006,10 @@
       </c>
       <c r="AP26" s="142">
         <f>AP25/Main!C7</f>
-        <v>171.0751180210232</v>
+        <v>141.89155303976727</v>
       </c>
       <c r="AQ26" s="68"/>
+      <c r="AS26" s="9"/>
     </row>
     <row r="27" spans="2:78" ht="15" x14ac:dyDescent="0.25">
       <c r="B27" s="16" t="s">
@@ -9062,7 +9079,7 @@
       </c>
       <c r="AP27" s="143">
         <f>Main!C6</f>
-        <v>40.75</v>
+        <v>46.5</v>
       </c>
     </row>
     <row r="28" spans="2:78" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -9196,7 +9213,7 @@
       </c>
       <c r="AP28" s="144">
         <f>AP26/AP27-1</f>
-        <v>3.198162405423882</v>
+        <v>2.051431248167038</v>
       </c>
     </row>
     <row r="29" spans="2:78" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -9210,7 +9227,7 @@
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
-      <c r="M29" s="250"/>
+      <c r="M29" s="225"/>
       <c r="N29" s="13"/>
       <c r="O29" s="13"/>
       <c r="Q29" s="82"/>
@@ -9233,83 +9250,79 @@
       <c r="AK29" s="13"/>
       <c r="AL29" s="13"/>
       <c r="AM29" s="13"/>
-      <c r="AO29" s="239"/>
-      <c r="AP29" s="240"/>
-    </row>
-    <row r="30" spans="2:78" s="241" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B30" s="241" t="s">
+    </row>
+    <row r="30" spans="2:78" s="218" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B30" s="218" t="s">
         <v>218</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="242">
-        <f t="shared" ref="D30:L30" si="88">D8/C8-1</f>
+      <c r="D30" s="219">
+        <f t="shared" ref="D30:K30" si="88">D8/C8-1</f>
         <v>-0.18539132546702008</v>
       </c>
-      <c r="E30" s="242">
+      <c r="E30" s="219">
         <f t="shared" si="88"/>
         <v>0.28470272553355347</v>
       </c>
-      <c r="F30" s="242">
+      <c r="F30" s="219">
         <f t="shared" si="88"/>
         <v>0.16165777055774733</v>
       </c>
-      <c r="G30" s="242">
+      <c r="G30" s="219">
         <f t="shared" si="88"/>
         <v>0.60893668736577489</v>
       </c>
-      <c r="H30" s="242">
+      <c r="H30" s="219">
         <f t="shared" si="88"/>
         <v>0.29079922188651119</v>
       </c>
-      <c r="I30" s="242">
+      <c r="I30" s="219">
         <f t="shared" si="88"/>
         <v>0.10819411934459877</v>
       </c>
-      <c r="J30" s="242">
+      <c r="J30" s="219">
         <f t="shared" si="88"/>
         <v>0.25552461210170341</v>
       </c>
-      <c r="K30" s="242">
+      <c r="K30" s="219">
         <f t="shared" si="88"/>
         <v>2.4151639108140888E-2</v>
       </c>
-      <c r="L30" s="242">
+      <c r="L30" s="219">
         <f>L8/K8-1</f>
         <v>0.19123884744771091</v>
       </c>
-      <c r="M30" s="251">
+      <c r="M30" s="226">
         <f t="shared" ref="M30:N30" si="89">M8/L8-1</f>
         <v>-0.14026981054699483</v>
       </c>
-      <c r="N30" s="248">
+      <c r="N30" s="223">
         <f t="shared" si="89"/>
         <v>1.2000000000000011E-2</v>
       </c>
-      <c r="O30" s="242"/>
-      <c r="Q30" s="244"/>
-      <c r="R30" s="245"/>
-      <c r="V30" s="242"/>
-      <c r="W30" s="242"/>
-      <c r="X30" s="243"/>
-      <c r="Y30" s="242"/>
-      <c r="Z30" s="242"/>
-      <c r="AA30" s="242"/>
-      <c r="AB30" s="242"/>
-      <c r="AC30" s="242"/>
-      <c r="AD30" s="242"/>
-      <c r="AE30" s="242"/>
-      <c r="AF30" s="242"/>
-      <c r="AG30" s="242"/>
-      <c r="AH30" s="242"/>
-      <c r="AI30" s="242"/>
-      <c r="AJ30" s="242"/>
-      <c r="AK30" s="242"/>
-      <c r="AL30" s="242"/>
-      <c r="AM30" s="242"/>
-      <c r="AO30" s="246"/>
-      <c r="AP30" s="247"/>
+      <c r="O30" s="219"/>
+      <c r="Q30" s="221"/>
+      <c r="R30" s="222"/>
+      <c r="V30" s="219"/>
+      <c r="W30" s="219"/>
+      <c r="X30" s="220"/>
+      <c r="Y30" s="219"/>
+      <c r="Z30" s="219"/>
+      <c r="AA30" s="219"/>
+      <c r="AB30" s="219"/>
+      <c r="AC30" s="219"/>
+      <c r="AD30" s="219"/>
+      <c r="AE30" s="219"/>
+      <c r="AF30" s="219"/>
+      <c r="AG30" s="219"/>
+      <c r="AH30" s="219"/>
+      <c r="AI30" s="219"/>
+      <c r="AJ30" s="219"/>
+      <c r="AK30" s="219"/>
+      <c r="AL30" s="219"/>
+      <c r="AM30" s="219"/>
     </row>
     <row r="31" spans="2:78" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
@@ -9351,11 +9364,11 @@
         <f>L8/H8-1</f>
         <v>0.69747811588161723</v>
       </c>
-      <c r="M31" s="250">
+      <c r="M31" s="225">
         <f t="shared" ref="M31:N31" si="91">M8/I8-1</f>
         <v>0.31689309362363915</v>
       </c>
-      <c r="N31" s="249">
+      <c r="N31" s="224">
         <f t="shared" si="91"/>
         <v>6.1465301358161195E-2</v>
       </c>
@@ -9383,8 +9396,6 @@
       <c r="AK31" s="13"/>
       <c r="AL31" s="13"/>
       <c r="AM31" s="13"/>
-      <c r="AO31" s="239"/>
-      <c r="AP31" s="240"/>
     </row>
     <row r="32" spans="2:78" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C32" s="2"/>
@@ -10702,13 +10713,24 @@
       <c r="C70" s="216"/>
       <c r="D70" s="216"/>
       <c r="E70" s="216"/>
-      <c r="F70" s="61"/>
-      <c r="G70" s="61"/>
-      <c r="H70" s="61"/>
-      <c r="I70" s="61"/>
-      <c r="J70" s="61"/>
-      <c r="K70" s="61"/>
-      <c r="L70" s="61"/>
+      <c r="G70" s="61">
+        <v>64.83</v>
+      </c>
+      <c r="H70" s="61">
+        <v>89.98</v>
+      </c>
+      <c r="I70" s="61">
+        <v>75.55</v>
+      </c>
+      <c r="J70" s="61">
+        <v>103.16</v>
+      </c>
+      <c r="K70" s="61">
+        <v>46.24</v>
+      </c>
+      <c r="L70" s="61">
+        <v>32.86</v>
+      </c>
       <c r="M70" s="61"/>
       <c r="N70" s="61"/>
       <c r="Q70" s="61"/>
@@ -10722,12 +10744,30 @@
       <c r="D71" s="216"/>
       <c r="E71" s="216"/>
       <c r="F71" s="61"/>
-      <c r="G71" s="61"/>
-      <c r="H71" s="61"/>
-      <c r="I71" s="61"/>
-      <c r="J71" s="61"/>
-      <c r="K71" s="61"/>
-      <c r="L71" s="61"/>
+      <c r="G71" s="217">
+        <f t="shared" ref="G71:I71" si="102">G70*G20</f>
+        <v>18870.327420000001</v>
+      </c>
+      <c r="H71" s="217">
+        <f t="shared" si="102"/>
+        <v>51405.574000000001</v>
+      </c>
+      <c r="I71" s="217">
+        <f t="shared" si="102"/>
+        <v>43511.662599999996</v>
+      </c>
+      <c r="J71" s="217">
+        <f>J70*J20</f>
+        <v>59991.150599999994</v>
+      </c>
+      <c r="K71" s="217">
+        <f t="shared" ref="K71:L71" si="103">K70*K20</f>
+        <v>27213.211039999998</v>
+      </c>
+      <c r="L71" s="217">
+        <f t="shared" si="103"/>
+        <v>19516.47408</v>
+      </c>
       <c r="M71" s="61"/>
       <c r="N71" s="61"/>
       <c r="Q71" s="61"/>
@@ -10737,59 +10777,136 @@
       <c r="B72" s="215" t="s">
         <v>5</v>
       </c>
-      <c r="F72" s="7">
-        <f>F71-F69</f>
-        <v>0</v>
-      </c>
-      <c r="G72" s="7">
-        <f t="shared" ref="G72:L72" si="102">G71-G69</f>
-        <v>0</v>
-      </c>
-      <c r="H72" s="7">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="I72" s="7">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="J72" s="7">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="K72" s="7">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="L72" s="7">
-        <f t="shared" si="102"/>
-        <v>0</v>
+      <c r="F72" s="5">
+        <f t="shared" ref="F72:K72" si="104">F71-F68</f>
+        <v>-893.94299999999998</v>
+      </c>
+      <c r="G72" s="5">
+        <f t="shared" si="104"/>
+        <v>17269.797420000003</v>
+      </c>
+      <c r="H72" s="5">
+        <f t="shared" si="104"/>
+        <v>49625.311999999998</v>
+      </c>
+      <c r="I72" s="5">
+        <f t="shared" si="104"/>
+        <v>41586.103599999995</v>
+      </c>
+      <c r="J72" s="5">
+        <f t="shared" si="104"/>
+        <v>57974.573599999996</v>
+      </c>
+      <c r="K72" s="5">
+        <f t="shared" si="104"/>
+        <v>25068.281039999998</v>
+      </c>
+      <c r="L72" s="5">
+        <f>L71-L68</f>
+        <v>17429.344079999999</v>
       </c>
     </row>
     <row r="74" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B74" s="215" t="s">
         <v>205</v>
       </c>
+      <c r="G74" s="248">
+        <f t="shared" ref="G74:J74" si="105">G70/G64</f>
+        <v>31.897428675747243</v>
+      </c>
+      <c r="H74" s="248">
+        <f t="shared" si="105"/>
+        <v>94.837408378363875</v>
+      </c>
+      <c r="I74" s="248">
+        <f t="shared" si="105"/>
+        <v>71.82145284741128</v>
+      </c>
+      <c r="J74" s="248">
+        <f>J70/J64</f>
+        <v>101.1783119281527</v>
+      </c>
+      <c r="K74" s="248">
+        <f t="shared" ref="K74:L74" si="106">K70/K64</f>
+        <v>47.956090444982024</v>
+      </c>
+      <c r="L74" s="248">
+        <f t="shared" si="106"/>
+        <v>35.381193604774282</v>
+      </c>
     </row>
     <row r="75" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B75" s="215" t="s">
         <v>215</v>
       </c>
+      <c r="G75" s="248">
+        <f t="shared" ref="G75" si="107">G71/SUM(D3:G3)</f>
+        <v>16.419103099215079</v>
+      </c>
+      <c r="H75" s="248">
+        <f t="shared" ref="H75" si="108">H71/SUM(E3:H3)</f>
+        <v>36.639779500911978</v>
+      </c>
+      <c r="I75" s="248">
+        <f t="shared" ref="I75" si="109">I71/SUM(F3:I3)</f>
+        <v>26.205198922441955</v>
+      </c>
+      <c r="J75" s="248">
+        <f t="shared" ref="J75:K75" si="110">J71/SUM(G3:J3)</f>
+        <v>31.25872473727074</v>
+      </c>
+      <c r="K75" s="248">
+        <f t="shared" si="110"/>
+        <v>13.150678086094159</v>
+      </c>
+      <c r="L75" s="248">
+        <f>L71/SUM(I3:L3)</f>
+        <v>8.8452081220206615</v>
+      </c>
     </row>
     <row r="76" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B76" s="215" t="s">
+      <c r="B76" s="249" t="s">
+        <v>220</v>
+      </c>
+      <c r="G76" s="248">
+        <f t="shared" ref="G76" si="111">G72/SUM(D3:G3)</f>
+        <v>15.026479298976499</v>
+      </c>
+      <c r="H76" s="248">
+        <f t="shared" ref="H76" si="112">H72/SUM(E3:H3)</f>
+        <v>35.370881946458979</v>
+      </c>
+      <c r="I76" s="248">
+        <f t="shared" ref="I76" si="113">I72/SUM(F3:I3)</f>
+        <v>25.045517733153215</v>
+      </c>
+      <c r="J76" s="248">
+        <f t="shared" ref="J76:K76" si="114">J72/SUM(G3:J3)</f>
+        <v>30.207976006431906</v>
+      </c>
+      <c r="K76" s="248">
+        <f t="shared" si="114"/>
+        <v>12.114149030197565</v>
+      </c>
+      <c r="L76" s="248">
+        <f>L72/SUM(I3:L3)</f>
+        <v>7.8992842244949566</v>
+      </c>
+    </row>
+    <row r="77" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B77" s="215" t="s">
         <v>216</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="22" type="noConversion"/>
+  <phoneticPr fontId="23" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="L1" r:id="rId1" xr:uid="{F0F1B078-C7E3-AA47-9924-08C1D4511F24}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="119" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId2"/>
   <ignoredErrors>
-    <ignoredError sqref="V3:V4 V6:V8 V9:V13 W3:W4 V17:V20 W17:W20 W6:W13 V15 W15" formulaRange="1"/>
+    <ignoredError sqref="V3:V4 V6:V8 V9:V13 W3:W4 V17:V20 W17:W20 W6:W13 V15 W15 K75:L75 K76:L76 G75:J76" formulaRange="1"/>
     <ignoredError sqref="V5 V16:W16 X5 V14:X14 X16 X21 Y16:AK16 Y18 Z18:AK20 AL13:AM18 X18:X19" formula="1"/>
     <ignoredError sqref="W5" formula="1" formulaRange="1"/>
   </ignoredErrors>
@@ -10805,7 +10922,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N17" sqref="N17"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12258,7 +12375,7 @@
       <c r="Q24" s="110"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="22" type="noConversion"/>
+  <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Add Q3, Q2 cashflow data
</commit_message>
<xml_diff>
--- a/$RBLX.xlsx
+++ b/$RBLX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F615CB2-6500-43F7-A913-B86459033241}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547339AC-A919-43D6-9452-130501473D87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18885" xr2:uid="{DB6ABC51-E0DE-6747-8CA5-53C172A4844D}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="18390" windowHeight="2400" activeTab="1" xr2:uid="{DB6ABC51-E0DE-6747-8CA5-53C172A4844D}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="282">
   <si>
     <t>Price</t>
   </si>
@@ -786,13 +786,100 @@
   </si>
   <si>
     <t>experience, then buying from the brand in the real world</t>
+  </si>
+  <si>
+    <t>Cashflow Statement</t>
+  </si>
+  <si>
+    <t>ROCE</t>
+  </si>
+  <si>
+    <t>D&amp;A</t>
+  </si>
+  <si>
+    <t>Stock Based Comp</t>
+  </si>
+  <si>
+    <t>Other Non Cash Charges (Credit)</t>
+  </si>
+  <si>
+    <t>Operating Lease Non-Cash</t>
+  </si>
+  <si>
+    <t>Amortisation of Debt Issuance</t>
+  </si>
+  <si>
+    <t>Changes in Operating Assets/Liabilities</t>
+  </si>
+  <si>
+    <t>CFOO</t>
+  </si>
+  <si>
+    <t>Acquisition of PP&amp;E</t>
+  </si>
+  <si>
+    <t>Net Payments re. business combination</t>
+  </si>
+  <si>
+    <t>Purchases of Intangibles</t>
+  </si>
+  <si>
+    <t>CFFI</t>
+  </si>
+  <si>
+    <t>Proceeds from Common Stock Issuance</t>
+  </si>
+  <si>
+    <t>Payment of Term License Related</t>
+  </si>
+  <si>
+    <t>Payment of Withholding Taxes</t>
+  </si>
+  <si>
+    <t>Net Proceeds from Preferred Stock Issuance</t>
+  </si>
+  <si>
+    <t>Payment of Debt Issuance</t>
+  </si>
+  <si>
+    <t>Payments of Business Combination</t>
+  </si>
+  <si>
+    <t>CFFF</t>
+  </si>
+  <si>
+    <t>Model NI</t>
+  </si>
+  <si>
+    <t>Reported NI</t>
+  </si>
+  <si>
+    <t>Prepaid Expenses &amp; OCA</t>
+  </si>
+  <si>
+    <t>Other Assets</t>
+  </si>
+  <si>
+    <t>Accrued Expenses &amp; OCL</t>
+  </si>
+  <si>
+    <t>Other LT Liability</t>
+  </si>
+  <si>
+    <t>Operating Lease Liabilities</t>
+  </si>
+  <si>
+    <t>Deferred Revenues</t>
+  </si>
+  <si>
+    <t>Deferred Cost of Revenues</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="10">
+  <numFmts count="11">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
@@ -803,10 +890,32 @@
     <numFmt numFmtId="170" formatCode="#,##0.0_);[Red]\(#,##0.0\)"/>
     <numFmt numFmtId="171" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="172" formatCode="0.0\x"/>
+    <numFmt numFmtId="175" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts count="48" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1344,598 +1453,610 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="273">
+  <cellXfs count="283">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="4" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="28" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="17" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="37" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="25" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="28" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="25" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="28" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="25" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="25" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="25" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="25" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="28" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="28" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="37" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="28" fillId="10" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="28" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="28" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="28" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="17" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="20" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="28" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="25" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="25" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="25" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="28" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="20" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="37" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="38" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="38" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="38" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="3" fontId="37" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="13" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="38" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="37" fillId="11" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="38" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="28" fillId="11" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="42" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="43" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="28" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="25" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="28" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="25" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="25" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="25" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="25" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="28" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="28" fillId="12" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="38" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="28" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="17" fontId="34" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="34" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="25" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="25" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="22" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="22" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="6" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="6" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="6" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="37" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="38" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="38" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="38" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="37" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="13" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="38" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="37" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="38" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="28" fillId="8" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="39" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="37" fillId="10" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="17" fontId="34" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="28" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="25" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="25" fillId="10" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="38" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="37" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="22" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="3" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="25" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="25" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="175" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="22" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="14" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="17" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="22" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="22" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="22" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="22" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="22" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="25" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="17" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="34" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="35" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="35" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="35" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="35" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="34" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="10" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="35" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="34" fillId="11" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="35" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="25" fillId="11" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="39" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="40" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="25" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="25" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="22" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="22" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="171" fontId="25" fillId="12" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="35" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="35" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="17" fontId="25" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="172" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="34" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="35" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="35" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="35" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="35" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="34" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="10" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="35" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="34" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="35" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="171" fontId="25" fillId="8" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="36" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="34" fillId="10" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="22" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="35" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="34" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="22" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="22" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent3" xfId="5" builtinId="38"/>
@@ -3450,8 +3571,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3466,8 +3587,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10877550" y="0"/>
-          <a:ext cx="0" cy="17211675"/>
+          <a:off x="10191750" y="0"/>
+          <a:ext cx="0" cy="22745700"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3500,7 +3621,7 @@
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>85</xdr:row>
+      <xdr:row>122</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3516,8 +3637,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17145000" y="0"/>
-          <a:ext cx="0" cy="15782925"/>
+          <a:off x="17154525" y="0"/>
+          <a:ext cx="0" cy="23955375"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3983,8 +4104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE4A73D-2F46-7341-9C57-6E5B7A39A15C}">
   <dimension ref="B1:AL86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:AL1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4002,36 +4123,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="L1" s="269" t="s">
+      <c r="L1" s="262" t="s">
         <v>125</v>
       </c>
-      <c r="M1" s="270"/>
-      <c r="N1" s="270"/>
-      <c r="O1" s="270"/>
-      <c r="P1" s="270"/>
-      <c r="Q1" s="270"/>
-      <c r="R1" s="270"/>
-      <c r="S1" s="270"/>
-      <c r="T1" s="270"/>
-      <c r="U1" s="271"/>
-      <c r="W1" s="264" t="s">
+      <c r="M1" s="263"/>
+      <c r="N1" s="263"/>
+      <c r="O1" s="263"/>
+      <c r="P1" s="263"/>
+      <c r="Q1" s="263"/>
+      <c r="R1" s="263"/>
+      <c r="S1" s="263"/>
+      <c r="T1" s="263"/>
+      <c r="U1" s="264"/>
+      <c r="W1" s="265" t="s">
         <v>127</v>
       </c>
-      <c r="X1" s="265"/>
-      <c r="Y1" s="265"/>
-      <c r="Z1" s="265"/>
-      <c r="AA1" s="265"/>
-      <c r="AB1" s="265"/>
-      <c r="AC1" s="265"/>
-      <c r="AD1" s="265"/>
-      <c r="AE1" s="265"/>
-      <c r="AF1" s="265"/>
-      <c r="AG1" s="265"/>
-      <c r="AH1" s="265"/>
-      <c r="AI1" s="265"/>
-      <c r="AJ1" s="265"/>
-      <c r="AK1" s="265"/>
-      <c r="AL1" s="266"/>
+      <c r="X1" s="266"/>
+      <c r="Y1" s="266"/>
+      <c r="Z1" s="266"/>
+      <c r="AA1" s="266"/>
+      <c r="AB1" s="266"/>
+      <c r="AC1" s="266"/>
+      <c r="AD1" s="266"/>
+      <c r="AE1" s="266"/>
+      <c r="AF1" s="266"/>
+      <c r="AG1" s="266"/>
+      <c r="AH1" s="266"/>
+      <c r="AI1" s="266"/>
+      <c r="AJ1" s="266"/>
+      <c r="AK1" s="266"/>
+      <c r="AL1" s="267"/>
     </row>
     <row r="2" spans="2:38" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
@@ -4230,16 +4351,16 @@
       </c>
     </row>
     <row r="5" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B5" s="250" t="s">
+      <c r="B5" s="254" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="251"/>
-      <c r="D5" s="252"/>
-      <c r="F5" s="250" t="s">
+      <c r="C5" s="255"/>
+      <c r="D5" s="256"/>
+      <c r="F5" s="254" t="s">
         <v>193</v>
       </c>
-      <c r="G5" s="251"/>
-      <c r="H5" s="252"/>
+      <c r="G5" s="255"/>
+      <c r="H5" s="256"/>
       <c r="K5" s="28" t="s">
         <v>73</v>
       </c>
@@ -4347,10 +4468,10 @@
       <c r="F6" s="176" t="s">
         <v>194</v>
       </c>
-      <c r="G6" s="267" t="s">
+      <c r="G6" s="257" t="s">
         <v>198</v>
       </c>
-      <c r="H6" s="256"/>
+      <c r="H6" s="253"/>
       <c r="K6" s="28" t="s">
         <v>74</v>
       </c>
@@ -4455,10 +4576,10 @@
       <c r="F7" s="176" t="s">
         <v>195</v>
       </c>
-      <c r="G7" s="255">
+      <c r="G7" s="258">
         <v>2004</v>
       </c>
-      <c r="H7" s="256"/>
+      <c r="H7" s="253"/>
       <c r="K7" s="28"/>
       <c r="L7" s="60"/>
       <c r="M7" s="60"/>
@@ -4499,11 +4620,11 @@
       <c r="F8" s="176" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="255">
+      <c r="G8" s="258">
         <f>AL4</f>
         <v>58.8</v>
       </c>
-      <c r="H8" s="256"/>
+      <c r="H8" s="253"/>
       <c r="K8" s="28" t="s">
         <v>75</v>
       </c>
@@ -4598,8 +4719,8 @@
         <v>Q322</v>
       </c>
       <c r="F9" s="162"/>
-      <c r="G9" s="255"/>
-      <c r="H9" s="256"/>
+      <c r="G9" s="258"/>
+      <c r="H9" s="253"/>
       <c r="K9" s="28" t="s">
         <v>77</v>
       </c>
@@ -4708,8 +4829,8 @@
         <v>Q322</v>
       </c>
       <c r="F10" s="162"/>
-      <c r="G10" s="255"/>
-      <c r="H10" s="256"/>
+      <c r="G10" s="258"/>
+      <c r="H10" s="253"/>
       <c r="K10" s="28" t="s">
         <v>78</v>
       </c>
@@ -4817,10 +4938,10 @@
       <c r="F11" s="176" t="s">
         <v>199</v>
       </c>
-      <c r="G11" s="268" t="s">
+      <c r="G11" s="259" t="s">
         <v>109</v>
       </c>
-      <c r="H11" s="256"/>
+      <c r="H11" s="253"/>
       <c r="K11" s="28"/>
       <c r="L11" s="60"/>
       <c r="M11" s="60"/>
@@ -4850,10 +4971,10 @@
       <c r="F12" s="177" t="s">
         <v>196</v>
       </c>
-      <c r="G12" s="259" t="s">
+      <c r="G12" s="260" t="s">
         <v>197</v>
       </c>
-      <c r="H12" s="260"/>
+      <c r="H12" s="261"/>
       <c r="K12" s="28" t="s">
         <v>76</v>
       </c>
@@ -5125,16 +5246,16 @@
       </c>
     </row>
     <row r="15" spans="2:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="250" t="s">
+      <c r="B15" s="254" t="s">
         <v>130</v>
       </c>
-      <c r="C15" s="251"/>
-      <c r="D15" s="252"/>
-      <c r="F15" s="250" t="s">
+      <c r="C15" s="255"/>
+      <c r="D15" s="256"/>
+      <c r="F15" s="254" t="s">
         <v>204</v>
       </c>
-      <c r="G15" s="251"/>
-      <c r="H15" s="252"/>
+      <c r="G15" s="255"/>
+      <c r="H15" s="256"/>
       <c r="K15" s="28"/>
       <c r="L15" s="62"/>
       <c r="M15" s="62"/>
@@ -5151,18 +5272,18 @@
       <c r="B16" s="92" t="s">
         <v>132</v>
       </c>
-      <c r="C16" s="263" t="s">
+      <c r="C16" s="252" t="s">
         <v>131</v>
       </c>
-      <c r="D16" s="256"/>
+      <c r="D16" s="253"/>
       <c r="F16" s="176" t="s">
         <v>205</v>
       </c>
-      <c r="G16" s="257">
+      <c r="G16" s="270">
         <f>C6/'Financial Model'!M64</f>
         <v>44.601967818517387</v>
       </c>
-      <c r="H16" s="258"/>
+      <c r="H16" s="271"/>
       <c r="J16" s="31" t="s">
         <v>86</v>
       </c>
@@ -5240,7 +5361,7 @@
       <c r="AK16" s="32">
         <v>11300</v>
       </c>
-      <c r="AL16" s="272">
+      <c r="AL16" s="250">
         <v>13400</v>
       </c>
     </row>
@@ -5248,18 +5369,18 @@
       <c r="B17" s="104" t="s">
         <v>164</v>
       </c>
-      <c r="C17" s="253" t="s">
+      <c r="C17" s="268" t="s">
         <v>165</v>
       </c>
-      <c r="D17" s="254"/>
+      <c r="D17" s="269"/>
       <c r="F17" s="176" t="s">
         <v>214</v>
       </c>
-      <c r="G17" s="257">
+      <c r="G17" s="270">
         <f>C8/'Financial Model'!W3</f>
         <v>9.8675626321852903</v>
       </c>
-      <c r="H17" s="258"/>
+      <c r="H17" s="271"/>
       <c r="K17" s="28" t="s">
         <v>84</v>
       </c>
@@ -5356,18 +5477,18 @@
       <c r="B18" s="92" t="s">
         <v>133</v>
       </c>
-      <c r="C18" s="263" t="s">
+      <c r="C18" s="252" t="s">
         <v>134</v>
       </c>
-      <c r="D18" s="256"/>
+      <c r="D18" s="253"/>
       <c r="F18" s="176" t="s">
         <v>215</v>
       </c>
-      <c r="G18" s="257">
+      <c r="G18" s="270">
         <f>C6/SUM('Financial Model'!J19:M19)</f>
         <v>-23.723072493855522</v>
       </c>
-      <c r="H18" s="258"/>
+      <c r="H18" s="271"/>
       <c r="K18" s="28" t="s">
         <v>85</v>
       </c>
@@ -5459,22 +5580,22 @@
     </row>
     <row r="19" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B19" s="90"/>
-      <c r="C19" s="255"/>
-      <c r="D19" s="256"/>
+      <c r="C19" s="258"/>
+      <c r="D19" s="253"/>
       <c r="F19" s="176"/>
-      <c r="G19" s="255"/>
-      <c r="H19" s="256"/>
+      <c r="G19" s="258"/>
+      <c r="H19" s="253"/>
       <c r="K19" s="28"/>
       <c r="L19" s="62"/>
       <c r="M19" s="62"/>
     </row>
     <row r="20" spans="2:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="91"/>
-      <c r="C20" s="261"/>
-      <c r="D20" s="262"/>
+      <c r="C20" s="272"/>
+      <c r="D20" s="273"/>
       <c r="F20" s="177"/>
-      <c r="G20" s="259"/>
-      <c r="H20" s="260"/>
+      <c r="G20" s="260"/>
+      <c r="H20" s="261"/>
       <c r="J20" s="31"/>
       <c r="K20" s="195" t="s">
         <v>213</v>
@@ -5505,14 +5626,14 @@
       </c>
     </row>
     <row r="23" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B23" s="250" t="s">
+      <c r="B23" s="254" t="s">
         <v>159</v>
       </c>
-      <c r="C23" s="251"/>
-      <c r="D23" s="251"/>
-      <c r="E23" s="251"/>
-      <c r="F23" s="251"/>
-      <c r="G23" s="252"/>
+      <c r="C23" s="255"/>
+      <c r="D23" s="255"/>
+      <c r="E23" s="255"/>
+      <c r="F23" s="255"/>
+      <c r="G23" s="256"/>
       <c r="K23" s="195" t="s">
         <v>210</v>
       </c>
@@ -5624,12 +5745,12 @@
       <c r="F31" s="101"/>
       <c r="G31" s="102"/>
       <c r="J31" s="7"/>
-      <c r="K31" s="250" t="s">
+      <c r="K31" s="254" t="s">
         <v>181</v>
       </c>
-      <c r="L31" s="251"/>
-      <c r="M31" s="251"/>
-      <c r="N31" s="252"/>
+      <c r="L31" s="255"/>
+      <c r="M31" s="255"/>
+      <c r="N31" s="256"/>
     </row>
     <row r="32" spans="2:38" x14ac:dyDescent="0.25">
       <c r="J32" s="7"/>
@@ -5641,14 +5762,14 @@
       <c r="N32" s="96"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="250" t="s">
+      <c r="B33" s="254" t="s">
         <v>187</v>
       </c>
-      <c r="C33" s="251"/>
-      <c r="D33" s="251"/>
-      <c r="E33" s="251"/>
-      <c r="F33" s="251"/>
-      <c r="G33" s="252"/>
+      <c r="C33" s="255"/>
+      <c r="D33" s="255"/>
+      <c r="E33" s="255"/>
+      <c r="F33" s="255"/>
+      <c r="G33" s="256"/>
       <c r="J33" s="7"/>
       <c r="K33" s="168" t="s">
         <v>177</v>
@@ -6096,15 +6217,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
     <mergeCell ref="L1:U1"/>
     <mergeCell ref="W1:AL1"/>
     <mergeCell ref="B33:G33"/>
@@ -6121,9 +6233,18 @@
     <mergeCell ref="B23:G23"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="C16:D16"/>
   </mergeCells>
-  <phoneticPr fontId="24" type="noConversion"/>
+  <phoneticPr fontId="27" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K58" r:id="rId1" xr:uid="{F79BC045-05D5-43FB-A051-BA2031CC85A7}"/>
     <hyperlink ref="K60" r:id="rId2" xr:uid="{58004FA9-9F7A-4B71-811E-FF4EE09F281F}"/>
@@ -6137,19 +6258,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0FDCAC-3416-844A-BCBB-390EC350CF59}">
-  <dimension ref="B1:BZ82"/>
+  <dimension ref="B1:BZ116"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C54" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J85" sqref="J85"/>
+      <selection pane="bottomRight" activeCell="M83" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="6" customWidth="1"/>
-    <col min="2" max="2" width="29.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.125" customWidth="1"/>
     <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
@@ -11573,39 +11694,1012 @@
         <f>M70/SUM(J19:M19)</f>
         <v>-26.838223427392109</v>
       </c>
+      <c r="P77" s="251"/>
+    </row>
+    <row r="78" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B78" s="251" t="s">
+        <v>254</v>
+      </c>
+      <c r="G78" s="87">
+        <f t="shared" ref="G78:L78" si="132">SUM(D12:G12)/(G48-SUM(G50:G53))</f>
+        <v>-0.25137548210801064</v>
+      </c>
+      <c r="H78" s="87">
+        <f t="shared" si="132"/>
+        <v>-0.30583278280508219</v>
+      </c>
+      <c r="I78" s="87">
+        <f t="shared" si="132"/>
+        <v>-0.31302756573649004</v>
+      </c>
+      <c r="J78" s="87">
+        <f t="shared" si="132"/>
+        <v>-0.20685053640976875</v>
+      </c>
+      <c r="K78" s="87">
+        <f t="shared" si="132"/>
+        <v>-0.2013507520159552</v>
+      </c>
+      <c r="L78" s="87">
+        <f t="shared" si="132"/>
+        <v>-0.20293605022212965</v>
+      </c>
+      <c r="M78" s="87">
+        <f>SUM(J12:M12)/(M48-SUM(M50:M53))</f>
+        <v>-0.27196075945524634</v>
+      </c>
+      <c r="P78" s="251"/>
+    </row>
+    <row r="79" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B79" s="251"/>
+      <c r="G79" s="87"/>
+      <c r="H79" s="87"/>
+      <c r="I79" s="87"/>
+      <c r="J79" s="87"/>
+      <c r="K79" s="87"/>
+      <c r="L79" s="87"/>
+      <c r="M79" s="87"/>
+      <c r="P79" s="251"/>
     </row>
     <row r="80" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="F80" s="5"/>
-      <c r="G80" s="5"/>
-      <c r="H80" s="5"/>
-      <c r="I80" s="5"/>
-      <c r="J80" s="5"/>
-      <c r="K80" s="5"/>
-      <c r="L80" s="5"/>
-      <c r="M80" s="5"/>
-    </row>
-    <row r="81" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="B80" s="251"/>
+      <c r="G80" s="87"/>
+      <c r="H80" s="87"/>
+      <c r="I80" s="87"/>
+      <c r="J80" s="87"/>
+      <c r="K80" s="87"/>
+      <c r="L80" s="87"/>
+      <c r="M80" s="87"/>
+      <c r="P80" s="251"/>
+    </row>
+    <row r="81" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="275" t="s">
+        <v>273</v>
+      </c>
+      <c r="C81" s="276"/>
+      <c r="D81" s="276"/>
+      <c r="E81" s="276"/>
       <c r="F81" s="5"/>
       <c r="G81" s="5"/>
-      <c r="H81" s="5"/>
-      <c r="I81" s="5"/>
-      <c r="J81" s="5"/>
-      <c r="K81" s="5"/>
-      <c r="L81" s="5"/>
-      <c r="M81" s="5"/>
-    </row>
-    <row r="82" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="H81" s="5">
+        <f>H18</f>
+        <v>-142.93999999999997</v>
+      </c>
+      <c r="I81" s="5">
+        <f>I18</f>
+        <v>-77.189999999999955</v>
+      </c>
+      <c r="J81" s="5">
+        <f t="shared" ref="J81:L81" si="133">J18</f>
+        <v>-147.25700000000003</v>
+      </c>
+      <c r="K81" s="5">
+        <f t="shared" si="133"/>
+        <v>-162.00600000000003</v>
+      </c>
+      <c r="L81" s="5">
+        <f t="shared" si="133"/>
+        <v>-179.29000000000002</v>
+      </c>
+      <c r="M81" s="5">
+        <f>M18</f>
+        <v>-301.90200000000004</v>
+      </c>
+      <c r="N81" s="118"/>
+      <c r="P81" s="277"/>
+      <c r="Q81" s="5"/>
+      <c r="R81" s="5"/>
+      <c r="S81" s="5"/>
+    </row>
+    <row r="82" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="275" t="s">
+        <v>274</v>
+      </c>
+      <c r="C82" s="276"/>
+      <c r="D82" s="276"/>
+      <c r="E82" s="276"/>
       <c r="F82" s="5"/>
       <c r="G82" s="5"/>
-      <c r="H82" s="5"/>
-      <c r="I82" s="5"/>
+      <c r="H82" s="5">
+        <v>-142.93</v>
+      </c>
+      <c r="I82" s="5">
+        <v>-77.19</v>
+      </c>
       <c r="J82" s="5"/>
       <c r="K82" s="5"/>
-      <c r="L82" s="5"/>
-      <c r="M82" s="5"/>
+      <c r="L82" s="5">
+        <v>-178.73400000000001</v>
+      </c>
+      <c r="M82" s="5">
+        <v>-301.90199999999999</v>
+      </c>
+      <c r="N82" s="118"/>
+      <c r="P82" s="277"/>
+      <c r="Q82" s="5"/>
+      <c r="R82" s="5"/>
+      <c r="S82" s="5"/>
+    </row>
+    <row r="83" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="278"/>
+      <c r="C83" s="276"/>
+      <c r="D83" s="276"/>
+      <c r="E83" s="276"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
+      <c r="I83" s="5"/>
+      <c r="J83" s="5"/>
+      <c r="K83" s="5"/>
+      <c r="L83" s="5"/>
+      <c r="M83" s="5"/>
+      <c r="N83" s="118"/>
+      <c r="Q83" s="5"/>
+      <c r="R83" s="5"/>
+      <c r="S83" s="5"/>
+    </row>
+    <row r="84" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="279" t="s">
+        <v>253</v>
+      </c>
+      <c r="C84" s="276"/>
+      <c r="D84" s="276"/>
+      <c r="E84" s="276"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="5"/>
+      <c r="J84" s="5"/>
+      <c r="K84" s="5"/>
+      <c r="L84" s="5"/>
+      <c r="M84" s="5"/>
+      <c r="N84" s="118"/>
+      <c r="Q84" s="5"/>
+      <c r="R84" s="5"/>
+      <c r="S84" s="5"/>
+    </row>
+    <row r="85" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="280" t="s">
+        <v>255</v>
+      </c>
+      <c r="C85" s="276"/>
+      <c r="D85" s="276"/>
+      <c r="E85" s="276"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5">
+        <v>17.79</v>
+      </c>
+      <c r="I85" s="5">
+        <v>19.029</v>
+      </c>
+      <c r="J85" s="5"/>
+      <c r="K85" s="5"/>
+      <c r="L85" s="5">
+        <v>28.995999999999999</v>
+      </c>
+      <c r="M85" s="5">
+        <v>34.052</v>
+      </c>
+      <c r="N85" s="118"/>
+      <c r="Q85" s="5"/>
+      <c r="R85" s="5"/>
+      <c r="S85" s="5"/>
+    </row>
+    <row r="86" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="280" t="s">
+        <v>256</v>
+      </c>
+      <c r="C86" s="276"/>
+      <c r="D86" s="276"/>
+      <c r="E86" s="276"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="5">
+        <v>81.659000000000006</v>
+      </c>
+      <c r="I86" s="5">
+        <v>89.319000000000003</v>
+      </c>
+      <c r="J86" s="5"/>
+      <c r="K86" s="5"/>
+      <c r="L86" s="5">
+        <v>146.38800000000001</v>
+      </c>
+      <c r="M86" s="5">
+        <v>161.35900000000001</v>
+      </c>
+      <c r="N86" s="118"/>
+      <c r="Q86" s="5"/>
+      <c r="R86" s="5"/>
+      <c r="S86" s="5"/>
+    </row>
+    <row r="87" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="280" t="s">
+        <v>258</v>
+      </c>
+      <c r="C87" s="276"/>
+      <c r="D87" s="276"/>
+      <c r="E87" s="276"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5"/>
+      <c r="H87" s="5">
+        <v>10.5</v>
+      </c>
+      <c r="I87" s="5">
+        <v>11.391999999999999</v>
+      </c>
+      <c r="J87" s="5"/>
+      <c r="K87" s="5"/>
+      <c r="L87" s="5">
+        <v>16.303000000000001</v>
+      </c>
+      <c r="M87" s="5">
+        <v>18.815000000000001</v>
+      </c>
+      <c r="N87" s="118"/>
+      <c r="Q87" s="5"/>
+      <c r="R87" s="5"/>
+      <c r="S87" s="5"/>
+    </row>
+    <row r="88" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="280" t="s">
+        <v>257</v>
+      </c>
+      <c r="C88" s="276"/>
+      <c r="D88" s="276"/>
+      <c r="E88" s="276"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="5">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="I88" s="5">
+        <v>1.121</v>
+      </c>
+      <c r="J88" s="5"/>
+      <c r="K88" s="5"/>
+      <c r="L88" s="5">
+        <v>2.048</v>
+      </c>
+      <c r="M88" s="5">
+        <v>-1.5149999999999999</v>
+      </c>
+      <c r="N88" s="118"/>
+      <c r="Q88" s="5"/>
+      <c r="R88" s="5"/>
+      <c r="S88" s="5"/>
+    </row>
+    <row r="89" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="280" t="s">
+        <v>259</v>
+      </c>
+      <c r="C89" s="276"/>
+      <c r="D89" s="276"/>
+      <c r="E89" s="276"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="5"/>
+      <c r="H89" s="5">
+        <v>0</v>
+      </c>
+      <c r="I89" s="5">
+        <v>0</v>
+      </c>
+      <c r="J89" s="5"/>
+      <c r="K89" s="5"/>
+      <c r="L89" s="5">
+        <v>0.311</v>
+      </c>
+      <c r="M89" s="5">
+        <v>0.318</v>
+      </c>
+      <c r="N89" s="118"/>
+      <c r="Q89" s="5"/>
+      <c r="R89" s="5"/>
+      <c r="S89" s="5"/>
+    </row>
+    <row r="90" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="280" t="s">
+        <v>260</v>
+      </c>
+      <c r="C90" s="276"/>
+      <c r="D90" s="276"/>
+      <c r="E90" s="276"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="5"/>
+      <c r="H90" s="9">
+        <f>SUM(H91:H100)</f>
+        <v>224.16400000000004</v>
+      </c>
+      <c r="I90" s="9">
+        <f>SUM(I91:I100)</f>
+        <v>137.49499999999998</v>
+      </c>
+      <c r="J90" s="5"/>
+      <c r="K90" s="5"/>
+      <c r="L90" s="9">
+        <f>SUM(L91:L100)</f>
+        <v>11.184999999999997</v>
+      </c>
+      <c r="M90" s="9">
+        <f>SUM(M91:M100)</f>
+        <v>156.023</v>
+      </c>
+      <c r="N90" s="118"/>
+      <c r="Q90" s="5"/>
+      <c r="R90" s="5"/>
+      <c r="S90" s="5"/>
+    </row>
+    <row r="91" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="275" t="s">
+        <v>37</v>
+      </c>
+      <c r="C91" s="276"/>
+      <c r="D91" s="276"/>
+      <c r="E91" s="276"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="5"/>
+      <c r="H91" s="5">
+        <v>16.704000000000001</v>
+      </c>
+      <c r="I91" s="5">
+        <v>47.125999999999998</v>
+      </c>
+      <c r="J91" s="5"/>
+      <c r="K91" s="5"/>
+      <c r="L91" s="5">
+        <v>-9.8650000000000002</v>
+      </c>
+      <c r="M91" s="5">
+        <v>1.63</v>
+      </c>
+      <c r="N91" s="118"/>
+      <c r="Q91" s="5"/>
+      <c r="R91" s="5"/>
+      <c r="S91" s="5"/>
+    </row>
+    <row r="92" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="275" t="s">
+        <v>46</v>
+      </c>
+      <c r="C92" s="276"/>
+      <c r="D92" s="276"/>
+      <c r="E92" s="276"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="5">
+        <v>3.0950000000000002</v>
+      </c>
+      <c r="I92" s="5">
+        <v>-2.5430000000000001</v>
+      </c>
+      <c r="J92" s="5"/>
+      <c r="K92" s="5"/>
+      <c r="L92" s="5">
+        <v>-6.867</v>
+      </c>
+      <c r="M92" s="5">
+        <v>2.3039999999999998</v>
+      </c>
+      <c r="N92" s="118"/>
+      <c r="Q92" s="5"/>
+      <c r="R92" s="5"/>
+      <c r="S92" s="5"/>
+    </row>
+    <row r="93" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="275" t="s">
+        <v>275</v>
+      </c>
+      <c r="C93" s="276"/>
+      <c r="D93" s="276"/>
+      <c r="E93" s="276"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="5">
+        <v>-16.297000000000001</v>
+      </c>
+      <c r="I93" s="5">
+        <v>7.7629999999999999</v>
+      </c>
+      <c r="J93" s="5"/>
+      <c r="K93" s="5"/>
+      <c r="L93" s="5">
+        <v>-15.983000000000001</v>
+      </c>
+      <c r="M93" s="5">
+        <v>-15.680999999999999</v>
+      </c>
+      <c r="N93" s="118"/>
+      <c r="Q93" s="5"/>
+      <c r="R93" s="5"/>
+      <c r="S93" s="5"/>
+    </row>
+    <row r="94" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="275" t="s">
+        <v>276</v>
+      </c>
+      <c r="C94" s="276"/>
+      <c r="D94" s="276"/>
+      <c r="E94" s="276"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="5">
+        <v>-3.0750000000000002</v>
+      </c>
+      <c r="I94" s="5">
+        <v>2.2879999999999998</v>
+      </c>
+      <c r="J94" s="5"/>
+      <c r="K94" s="5"/>
+      <c r="L94" s="5">
+        <v>1.1990000000000001</v>
+      </c>
+      <c r="M94" s="9">
+        <v>-0.26600000000000001</v>
+      </c>
+      <c r="N94" s="118"/>
+      <c r="Q94" s="5"/>
+      <c r="R94" s="5"/>
+      <c r="S94" s="5"/>
+    </row>
+    <row r="95" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="275" t="s">
+        <v>48</v>
+      </c>
+      <c r="C95" s="276"/>
+      <c r="D95" s="276"/>
+      <c r="E95" s="276"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="5">
+        <v>6.2779999999999996</v>
+      </c>
+      <c r="I95" s="5">
+        <v>27.140999999999998</v>
+      </c>
+      <c r="J95" s="5"/>
+      <c r="K95" s="5"/>
+      <c r="L95" s="5">
+        <v>-2.6240000000000001</v>
+      </c>
+      <c r="M95" s="5">
+        <v>21.175000000000001</v>
+      </c>
+      <c r="N95" s="118"/>
+      <c r="Q95" s="5"/>
+      <c r="R95" s="5"/>
+      <c r="S95" s="5"/>
+    </row>
+    <row r="96" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="275" t="s">
+        <v>277</v>
+      </c>
+      <c r="C96" s="276"/>
+      <c r="D96" s="276"/>
+      <c r="E96" s="276"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="5">
+        <v>57.856000000000002</v>
+      </c>
+      <c r="I96" s="5">
+        <v>-36.030999999999999</v>
+      </c>
+      <c r="J96" s="5"/>
+      <c r="K96" s="5"/>
+      <c r="L96" s="5">
+        <v>6.4059999999999997</v>
+      </c>
+      <c r="M96" s="5">
+        <v>2.6419999999999999</v>
+      </c>
+      <c r="N96" s="118"/>
+      <c r="Q96" s="5"/>
+      <c r="R96" s="5"/>
+      <c r="S96" s="5"/>
+    </row>
+    <row r="97" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="275" t="s">
+        <v>278</v>
+      </c>
+      <c r="C97" s="276"/>
+      <c r="D97" s="276"/>
+      <c r="E97" s="276"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="5"/>
+      <c r="H97" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I97" s="5">
+        <v>-1.6060000000000001</v>
+      </c>
+      <c r="J97" s="5"/>
+      <c r="K97" s="5"/>
+      <c r="L97" s="5">
+        <v>-0.57899999999999996</v>
+      </c>
+      <c r="M97" s="9">
+        <v>0</v>
+      </c>
+      <c r="N97" s="118"/>
+      <c r="Q97" s="5"/>
+      <c r="R97" s="5"/>
+      <c r="S97" s="5"/>
+    </row>
+    <row r="98" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="275" t="s">
+        <v>279</v>
+      </c>
+      <c r="C98" s="276"/>
+      <c r="D98" s="276"/>
+      <c r="E98" s="276"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="5">
+        <v>-10.573</v>
+      </c>
+      <c r="I98" s="5">
+        <v>-11.413</v>
+      </c>
+      <c r="J98" s="5"/>
+      <c r="K98" s="5"/>
+      <c r="L98" s="5">
+        <v>-10.021000000000001</v>
+      </c>
+      <c r="M98" s="5">
+        <v>-11.259</v>
+      </c>
+      <c r="N98" s="118"/>
+      <c r="Q98" s="5"/>
+      <c r="R98" s="5"/>
+      <c r="S98" s="5"/>
+    </row>
+    <row r="99" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="275" t="s">
+        <v>280</v>
+      </c>
+      <c r="C99" s="276"/>
+      <c r="D99" s="276"/>
+      <c r="E99" s="276"/>
+      <c r="F99" s="5"/>
+      <c r="G99" s="5"/>
+      <c r="H99" s="5">
+        <v>215.49700000000001</v>
+      </c>
+      <c r="I99" s="5">
+        <v>131.43899999999999</v>
+      </c>
+      <c r="J99" s="5"/>
+      <c r="K99" s="5"/>
+      <c r="L99" s="5">
+        <v>52.14</v>
+      </c>
+      <c r="M99" s="5">
+        <v>187.99100000000001</v>
+      </c>
+      <c r="N99" s="118"/>
+      <c r="Q99" s="5"/>
+      <c r="R99" s="5"/>
+      <c r="S99" s="5"/>
+    </row>
+    <row r="100" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="275" t="s">
+        <v>281</v>
+      </c>
+      <c r="C100" s="276"/>
+      <c r="D100" s="276"/>
+      <c r="E100" s="276"/>
+      <c r="F100" s="5"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="5">
+        <v>-45.600999999999999</v>
+      </c>
+      <c r="I100" s="5">
+        <v>-26.669</v>
+      </c>
+      <c r="J100" s="5"/>
+      <c r="K100" s="5"/>
+      <c r="L100" s="5">
+        <v>-2.621</v>
+      </c>
+      <c r="M100" s="5">
+        <v>-32.512999999999998</v>
+      </c>
+      <c r="N100" s="118"/>
+      <c r="Q100" s="5"/>
+      <c r="R100" s="5"/>
+      <c r="S100" s="5"/>
+    </row>
+    <row r="101" spans="2:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C101" s="281"/>
+      <c r="D101" s="281"/>
+      <c r="E101" s="281"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4">
+        <f>H82+SUM(H85:H90)</f>
+        <v>191.25100000000003</v>
+      </c>
+      <c r="I101" s="4">
+        <f>I82+SUM(I85:I90)</f>
+        <v>181.166</v>
+      </c>
+      <c r="J101" s="4"/>
+      <c r="K101" s="4"/>
+      <c r="L101" s="4">
+        <f>L82+SUM(L85:L90)</f>
+        <v>26.497000000000014</v>
+      </c>
+      <c r="M101" s="4">
+        <f>M82+SUM(M85:M90)</f>
+        <v>67.150000000000034</v>
+      </c>
+      <c r="N101" s="117"/>
+      <c r="Q101" s="4"/>
+      <c r="R101" s="4"/>
+      <c r="S101" s="4"/>
+    </row>
+    <row r="102" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="278"/>
+      <c r="C102" s="276"/>
+      <c r="D102" s="276"/>
+      <c r="E102" s="276"/>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
+      <c r="I102" s="5"/>
+      <c r="J102" s="5"/>
+      <c r="K102" s="5"/>
+      <c r="L102" s="5"/>
+      <c r="M102" s="5"/>
+      <c r="N102" s="118"/>
+      <c r="Q102" s="5"/>
+      <c r="R102" s="5"/>
+      <c r="S102" s="5"/>
+    </row>
+    <row r="103" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="280" t="s">
+        <v>262</v>
+      </c>
+      <c r="C103" s="276"/>
+      <c r="D103" s="276"/>
+      <c r="E103" s="276"/>
+      <c r="F103" s="5"/>
+      <c r="G103" s="5"/>
+      <c r="H103" s="5">
+        <v>-23.234999999999999</v>
+      </c>
+      <c r="I103" s="5">
+        <v>-2.9620000000000002</v>
+      </c>
+      <c r="J103" s="5"/>
+      <c r="K103" s="5"/>
+      <c r="L103" s="5">
+        <v>-83.811999999999998</v>
+      </c>
+      <c r="M103" s="5">
+        <v>-133.35599999999999</v>
+      </c>
+      <c r="N103" s="118"/>
+      <c r="Q103" s="5"/>
+      <c r="R103" s="5"/>
+      <c r="S103" s="5"/>
+    </row>
+    <row r="104" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="280" t="s">
+        <v>263</v>
+      </c>
+      <c r="C104" s="276"/>
+      <c r="D104" s="276"/>
+      <c r="E104" s="276"/>
+      <c r="F104" s="5"/>
+      <c r="G104" s="5"/>
+      <c r="H104" s="5">
+        <v>0</v>
+      </c>
+      <c r="I104" s="5">
+        <v>-45.692</v>
+      </c>
+      <c r="J104" s="5"/>
+      <c r="K104" s="5"/>
+      <c r="L104" s="5">
+        <v>-6.165</v>
+      </c>
+      <c r="M104" s="5">
+        <v>0</v>
+      </c>
+      <c r="N104" s="118"/>
+      <c r="Q104" s="5"/>
+      <c r="R104" s="5"/>
+      <c r="S104" s="5"/>
+    </row>
+    <row r="105" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="280" t="s">
+        <v>264</v>
+      </c>
+      <c r="C105" s="276"/>
+      <c r="D105" s="276"/>
+      <c r="E105" s="276"/>
+      <c r="F105" s="5"/>
+      <c r="G105" s="5"/>
+      <c r="H105" s="5">
+        <v>0</v>
+      </c>
+      <c r="I105" s="5">
+        <v>-7.6</v>
+      </c>
+      <c r="J105" s="5"/>
+      <c r="K105" s="5"/>
+      <c r="L105" s="5">
+        <v>0</v>
+      </c>
+      <c r="M105" s="5">
+        <v>-1.5</v>
+      </c>
+      <c r="N105" s="118"/>
+      <c r="Q105" s="5"/>
+      <c r="R105" s="5"/>
+      <c r="S105" s="5"/>
+    </row>
+    <row r="106" spans="2:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C106" s="281"/>
+      <c r="D106" s="281"/>
+      <c r="E106" s="281"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="4"/>
+      <c r="H106" s="4">
+        <f>SUM(H103:H105)</f>
+        <v>-23.234999999999999</v>
+      </c>
+      <c r="I106" s="4">
+        <f>SUM(I103:I105)</f>
+        <v>-56.254000000000005</v>
+      </c>
+      <c r="J106" s="4"/>
+      <c r="K106" s="4"/>
+      <c r="L106" s="4">
+        <f>SUM(L103:L105)</f>
+        <v>-89.977000000000004</v>
+      </c>
+      <c r="M106" s="4">
+        <f>SUM(M103:M105)</f>
+        <v>-134.85599999999999</v>
+      </c>
+      <c r="N106" s="117"/>
+      <c r="Q106" s="4"/>
+      <c r="R106" s="4"/>
+      <c r="S106" s="4"/>
+    </row>
+    <row r="107" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="278"/>
+      <c r="C107" s="276"/>
+      <c r="D107" s="276"/>
+      <c r="E107" s="276"/>
+      <c r="F107" s="5"/>
+      <c r="G107" s="5"/>
+      <c r="H107" s="5"/>
+      <c r="I107" s="5"/>
+      <c r="J107" s="5"/>
+      <c r="K107" s="5"/>
+      <c r="L107" s="5"/>
+      <c r="M107" s="5"/>
+      <c r="N107" s="118"/>
+      <c r="Q107" s="5"/>
+      <c r="R107" s="5"/>
+      <c r="S107" s="5"/>
+    </row>
+    <row r="108" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="280" t="s">
+        <v>266</v>
+      </c>
+      <c r="C108" s="276"/>
+      <c r="D108" s="276"/>
+      <c r="E108" s="276"/>
+      <c r="F108" s="5"/>
+      <c r="G108" s="5"/>
+      <c r="H108" s="5">
+        <v>11.667999999999999</v>
+      </c>
+      <c r="I108" s="5">
+        <v>20.388999999999999</v>
+      </c>
+      <c r="J108" s="5"/>
+      <c r="K108" s="5"/>
+      <c r="L108" s="5">
+        <v>5.548</v>
+      </c>
+      <c r="M108" s="5">
+        <v>12.83</v>
+      </c>
+      <c r="N108" s="118"/>
+      <c r="Q108" s="5"/>
+      <c r="R108" s="5"/>
+      <c r="S108" s="5"/>
+    </row>
+    <row r="109" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="280" t="s">
+        <v>267</v>
+      </c>
+      <c r="C109" s="276"/>
+      <c r="D109" s="276"/>
+      <c r="E109" s="276"/>
+      <c r="F109" s="5"/>
+      <c r="G109" s="5"/>
+      <c r="H109" s="5">
+        <v>0</v>
+      </c>
+      <c r="I109" s="5">
+        <v>0</v>
+      </c>
+      <c r="J109" s="5"/>
+      <c r="K109" s="5"/>
+      <c r="L109" s="5">
+        <v>-0.42</v>
+      </c>
+      <c r="M109" s="5">
+        <v>0</v>
+      </c>
+      <c r="N109" s="118"/>
+      <c r="Q109" s="5"/>
+      <c r="R109" s="5"/>
+      <c r="S109" s="5"/>
+    </row>
+    <row r="110" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="280" t="s">
+        <v>268</v>
+      </c>
+      <c r="C110" s="276"/>
+      <c r="D110" s="276"/>
+      <c r="E110" s="276"/>
+      <c r="F110" s="5"/>
+      <c r="G110" s="5"/>
+      <c r="H110" s="5">
+        <v>0</v>
+      </c>
+      <c r="I110" s="5">
+        <v>0</v>
+      </c>
+      <c r="J110" s="5"/>
+      <c r="K110" s="5"/>
+      <c r="L110" s="5">
+        <v>0</v>
+      </c>
+      <c r="M110" s="5">
+        <v>0</v>
+      </c>
+      <c r="N110" s="118"/>
+      <c r="Q110" s="5"/>
+      <c r="R110" s="5"/>
+      <c r="S110" s="5"/>
+    </row>
+    <row r="111" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B111" s="280" t="s">
+        <v>269</v>
+      </c>
+      <c r="C111" s="276"/>
+      <c r="D111" s="276"/>
+      <c r="E111" s="276"/>
+      <c r="F111" s="5"/>
+      <c r="G111" s="5"/>
+      <c r="H111" s="5">
+        <v>0</v>
+      </c>
+      <c r="I111" s="5">
+        <v>0</v>
+      </c>
+      <c r="J111" s="5"/>
+      <c r="K111" s="5"/>
+      <c r="L111" s="5">
+        <v>0</v>
+      </c>
+      <c r="M111" s="5">
+        <v>0</v>
+      </c>
+      <c r="N111" s="118"/>
+      <c r="Q111" s="5"/>
+      <c r="R111" s="5"/>
+      <c r="S111" s="5"/>
+    </row>
+    <row r="112" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="280" t="s">
+        <v>270</v>
+      </c>
+      <c r="C112" s="276"/>
+      <c r="D112" s="276"/>
+      <c r="E112" s="276"/>
+      <c r="F112" s="5"/>
+      <c r="G112" s="5"/>
+      <c r="H112" s="5">
+        <v>0</v>
+      </c>
+      <c r="I112" s="5">
+        <v>0</v>
+      </c>
+      <c r="J112" s="5"/>
+      <c r="K112" s="5"/>
+      <c r="L112" s="5">
+        <v>0</v>
+      </c>
+      <c r="M112" s="5">
+        <v>0</v>
+      </c>
+      <c r="N112" s="118"/>
+      <c r="Q112" s="5"/>
+      <c r="R112" s="5"/>
+      <c r="S112" s="5"/>
+    </row>
+    <row r="113" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="280" t="s">
+        <v>271</v>
+      </c>
+      <c r="C113" s="276"/>
+      <c r="D113" s="276"/>
+      <c r="E113" s="276"/>
+      <c r="F113" s="5"/>
+      <c r="G113" s="5"/>
+      <c r="H113" s="5">
+        <v>0</v>
+      </c>
+      <c r="I113" s="5">
+        <v>0</v>
+      </c>
+      <c r="J113" s="5"/>
+      <c r="K113" s="5"/>
+      <c r="L113" s="5">
+        <v>0</v>
+      </c>
+      <c r="M113" s="5">
+        <v>-0.15</v>
+      </c>
+      <c r="N113" s="118"/>
+      <c r="Q113" s="5"/>
+      <c r="R113" s="5"/>
+      <c r="S113" s="5"/>
+    </row>
+    <row r="114" spans="2:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C114" s="281"/>
+      <c r="D114" s="281"/>
+      <c r="E114" s="281"/>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4"/>
+      <c r="H114" s="4">
+        <f>SUM(H108:H113)</f>
+        <v>11.667999999999999</v>
+      </c>
+      <c r="I114" s="4">
+        <f>SUM(I108:I113)</f>
+        <v>20.388999999999999</v>
+      </c>
+      <c r="J114" s="4"/>
+      <c r="K114" s="4"/>
+      <c r="L114" s="4">
+        <f>SUM(L108:L113)</f>
+        <v>5.1280000000000001</v>
+      </c>
+      <c r="M114" s="4">
+        <f>SUM(M108:M113)</f>
+        <v>12.68</v>
+      </c>
+      <c r="N114" s="117"/>
+      <c r="Q114" s="4"/>
+      <c r="R114" s="4"/>
+      <c r="S114" s="4"/>
+    </row>
+    <row r="116" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B116" s="274"/>
+      <c r="M116" s="282"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="24" type="noConversion"/>
+  <phoneticPr fontId="27" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="L1" r:id="rId1" xr:uid="{F0F1B078-C7E3-AA47-9924-08C1D4511F24}"/>
     <hyperlink ref="M1" r:id="rId2" xr:uid="{9D82E829-DF9B-4456-A9EF-305989A97DF8}"/>
@@ -11613,7 +12707,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="119" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId3"/>
   <ignoredErrors>
-    <ignoredError sqref="V3:V4 V6:V8 V9:V13 W3:W4 V17:V20 W17:W20 W6:W13 V15 W15 K75 K76 G75:J76 L75:M76" formulaRange="1"/>
+    <ignoredError sqref="V3:V4 V6:V8 V9:V13 W3:W4 V17:V20 W17:W20 W6:W13 V15 W15 K75 K76 G75:J76 L75:M76 G78:M78" formulaRange="1"/>
     <ignoredError sqref="V5 V16:W16 X5 V14 X16 X21 Y16:AK16 Y18 Z18:AK20 AL13:AM18 X18:X19 X14" formula="1"/>
     <ignoredError sqref="W5 W14" formula="1" formulaRange="1"/>
   </ignoredErrors>
@@ -13151,7 +14245,7 @@
       <c r="R24" s="109"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="24" type="noConversion"/>
+  <phoneticPr fontId="27" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
More Software models, updates to Overview
</commit_message>
<xml_diff>
--- a/$RBLX.xlsx
+++ b/$RBLX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547339AC-A919-43D6-9452-130501473D87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558D09B3-F6A4-4B55-BBD2-D0B12E82E084}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="18390" windowHeight="2400" activeTab="1" xr2:uid="{DB6ABC51-E0DE-6747-8CA5-53C172A4844D}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" xr2:uid="{DB6ABC51-E0DE-6747-8CA5-53C172A4844D}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="285">
   <si>
     <t>Price</t>
   </si>
@@ -623,9 +623,6 @@
     <t>Link</t>
   </si>
   <si>
-    <t>California, US</t>
-  </si>
-  <si>
     <t>Update</t>
   </si>
   <si>
@@ -873,13 +870,25 @@
   </si>
   <si>
     <t>Deferred Cost of Revenues</t>
+  </si>
+  <si>
+    <t>CapEx</t>
+  </si>
+  <si>
+    <t>FCF</t>
+  </si>
+  <si>
+    <t>IPO</t>
+  </si>
+  <si>
+    <t>San Mateo, CA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="11">
+  <numFmts count="10">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
@@ -890,11 +899,17 @@
     <numFmt numFmtId="170" formatCode="#,##0.0_);[Red]\(#,##0.0\)"/>
     <numFmt numFmtId="171" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="172" formatCode="0.0\x"/>
-    <numFmt numFmtId="175" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="48" x14ac:knownFonts="1">
+  <fonts count="49" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1246,7 +1261,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1321,6 +1336,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0E1FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1453,609 +1474,620 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="283">
+  <cellXfs count="288">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="26" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="26" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="17" fontId="38" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="38" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="26" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="29" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="26" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="29" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="26" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="26" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="26" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="26" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="29" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="38" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="29" fillId="10" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="29" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="26" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="26" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="26" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="29" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="29" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="18" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="21" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="26" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="26" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="26" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="26" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="26" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="29" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="21" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="38" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="39" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="39" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="39" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="38" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="14" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="39" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="38" fillId="11" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="39" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="29" fillId="11" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="43" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="44" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="28" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="25" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="17" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="37" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="25" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="28" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="25" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="28" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="25" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="25" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="25" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="25" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="28" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="28" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="17" fontId="37" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="28" fillId="10" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="28" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="28" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="28" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="17" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="20" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="28" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="25" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="25" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="25" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="28" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="20" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="37" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="38" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="38" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="38" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="38" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="37" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="13" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="38" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="37" fillId="11" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="38" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="28" fillId="11" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="42" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="43" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="29" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="28" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="26" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="29" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="28" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="26" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="25" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="26" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="25" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="26" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="25" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="26" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="25" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="26" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="25" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="26" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="25" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="29" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="28" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="29" fillId="12" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="28" fillId="12" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="26" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="25" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="39" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="38" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="39" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="38" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="29" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="17" fontId="28" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="38" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="39" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="39" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="39" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="38" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="14" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="39" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="38" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="39" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="29" fillId="8" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="40" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="38" fillId="10" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="29" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="26" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="26" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="37" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="38" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="38" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="38" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="38" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="37" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="13" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="38" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="37" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="38" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="171" fontId="28" fillId="8" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="39" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="37" fillId="10" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="28" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="25" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="25" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="39" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="38" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="37" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="3" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="3" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="29" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="26" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="26" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="25" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="25" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -4104,8 +4136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE4A73D-2F46-7341-9C57-6E5B7A39A15C}">
   <dimension ref="B1:AL86"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:H6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4123,36 +4155,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="L1" s="262" t="s">
+      <c r="L1" s="267" t="s">
         <v>125</v>
       </c>
-      <c r="M1" s="263"/>
-      <c r="N1" s="263"/>
-      <c r="O1" s="263"/>
-      <c r="P1" s="263"/>
-      <c r="Q1" s="263"/>
-      <c r="R1" s="263"/>
-      <c r="S1" s="263"/>
-      <c r="T1" s="263"/>
-      <c r="U1" s="264"/>
-      <c r="W1" s="265" t="s">
+      <c r="M1" s="268"/>
+      <c r="N1" s="268"/>
+      <c r="O1" s="268"/>
+      <c r="P1" s="268"/>
+      <c r="Q1" s="268"/>
+      <c r="R1" s="268"/>
+      <c r="S1" s="268"/>
+      <c r="T1" s="268"/>
+      <c r="U1" s="269"/>
+      <c r="W1" s="270" t="s">
         <v>127</v>
       </c>
-      <c r="X1" s="266"/>
-      <c r="Y1" s="266"/>
-      <c r="Z1" s="266"/>
-      <c r="AA1" s="266"/>
-      <c r="AB1" s="266"/>
-      <c r="AC1" s="266"/>
-      <c r="AD1" s="266"/>
-      <c r="AE1" s="266"/>
-      <c r="AF1" s="266"/>
-      <c r="AG1" s="266"/>
-      <c r="AH1" s="266"/>
-      <c r="AI1" s="266"/>
-      <c r="AJ1" s="266"/>
-      <c r="AK1" s="266"/>
-      <c r="AL1" s="267"/>
+      <c r="X1" s="271"/>
+      <c r="Y1" s="271"/>
+      <c r="Z1" s="271"/>
+      <c r="AA1" s="271"/>
+      <c r="AB1" s="271"/>
+      <c r="AC1" s="271"/>
+      <c r="AD1" s="271"/>
+      <c r="AE1" s="271"/>
+      <c r="AF1" s="271"/>
+      <c r="AG1" s="271"/>
+      <c r="AH1" s="271"/>
+      <c r="AI1" s="271"/>
+      <c r="AJ1" s="271"/>
+      <c r="AK1" s="271"/>
+      <c r="AL1" s="272"/>
     </row>
     <row r="2" spans="2:38" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
@@ -4351,16 +4383,16 @@
       </c>
     </row>
     <row r="5" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B5" s="254" t="s">
+      <c r="B5" s="273" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="255"/>
-      <c r="D5" s="256"/>
-      <c r="F5" s="254" t="s">
+      <c r="C5" s="274"/>
+      <c r="D5" s="275"/>
+      <c r="F5" s="273" t="s">
         <v>193</v>
       </c>
-      <c r="G5" s="255"/>
-      <c r="H5" s="256"/>
+      <c r="G5" s="274"/>
+      <c r="H5" s="275"/>
       <c r="K5" s="28" t="s">
         <v>73</v>
       </c>
@@ -4468,10 +4500,10 @@
       <c r="F6" s="176" t="s">
         <v>194</v>
       </c>
-      <c r="G6" s="257" t="s">
-        <v>198</v>
-      </c>
-      <c r="H6" s="253"/>
+      <c r="G6" s="287" t="s">
+        <v>284</v>
+      </c>
+      <c r="H6" s="279"/>
       <c r="K6" s="28" t="s">
         <v>74</v>
       </c>
@@ -4574,12 +4606,12 @@
         <v>Q322</v>
       </c>
       <c r="F7" s="176" t="s">
-        <v>195</v>
-      </c>
-      <c r="G7" s="258">
-        <v>2004</v>
-      </c>
-      <c r="H7" s="253"/>
+        <v>283</v>
+      </c>
+      <c r="G7" s="278">
+        <v>2021</v>
+      </c>
+      <c r="H7" s="279"/>
       <c r="K7" s="28"/>
       <c r="L7" s="60"/>
       <c r="M7" s="60"/>
@@ -4618,13 +4650,12 @@
       </c>
       <c r="D8" s="41"/>
       <c r="F8" s="176" t="s">
-        <v>62</v>
-      </c>
-      <c r="G8" s="258">
-        <f>AL4</f>
-        <v>58.8</v>
-      </c>
-      <c r="H8" s="253"/>
+        <v>195</v>
+      </c>
+      <c r="G8" s="278">
+        <v>2004</v>
+      </c>
+      <c r="H8" s="279"/>
       <c r="K8" s="28" t="s">
         <v>75</v>
       </c>
@@ -4718,9 +4749,14 @@
         <f t="shared" ref="D9:D11" si="6">$G$11</f>
         <v>Q322</v>
       </c>
-      <c r="F9" s="162"/>
-      <c r="G9" s="258"/>
-      <c r="H9" s="253"/>
+      <c r="F9" s="176" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="278">
+        <f>AL4</f>
+        <v>58.8</v>
+      </c>
+      <c r="H9" s="279"/>
       <c r="K9" s="28" t="s">
         <v>77</v>
       </c>
@@ -4828,9 +4864,9 @@
         <f t="shared" si="6"/>
         <v>Q322</v>
       </c>
-      <c r="F10" s="162"/>
-      <c r="G10" s="258"/>
-      <c r="H10" s="253"/>
+      <c r="F10" s="176"/>
+      <c r="G10" s="278"/>
+      <c r="H10" s="279"/>
       <c r="K10" s="28" t="s">
         <v>78</v>
       </c>
@@ -4936,12 +4972,12 @@
         <v>Q322</v>
       </c>
       <c r="F11" s="176" t="s">
-        <v>199</v>
-      </c>
-      <c r="G11" s="259" t="s">
+        <v>198</v>
+      </c>
+      <c r="G11" s="266" t="s">
         <v>109</v>
       </c>
-      <c r="H11" s="253"/>
+      <c r="H11" s="265"/>
       <c r="K11" s="28"/>
       <c r="L11" s="60"/>
       <c r="M11" s="60"/>
@@ -4971,10 +5007,10 @@
       <c r="F12" s="177" t="s">
         <v>196</v>
       </c>
-      <c r="G12" s="260" t="s">
+      <c r="G12" s="282" t="s">
         <v>197</v>
       </c>
-      <c r="H12" s="261"/>
+      <c r="H12" s="283"/>
       <c r="K12" s="28" t="s">
         <v>76</v>
       </c>
@@ -5246,16 +5282,16 @@
       </c>
     </row>
     <row r="15" spans="2:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="254" t="s">
+      <c r="B15" s="273" t="s">
         <v>130</v>
       </c>
-      <c r="C15" s="255"/>
-      <c r="D15" s="256"/>
-      <c r="F15" s="254" t="s">
-        <v>204</v>
-      </c>
-      <c r="G15" s="255"/>
-      <c r="H15" s="256"/>
+      <c r="C15" s="274"/>
+      <c r="D15" s="275"/>
+      <c r="F15" s="273" t="s">
+        <v>203</v>
+      </c>
+      <c r="G15" s="274"/>
+      <c r="H15" s="275"/>
       <c r="K15" s="28"/>
       <c r="L15" s="62"/>
       <c r="M15" s="62"/>
@@ -5272,18 +5308,18 @@
       <c r="B16" s="92" t="s">
         <v>132</v>
       </c>
-      <c r="C16" s="252" t="s">
+      <c r="C16" s="286" t="s">
         <v>131</v>
       </c>
-      <c r="D16" s="253"/>
+      <c r="D16" s="279"/>
       <c r="F16" s="176" t="s">
-        <v>205</v>
-      </c>
-      <c r="G16" s="270">
+        <v>204</v>
+      </c>
+      <c r="G16" s="280">
         <f>C6/'Financial Model'!M64</f>
         <v>44.601967818517387</v>
       </c>
-      <c r="H16" s="271"/>
+      <c r="H16" s="281"/>
       <c r="J16" s="31" t="s">
         <v>86</v>
       </c>
@@ -5369,18 +5405,18 @@
       <c r="B17" s="104" t="s">
         <v>164</v>
       </c>
-      <c r="C17" s="268" t="s">
+      <c r="C17" s="276" t="s">
         <v>165</v>
       </c>
-      <c r="D17" s="269"/>
+      <c r="D17" s="277"/>
       <c r="F17" s="176" t="s">
-        <v>214</v>
-      </c>
-      <c r="G17" s="270">
+        <v>213</v>
+      </c>
+      <c r="G17" s="280">
         <f>C8/'Financial Model'!W3</f>
         <v>9.8675626321852903</v>
       </c>
-      <c r="H17" s="271"/>
+      <c r="H17" s="281"/>
       <c r="K17" s="28" t="s">
         <v>84</v>
       </c>
@@ -5477,18 +5513,18 @@
       <c r="B18" s="92" t="s">
         <v>133</v>
       </c>
-      <c r="C18" s="252" t="s">
+      <c r="C18" s="286" t="s">
         <v>134</v>
       </c>
-      <c r="D18" s="253"/>
+      <c r="D18" s="279"/>
       <c r="F18" s="176" t="s">
-        <v>215</v>
-      </c>
-      <c r="G18" s="270">
+        <v>214</v>
+      </c>
+      <c r="G18" s="280">
         <f>C6/SUM('Financial Model'!J19:M19)</f>
         <v>-23.723072493855522</v>
       </c>
-      <c r="H18" s="271"/>
+      <c r="H18" s="281"/>
       <c r="K18" s="28" t="s">
         <v>85</v>
       </c>
@@ -5580,25 +5616,25 @@
     </row>
     <row r="19" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B19" s="90"/>
-      <c r="C19" s="258"/>
-      <c r="D19" s="253"/>
+      <c r="C19" s="278"/>
+      <c r="D19" s="279"/>
       <c r="F19" s="176"/>
-      <c r="G19" s="258"/>
-      <c r="H19" s="253"/>
+      <c r="G19" s="278"/>
+      <c r="H19" s="279"/>
       <c r="K19" s="28"/>
       <c r="L19" s="62"/>
       <c r="M19" s="62"/>
     </row>
     <row r="20" spans="2:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="91"/>
-      <c r="C20" s="272"/>
-      <c r="D20" s="273"/>
+      <c r="C20" s="284"/>
+      <c r="D20" s="285"/>
       <c r="F20" s="177"/>
-      <c r="G20" s="260"/>
-      <c r="H20" s="261"/>
+      <c r="G20" s="282"/>
+      <c r="H20" s="283"/>
       <c r="J20" s="31"/>
       <c r="K20" s="195" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M20" s="59"/>
       <c r="W20" s="1"/>
@@ -5617,25 +5653,25 @@
     </row>
     <row r="21" spans="2:38" x14ac:dyDescent="0.25">
       <c r="K21" s="195" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="2:38" x14ac:dyDescent="0.25">
       <c r="K22" s="195" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B23" s="254" t="s">
+      <c r="B23" s="273" t="s">
         <v>159</v>
       </c>
-      <c r="C23" s="255"/>
-      <c r="D23" s="255"/>
-      <c r="E23" s="255"/>
-      <c r="F23" s="255"/>
-      <c r="G23" s="256"/>
+      <c r="C23" s="274"/>
+      <c r="D23" s="274"/>
+      <c r="E23" s="274"/>
+      <c r="F23" s="274"/>
+      <c r="G23" s="275"/>
       <c r="K23" s="195" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="2:38" x14ac:dyDescent="0.25">
@@ -5745,12 +5781,12 @@
       <c r="F31" s="101"/>
       <c r="G31" s="102"/>
       <c r="J31" s="7"/>
-      <c r="K31" s="254" t="s">
+      <c r="K31" s="273" t="s">
         <v>181</v>
       </c>
-      <c r="L31" s="255"/>
-      <c r="M31" s="255"/>
-      <c r="N31" s="256"/>
+      <c r="L31" s="274"/>
+      <c r="M31" s="274"/>
+      <c r="N31" s="275"/>
     </row>
     <row r="32" spans="2:38" x14ac:dyDescent="0.25">
       <c r="J32" s="7"/>
@@ -5762,14 +5798,14 @@
       <c r="N32" s="96"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="254" t="s">
+      <c r="B33" s="273" t="s">
         <v>187</v>
       </c>
-      <c r="C33" s="255"/>
-      <c r="D33" s="255"/>
-      <c r="E33" s="255"/>
-      <c r="F33" s="255"/>
-      <c r="G33" s="256"/>
+      <c r="C33" s="274"/>
+      <c r="D33" s="274"/>
+      <c r="E33" s="274"/>
+      <c r="F33" s="274"/>
+      <c r="G33" s="275"/>
       <c r="J33" s="7"/>
       <c r="K33" s="168" t="s">
         <v>177</v>
@@ -5785,7 +5821,7 @@
         <v>44743</v>
       </c>
       <c r="C34" s="204" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D34" s="95"/>
       <c r="E34" s="95"/>
@@ -5804,14 +5840,14 @@
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="162"/>
       <c r="C35" s="205" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D35" s="95"/>
       <c r="E35" s="95"/>
       <c r="F35" s="95"/>
       <c r="G35" s="96"/>
       <c r="J35" s="206" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K35" s="168" t="s">
         <v>184</v>
@@ -5894,7 +5930,7 @@
       <c r="F40" s="95"/>
       <c r="G40" s="96"/>
       <c r="J40" s="206" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K40" s="168" t="s">
         <v>182</v>
@@ -5955,7 +5991,7 @@
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B45" s="209" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J45" s="7"/>
       <c r="K45" s="169" t="s">
@@ -5976,7 +6012,7 @@
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J47" s="7"/>
       <c r="K47" s="169" t="s">
@@ -5988,7 +6024,7 @@
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B48" s="237" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J48" s="7"/>
       <c r="K48" s="239" t="s">
@@ -6000,7 +6036,7 @@
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B49" s="237" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K49" s="170"/>
       <c r="L49" s="95"/>
@@ -6009,23 +6045,23 @@
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B50" s="238" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J50" s="240" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K50" s="239" t="s">
+        <v>236</v>
+      </c>
+      <c r="L50" s="166" t="s">
         <v>237</v>
-      </c>
-      <c r="L50" s="166" t="s">
-        <v>238</v>
       </c>
       <c r="M50" s="95"/>
       <c r="N50" s="96"/>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B51" s="238" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K51" s="171"/>
       <c r="L51" s="100"/>
@@ -6034,12 +6070,12 @@
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B52" s="238" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B53" s="238" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.25">
@@ -6049,7 +6085,7 @@
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B55" s="237" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K55" s="21" t="s">
         <v>59</v>
@@ -6062,7 +6098,7 @@
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B57" s="237" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K57" s="21" t="s">
         <v>61</v>
@@ -6070,7 +6106,7 @@
     </row>
     <row r="58" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="237" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K58" s="22" t="s">
         <v>63</v>
@@ -6078,7 +6114,7 @@
     </row>
     <row r="59" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="238" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K59" s="22" t="s">
         <v>88</v>
@@ -6086,7 +6122,7 @@
     </row>
     <row r="60" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="238" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K60" s="22" t="s">
         <v>64</v>
@@ -6094,7 +6130,7 @@
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B61" s="238" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K61" s="89" t="s">
         <v>126</v>
@@ -6102,12 +6138,12 @@
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B62" s="238" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B64" s="237" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K64" s="105" t="s">
         <v>168</v>
@@ -6115,7 +6151,7 @@
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B65" s="237" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>135</v>
@@ -6128,7 +6164,7 @@
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B67" s="237" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K67" s="93" t="s">
         <v>144</v>
@@ -6141,7 +6177,7 @@
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69" s="237" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K69" s="93" t="s">
         <v>146</v>
@@ -6154,7 +6190,7 @@
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B71" s="237" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K71" s="93" t="s">
         <v>147</v>
@@ -6162,61 +6198,70 @@
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B72" s="238" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B74" s="237" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B76" s="237" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B77" s="238" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B79" s="237" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B80" s="238" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="237" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="238" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="238" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="238" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="249" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="25">
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="L1:U1"/>
     <mergeCell ref="W1:AL1"/>
     <mergeCell ref="B33:G33"/>
@@ -6233,18 +6278,8 @@
     <mergeCell ref="B23:G23"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C16:D16"/>
   </mergeCells>
-  <phoneticPr fontId="27" type="noConversion"/>
+  <phoneticPr fontId="28" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K58" r:id="rId1" xr:uid="{F79BC045-05D5-43FB-A051-BA2031CC85A7}"/>
     <hyperlink ref="K60" r:id="rId2" xr:uid="{58004FA9-9F7A-4B71-811E-FF4EE09F281F}"/>
@@ -6258,13 +6293,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0FDCAC-3416-844A-BCBB-390EC350CF59}">
-  <dimension ref="B1:BZ116"/>
+  <dimension ref="B1:BZ120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C49" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M83" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="AP22" sqref="AP22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8548,7 +8583,7 @@
         <f t="shared" si="49"/>
         <v>-252.40528603293131</v>
       </c>
-      <c r="AB18" s="3">
+      <c r="AB18" s="264">
         <f t="shared" si="49"/>
         <v>80.434307742151219</v>
       </c>
@@ -9174,7 +9209,7 @@
         <v>114</v>
       </c>
       <c r="AP22" s="135">
-        <v>0.06</v>
+        <v>0.09</v>
       </c>
       <c r="AR22" s="67"/>
     </row>
@@ -9320,7 +9355,7 @@
       </c>
       <c r="AP23" s="136">
         <f>NPV(AP22,X18:BZ18)</f>
-        <v>71290.030046149914</v>
+        <v>37523.031429501891</v>
       </c>
       <c r="AR23" s="68"/>
     </row>
@@ -9611,7 +9646,7 @@
       </c>
       <c r="AP25" s="136">
         <f>AP23+AP24</f>
-        <v>73322.874046149911</v>
+        <v>39555.875429501888</v>
       </c>
     </row>
     <row r="26" spans="2:78" x14ac:dyDescent="0.25">
@@ -9628,7 +9663,7 @@
       </c>
       <c r="AP26" s="137">
         <f>AP25/Main!C7</f>
-        <v>122.65883218739687</v>
+        <v>66.171403527895578</v>
       </c>
       <c r="AQ26" s="67"/>
       <c r="AS26" s="9"/>
@@ -9847,7 +9882,7 @@
       </c>
       <c r="AP28" s="139">
         <f>AP26/AP27-1</f>
-        <v>2.871806571571871</v>
+        <v>1.0887437982290269</v>
       </c>
     </row>
     <row r="29" spans="2:78" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -9888,7 +9923,7 @@
     </row>
     <row r="30" spans="2:78" s="212" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" s="212" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>33</v>
@@ -9965,7 +10000,7 @@
     </row>
     <row r="31" spans="2:78" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>33</v>
@@ -11225,7 +11260,7 @@
     </row>
     <row r="63" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B63" s="195" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F63" s="5">
         <f t="shared" ref="F63:K63" si="103">F48-F58</f>
@@ -11262,7 +11297,7 @@
     </row>
     <row r="64" spans="2:19" s="207" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B64" s="207" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>33</v>
@@ -11565,7 +11600,7 @@
     </row>
     <row r="74" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B74" s="209" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G74" s="217">
         <f t="shared" ref="G74:I74" si="118">G70/G64</f>
@@ -11598,7 +11633,7 @@
     </row>
     <row r="75" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B75" s="209" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G75" s="217">
         <f t="shared" ref="G75" si="121">G71/SUM(D3:G3)</f>
@@ -11631,7 +11666,7 @@
     </row>
     <row r="76" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B76" s="233" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G76" s="217">
         <f t="shared" ref="G76" si="126">G72/SUM(D3:G3)</f>
@@ -11664,7 +11699,7 @@
     </row>
     <row r="77" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B77" s="209" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G77" s="217">
         <f t="shared" ref="G77:L77" si="131">G70/SUM(D19:G19)</f>
@@ -11698,7 +11733,7 @@
     </row>
     <row r="78" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B78" s="251" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G78" s="87">
         <f t="shared" ref="G78:L78" si="132">SUM(D12:G12)/(G48-SUM(G50:G53))</f>
@@ -11753,12 +11788,12 @@
       <c r="P80" s="251"/>
     </row>
     <row r="81" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="275" t="s">
-        <v>273</v>
-      </c>
-      <c r="C81" s="276"/>
-      <c r="D81" s="276"/>
-      <c r="E81" s="276"/>
+      <c r="B81" s="253" t="s">
+        <v>272</v>
+      </c>
+      <c r="C81" s="254"/>
+      <c r="D81" s="254"/>
+      <c r="E81" s="254"/>
       <c r="F81" s="5"/>
       <c r="G81" s="5"/>
       <c r="H81" s="5">
@@ -11786,18 +11821,18 @@
         <v>-301.90200000000004</v>
       </c>
       <c r="N81" s="118"/>
-      <c r="P81" s="277"/>
+      <c r="P81" s="255"/>
       <c r="Q81" s="5"/>
       <c r="R81" s="5"/>
       <c r="S81" s="5"/>
     </row>
     <row r="82" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="275" t="s">
-        <v>274</v>
-      </c>
-      <c r="C82" s="276"/>
-      <c r="D82" s="276"/>
-      <c r="E82" s="276"/>
+      <c r="B82" s="253" t="s">
+        <v>273</v>
+      </c>
+      <c r="C82" s="254"/>
+      <c r="D82" s="254"/>
+      <c r="E82" s="254"/>
       <c r="F82" s="5"/>
       <c r="G82" s="5"/>
       <c r="H82" s="5">
@@ -11815,16 +11850,16 @@
         <v>-301.90199999999999</v>
       </c>
       <c r="N82" s="118"/>
-      <c r="P82" s="277"/>
+      <c r="P82" s="255"/>
       <c r="Q82" s="5"/>
       <c r="R82" s="5"/>
       <c r="S82" s="5"/>
     </row>
     <row r="83" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="278"/>
-      <c r="C83" s="276"/>
-      <c r="D83" s="276"/>
-      <c r="E83" s="276"/>
+      <c r="B83" s="256"/>
+      <c r="C83" s="254"/>
+      <c r="D83" s="254"/>
+      <c r="E83" s="254"/>
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
@@ -11839,12 +11874,12 @@
       <c r="S83" s="5"/>
     </row>
     <row r="84" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="279" t="s">
-        <v>253</v>
-      </c>
-      <c r="C84" s="276"/>
-      <c r="D84" s="276"/>
-      <c r="E84" s="276"/>
+      <c r="B84" s="257" t="s">
+        <v>252</v>
+      </c>
+      <c r="C84" s="254"/>
+      <c r="D84" s="254"/>
+      <c r="E84" s="254"/>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>
@@ -11859,12 +11894,12 @@
       <c r="S84" s="5"/>
     </row>
     <row r="85" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="280" t="s">
-        <v>255</v>
-      </c>
-      <c r="C85" s="276"/>
-      <c r="D85" s="276"/>
-      <c r="E85" s="276"/>
+      <c r="B85" s="258" t="s">
+        <v>254</v>
+      </c>
+      <c r="C85" s="254"/>
+      <c r="D85" s="254"/>
+      <c r="E85" s="254"/>
       <c r="F85" s="5"/>
       <c r="G85" s="5"/>
       <c r="H85" s="5">
@@ -11887,12 +11922,12 @@
       <c r="S85" s="5"/>
     </row>
     <row r="86" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="280" t="s">
-        <v>256</v>
-      </c>
-      <c r="C86" s="276"/>
-      <c r="D86" s="276"/>
-      <c r="E86" s="276"/>
+      <c r="B86" s="258" t="s">
+        <v>255</v>
+      </c>
+      <c r="C86" s="254"/>
+      <c r="D86" s="254"/>
+      <c r="E86" s="254"/>
       <c r="F86" s="5"/>
       <c r="G86" s="5"/>
       <c r="H86" s="5">
@@ -11915,12 +11950,12 @@
       <c r="S86" s="5"/>
     </row>
     <row r="87" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="280" t="s">
-        <v>258</v>
-      </c>
-      <c r="C87" s="276"/>
-      <c r="D87" s="276"/>
-      <c r="E87" s="276"/>
+      <c r="B87" s="258" t="s">
+        <v>257</v>
+      </c>
+      <c r="C87" s="254"/>
+      <c r="D87" s="254"/>
+      <c r="E87" s="254"/>
       <c r="F87" s="5"/>
       <c r="G87" s="5"/>
       <c r="H87" s="5">
@@ -11943,12 +11978,12 @@
       <c r="S87" s="5"/>
     </row>
     <row r="88" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="280" t="s">
-        <v>257</v>
-      </c>
-      <c r="C88" s="276"/>
-      <c r="D88" s="276"/>
-      <c r="E88" s="276"/>
+      <c r="B88" s="258" t="s">
+        <v>256</v>
+      </c>
+      <c r="C88" s="254"/>
+      <c r="D88" s="254"/>
+      <c r="E88" s="254"/>
       <c r="F88" s="5"/>
       <c r="G88" s="5"/>
       <c r="H88" s="5">
@@ -11971,12 +12006,12 @@
       <c r="S88" s="5"/>
     </row>
     <row r="89" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="280" t="s">
-        <v>259</v>
-      </c>
-      <c r="C89" s="276"/>
-      <c r="D89" s="276"/>
-      <c r="E89" s="276"/>
+      <c r="B89" s="258" t="s">
+        <v>258</v>
+      </c>
+      <c r="C89" s="254"/>
+      <c r="D89" s="254"/>
+      <c r="E89" s="254"/>
       <c r="F89" s="5"/>
       <c r="G89" s="5"/>
       <c r="H89" s="5">
@@ -11999,12 +12034,12 @@
       <c r="S89" s="5"/>
     </row>
     <row r="90" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="280" t="s">
-        <v>260</v>
-      </c>
-      <c r="C90" s="276"/>
-      <c r="D90" s="276"/>
-      <c r="E90" s="276"/>
+      <c r="B90" s="258" t="s">
+        <v>259</v>
+      </c>
+      <c r="C90" s="254"/>
+      <c r="D90" s="254"/>
+      <c r="E90" s="254"/>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="9">
@@ -12031,12 +12066,12 @@
       <c r="S90" s="5"/>
     </row>
     <row r="91" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="275" t="s">
+      <c r="B91" s="253" t="s">
         <v>37</v>
       </c>
-      <c r="C91" s="276"/>
-      <c r="D91" s="276"/>
-      <c r="E91" s="276"/>
+      <c r="C91" s="254"/>
+      <c r="D91" s="254"/>
+      <c r="E91" s="254"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5">
@@ -12059,12 +12094,12 @@
       <c r="S91" s="5"/>
     </row>
     <row r="92" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="275" t="s">
+      <c r="B92" s="253" t="s">
         <v>46</v>
       </c>
-      <c r="C92" s="276"/>
-      <c r="D92" s="276"/>
-      <c r="E92" s="276"/>
+      <c r="C92" s="254"/>
+      <c r="D92" s="254"/>
+      <c r="E92" s="254"/>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
       <c r="H92" s="5">
@@ -12087,12 +12122,12 @@
       <c r="S92" s="5"/>
     </row>
     <row r="93" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="275" t="s">
-        <v>275</v>
-      </c>
-      <c r="C93" s="276"/>
-      <c r="D93" s="276"/>
-      <c r="E93" s="276"/>
+      <c r="B93" s="253" t="s">
+        <v>274</v>
+      </c>
+      <c r="C93" s="254"/>
+      <c r="D93" s="254"/>
+      <c r="E93" s="254"/>
       <c r="F93" s="5"/>
       <c r="G93" s="5"/>
       <c r="H93" s="5">
@@ -12115,12 +12150,12 @@
       <c r="S93" s="5"/>
     </row>
     <row r="94" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="275" t="s">
-        <v>276</v>
-      </c>
-      <c r="C94" s="276"/>
-      <c r="D94" s="276"/>
-      <c r="E94" s="276"/>
+      <c r="B94" s="253" t="s">
+        <v>275</v>
+      </c>
+      <c r="C94" s="254"/>
+      <c r="D94" s="254"/>
+      <c r="E94" s="254"/>
       <c r="F94" s="5"/>
       <c r="G94" s="5"/>
       <c r="H94" s="5">
@@ -12143,12 +12178,12 @@
       <c r="S94" s="5"/>
     </row>
     <row r="95" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="275" t="s">
+      <c r="B95" s="253" t="s">
         <v>48</v>
       </c>
-      <c r="C95" s="276"/>
-      <c r="D95" s="276"/>
-      <c r="E95" s="276"/>
+      <c r="C95" s="254"/>
+      <c r="D95" s="254"/>
+      <c r="E95" s="254"/>
       <c r="F95" s="5"/>
       <c r="G95" s="5"/>
       <c r="H95" s="5">
@@ -12171,12 +12206,12 @@
       <c r="S95" s="5"/>
     </row>
     <row r="96" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="275" t="s">
-        <v>277</v>
-      </c>
-      <c r="C96" s="276"/>
-      <c r="D96" s="276"/>
-      <c r="E96" s="276"/>
+      <c r="B96" s="253" t="s">
+        <v>276</v>
+      </c>
+      <c r="C96" s="254"/>
+      <c r="D96" s="254"/>
+      <c r="E96" s="254"/>
       <c r="F96" s="5"/>
       <c r="G96" s="5"/>
       <c r="H96" s="5">
@@ -12199,12 +12234,12 @@
       <c r="S96" s="5"/>
     </row>
     <row r="97" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="275" t="s">
-        <v>278</v>
-      </c>
-      <c r="C97" s="276"/>
-      <c r="D97" s="276"/>
-      <c r="E97" s="276"/>
+      <c r="B97" s="253" t="s">
+        <v>277</v>
+      </c>
+      <c r="C97" s="254"/>
+      <c r="D97" s="254"/>
+      <c r="E97" s="254"/>
       <c r="F97" s="5"/>
       <c r="G97" s="5"/>
       <c r="H97" s="5">
@@ -12227,12 +12262,12 @@
       <c r="S97" s="5"/>
     </row>
     <row r="98" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="275" t="s">
-        <v>279</v>
-      </c>
-      <c r="C98" s="276"/>
-      <c r="D98" s="276"/>
-      <c r="E98" s="276"/>
+      <c r="B98" s="253" t="s">
+        <v>278</v>
+      </c>
+      <c r="C98" s="254"/>
+      <c r="D98" s="254"/>
+      <c r="E98" s="254"/>
       <c r="F98" s="5"/>
       <c r="G98" s="5"/>
       <c r="H98" s="5">
@@ -12255,12 +12290,12 @@
       <c r="S98" s="5"/>
     </row>
     <row r="99" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="275" t="s">
-        <v>280</v>
-      </c>
-      <c r="C99" s="276"/>
-      <c r="D99" s="276"/>
-      <c r="E99" s="276"/>
+      <c r="B99" s="253" t="s">
+        <v>279</v>
+      </c>
+      <c r="C99" s="254"/>
+      <c r="D99" s="254"/>
+      <c r="E99" s="254"/>
       <c r="F99" s="5"/>
       <c r="G99" s="5"/>
       <c r="H99" s="5">
@@ -12283,12 +12318,12 @@
       <c r="S99" s="5"/>
     </row>
     <row r="100" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="275" t="s">
-        <v>281</v>
-      </c>
-      <c r="C100" s="276"/>
-      <c r="D100" s="276"/>
-      <c r="E100" s="276"/>
+      <c r="B100" s="253" t="s">
+        <v>280</v>
+      </c>
+      <c r="C100" s="254"/>
+      <c r="D100" s="254"/>
+      <c r="E100" s="254"/>
       <c r="F100" s="5"/>
       <c r="G100" s="5"/>
       <c r="H100" s="5">
@@ -12312,11 +12347,11 @@
     </row>
     <row r="101" spans="2:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B101" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="C101" s="281"/>
-      <c r="D101" s="281"/>
-      <c r="E101" s="281"/>
+        <v>260</v>
+      </c>
+      <c r="C101" s="259"/>
+      <c r="D101" s="259"/>
+      <c r="E101" s="259"/>
       <c r="F101" s="4"/>
       <c r="G101" s="4"/>
       <c r="H101" s="4">
@@ -12343,10 +12378,10 @@
       <c r="S101" s="4"/>
     </row>
     <row r="102" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="278"/>
-      <c r="C102" s="276"/>
-      <c r="D102" s="276"/>
-      <c r="E102" s="276"/>
+      <c r="B102" s="256"/>
+      <c r="C102" s="254"/>
+      <c r="D102" s="254"/>
+      <c r="E102" s="254"/>
       <c r="F102" s="5"/>
       <c r="G102" s="5"/>
       <c r="H102" s="5"/>
@@ -12361,12 +12396,12 @@
       <c r="S102" s="5"/>
     </row>
     <row r="103" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="280" t="s">
-        <v>262</v>
-      </c>
-      <c r="C103" s="276"/>
-      <c r="D103" s="276"/>
-      <c r="E103" s="276"/>
+      <c r="B103" s="258" t="s">
+        <v>261</v>
+      </c>
+      <c r="C103" s="254"/>
+      <c r="D103" s="254"/>
+      <c r="E103" s="254"/>
       <c r="F103" s="5"/>
       <c r="G103" s="5"/>
       <c r="H103" s="5">
@@ -12389,12 +12424,12 @@
       <c r="S103" s="5"/>
     </row>
     <row r="104" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="280" t="s">
-        <v>263</v>
-      </c>
-      <c r="C104" s="276"/>
-      <c r="D104" s="276"/>
-      <c r="E104" s="276"/>
+      <c r="B104" s="258" t="s">
+        <v>262</v>
+      </c>
+      <c r="C104" s="254"/>
+      <c r="D104" s="254"/>
+      <c r="E104" s="254"/>
       <c r="F104" s="5"/>
       <c r="G104" s="5"/>
       <c r="H104" s="5">
@@ -12417,12 +12452,12 @@
       <c r="S104" s="5"/>
     </row>
     <row r="105" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="280" t="s">
-        <v>264</v>
-      </c>
-      <c r="C105" s="276"/>
-      <c r="D105" s="276"/>
-      <c r="E105" s="276"/>
+      <c r="B105" s="258" t="s">
+        <v>263</v>
+      </c>
+      <c r="C105" s="254"/>
+      <c r="D105" s="254"/>
+      <c r="E105" s="254"/>
       <c r="F105" s="5"/>
       <c r="G105" s="5"/>
       <c r="H105" s="5">
@@ -12446,11 +12481,11 @@
     </row>
     <row r="106" spans="2:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="C106" s="281"/>
-      <c r="D106" s="281"/>
-      <c r="E106" s="281"/>
+        <v>264</v>
+      </c>
+      <c r="C106" s="259"/>
+      <c r="D106" s="259"/>
+      <c r="E106" s="259"/>
       <c r="F106" s="4"/>
       <c r="G106" s="4"/>
       <c r="H106" s="4">
@@ -12477,10 +12512,10 @@
       <c r="S106" s="4"/>
     </row>
     <row r="107" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="278"/>
-      <c r="C107" s="276"/>
-      <c r="D107" s="276"/>
-      <c r="E107" s="276"/>
+      <c r="B107" s="256"/>
+      <c r="C107" s="254"/>
+      <c r="D107" s="254"/>
+      <c r="E107" s="254"/>
       <c r="F107" s="5"/>
       <c r="G107" s="5"/>
       <c r="H107" s="5"/>
@@ -12495,12 +12530,12 @@
       <c r="S107" s="5"/>
     </row>
     <row r="108" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="280" t="s">
-        <v>266</v>
-      </c>
-      <c r="C108" s="276"/>
-      <c r="D108" s="276"/>
-      <c r="E108" s="276"/>
+      <c r="B108" s="258" t="s">
+        <v>265</v>
+      </c>
+      <c r="C108" s="254"/>
+      <c r="D108" s="254"/>
+      <c r="E108" s="254"/>
       <c r="F108" s="5"/>
       <c r="G108" s="5"/>
       <c r="H108" s="5">
@@ -12523,12 +12558,12 @@
       <c r="S108" s="5"/>
     </row>
     <row r="109" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="280" t="s">
-        <v>267</v>
-      </c>
-      <c r="C109" s="276"/>
-      <c r="D109" s="276"/>
-      <c r="E109" s="276"/>
+      <c r="B109" s="258" t="s">
+        <v>266</v>
+      </c>
+      <c r="C109" s="254"/>
+      <c r="D109" s="254"/>
+      <c r="E109" s="254"/>
       <c r="F109" s="5"/>
       <c r="G109" s="5"/>
       <c r="H109" s="5">
@@ -12551,12 +12586,12 @@
       <c r="S109" s="5"/>
     </row>
     <row r="110" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="280" t="s">
-        <v>268</v>
-      </c>
-      <c r="C110" s="276"/>
-      <c r="D110" s="276"/>
-      <c r="E110" s="276"/>
+      <c r="B110" s="258" t="s">
+        <v>267</v>
+      </c>
+      <c r="C110" s="254"/>
+      <c r="D110" s="254"/>
+      <c r="E110" s="254"/>
       <c r="F110" s="5"/>
       <c r="G110" s="5"/>
       <c r="H110" s="5">
@@ -12579,12 +12614,12 @@
       <c r="S110" s="5"/>
     </row>
     <row r="111" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="280" t="s">
-        <v>269</v>
-      </c>
-      <c r="C111" s="276"/>
-      <c r="D111" s="276"/>
-      <c r="E111" s="276"/>
+      <c r="B111" s="258" t="s">
+        <v>268</v>
+      </c>
+      <c r="C111" s="254"/>
+      <c r="D111" s="254"/>
+      <c r="E111" s="254"/>
       <c r="F111" s="5"/>
       <c r="G111" s="5"/>
       <c r="H111" s="5">
@@ -12607,12 +12642,12 @@
       <c r="S111" s="5"/>
     </row>
     <row r="112" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="280" t="s">
-        <v>270</v>
-      </c>
-      <c r="C112" s="276"/>
-      <c r="D112" s="276"/>
-      <c r="E112" s="276"/>
+      <c r="B112" s="258" t="s">
+        <v>269</v>
+      </c>
+      <c r="C112" s="254"/>
+      <c r="D112" s="254"/>
+      <c r="E112" s="254"/>
       <c r="F112" s="5"/>
       <c r="G112" s="5"/>
       <c r="H112" s="5">
@@ -12635,12 +12670,12 @@
       <c r="S112" s="5"/>
     </row>
     <row r="113" spans="2:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="280" t="s">
-        <v>271</v>
-      </c>
-      <c r="C113" s="276"/>
-      <c r="D113" s="276"/>
-      <c r="E113" s="276"/>
+      <c r="B113" s="258" t="s">
+        <v>270</v>
+      </c>
+      <c r="C113" s="254"/>
+      <c r="D113" s="254"/>
+      <c r="E113" s="254"/>
       <c r="F113" s="5"/>
       <c r="G113" s="5"/>
       <c r="H113" s="5">
@@ -12664,11 +12699,11 @@
     </row>
     <row r="114" spans="2:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B114" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="C114" s="281"/>
-      <c r="D114" s="281"/>
-      <c r="E114" s="281"/>
+        <v>271</v>
+      </c>
+      <c r="C114" s="259"/>
+      <c r="D114" s="259"/>
+      <c r="E114" s="259"/>
       <c r="F114" s="4"/>
       <c r="G114" s="4"/>
       <c r="H114" s="4">
@@ -12694,12 +12729,67 @@
       <c r="R114" s="4"/>
       <c r="S114" s="4"/>
     </row>
-    <row r="116" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B116" s="274"/>
-      <c r="M116" s="282"/>
+    <row r="116" spans="2:19" s="252" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="252" t="s">
+        <v>281</v>
+      </c>
+      <c r="C116" s="260"/>
+      <c r="D116" s="260"/>
+      <c r="E116" s="260"/>
+      <c r="F116" s="261"/>
+      <c r="G116" s="261"/>
+      <c r="H116" s="262">
+        <f>H103</f>
+        <v>-23.234999999999999</v>
+      </c>
+      <c r="I116" s="262">
+        <f>I103</f>
+        <v>-2.9620000000000002</v>
+      </c>
+      <c r="J116" s="261"/>
+      <c r="K116" s="261"/>
+      <c r="L116" s="262">
+        <f>L103</f>
+        <v>-83.811999999999998</v>
+      </c>
+      <c r="M116" s="262">
+        <f>M103</f>
+        <v>-133.35599999999999</v>
+      </c>
+      <c r="N116" s="263"/>
+      <c r="Q116" s="261"/>
+      <c r="R116" s="261"/>
+      <c r="S116" s="261"/>
+    </row>
+    <row r="117" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B117" s="252" t="s">
+        <v>282</v>
+      </c>
+      <c r="H117" s="5">
+        <f>+H101+H106</f>
+        <v>168.01600000000002</v>
+      </c>
+      <c r="I117" s="5">
+        <f>+I101+I106</f>
+        <v>124.91199999999999</v>
+      </c>
+      <c r="L117" s="5">
+        <f>+L101+L106</f>
+        <v>-63.47999999999999</v>
+      </c>
+      <c r="M117" s="5">
+        <f>+M101+M106</f>
+        <v>-67.70599999999996</v>
+      </c>
+    </row>
+    <row r="119" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B119" s="252"/>
+    </row>
+    <row r="120" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B120" s="252"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="27" type="noConversion"/>
+  <phoneticPr fontId="28" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="L1" r:id="rId1" xr:uid="{F0F1B078-C7E3-AA47-9924-08C1D4511F24}"/>
     <hyperlink ref="M1" r:id="rId2" xr:uid="{9D82E829-DF9B-4456-A9EF-305989A97DF8}"/>
@@ -12720,10 +12810,10 @@
   <dimension ref="A1:AE24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z31" sqref="Z31"/>
+      <selection pane="bottomRight" activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14093,7 +14183,7 @@
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="31"/>
       <c r="B20" s="195" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C20" s="25" t="s">
         <v>33</v>
@@ -14166,7 +14256,7 @@
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="31"/>
       <c r="B21" s="195" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C21" s="25" t="s">
         <v>33</v>
@@ -14245,7 +14335,7 @@
       <c r="R24" s="109"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="27" type="noConversion"/>
+  <phoneticPr fontId="28" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
$RBLX SVB collapse key event
</commit_message>
<xml_diff>
--- a/$RBLX.xlsx
+++ b/$RBLX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1E7C42-B562-447A-9E10-5C84D267BBFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF74270-29D4-4CA7-B9EB-DD662E78CC8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{DB6ABC51-E0DE-6747-8CA5-53C172A4844D}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" xr2:uid="{DB6ABC51-E0DE-6747-8CA5-53C172A4844D}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="323">
   <si>
     <t>Price</t>
   </si>
@@ -990,6 +990,12 @@
   </si>
   <si>
     <t>P/Bookings</t>
+  </si>
+  <si>
+    <t>$150m (5%) of $3bn cash at hand/bank was in failed bank</t>
+  </si>
+  <si>
+    <t>SVB which is being liquidated by regulators</t>
   </si>
 </sst>
 </file>
@@ -1008,9 +1014,16 @@
     <numFmt numFmtId="171" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="172" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="53" x14ac:knownFonts="1">
+  <fonts count="54" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1610,731 +1623,735 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="329">
+  <cellXfs count="331">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="25" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="25" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="17" fontId="42" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="42" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="30" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="30" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="33" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="30" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="33" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="30" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="30" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="30" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="30" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="30" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="33" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="42" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="10" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="33" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="30" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="30" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="33" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="33" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="30" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="30" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="30" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="30" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="30" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="33" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="25" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="42" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="43" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="43" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="47" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="2" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="48" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="32" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="17" fontId="41" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="41" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="29" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="29" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="29" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="32" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="29" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="29" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="29" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="29" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="29" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="32" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="20" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="17" fontId="41" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="32" fillId="10" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="29" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="29" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="32" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="29" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="29" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="29" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="29" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="29" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="32" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="24" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="41" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="42" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="42" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="42" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="37" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="42" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="42" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="46" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="47" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="33" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="32" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="30" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="33" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="32" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="30" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="29" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="30" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="29" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="30" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="29" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="30" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="29" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="30" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="29" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="33" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="32" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="33" fillId="12" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="32" fillId="12" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="30" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="29" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="43" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="42" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="43" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="42" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="33" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="17" fontId="32" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="42" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="43" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="33" fillId="8" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="30" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="44" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="42" fillId="10" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="172" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="41" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="42" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="171" fontId="32" fillId="8" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="29" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="43" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="41" fillId="10" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="43" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="42" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="41" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="3" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="33" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="33" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="30" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="30" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="30" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="3" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="29" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="171" fontId="32" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="29" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="29" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="29" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="41" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="42" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="42" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="169" fontId="42" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="41" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="43" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="42" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="43" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="42" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="42" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="41" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="43" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="43" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="42" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="32" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="32" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="33" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="29" fillId="14" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="30" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="29" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="33" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="29" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="30" fillId="14" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="29" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="30" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="30" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="29" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="30" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="32" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="30" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="33" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="43" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="42" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="41" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="33" fillId="14" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="32" fillId="14" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="30" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="29" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="53" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="43" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="30" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="30" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="30" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="30" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="42" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="29" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="29" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="29" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="29" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="30" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="30" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="30" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="29" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="30" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="29" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="6" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="6" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="30" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="30" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="6" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="6" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="29" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="172" fontId="29" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="29" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="29" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -4345,8 +4362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE4A73D-2F46-7341-9C57-6E5B7A39A15C}">
   <dimension ref="B1:AL86"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4364,36 +4381,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="L1" s="313" t="s">
+      <c r="L1" s="304" t="s">
         <v>125</v>
       </c>
-      <c r="M1" s="314"/>
-      <c r="N1" s="314"/>
-      <c r="O1" s="314"/>
-      <c r="P1" s="314"/>
-      <c r="Q1" s="314"/>
-      <c r="R1" s="314"/>
-      <c r="S1" s="314"/>
-      <c r="T1" s="314"/>
-      <c r="U1" s="315"/>
-      <c r="W1" s="316" t="s">
+      <c r="M1" s="305"/>
+      <c r="N1" s="305"/>
+      <c r="O1" s="305"/>
+      <c r="P1" s="305"/>
+      <c r="Q1" s="305"/>
+      <c r="R1" s="305"/>
+      <c r="S1" s="305"/>
+      <c r="T1" s="305"/>
+      <c r="U1" s="306"/>
+      <c r="W1" s="307" t="s">
         <v>127</v>
       </c>
-      <c r="X1" s="317"/>
-      <c r="Y1" s="317"/>
-      <c r="Z1" s="317"/>
-      <c r="AA1" s="317"/>
-      <c r="AB1" s="317"/>
-      <c r="AC1" s="317"/>
-      <c r="AD1" s="317"/>
-      <c r="AE1" s="317"/>
-      <c r="AF1" s="317"/>
-      <c r="AG1" s="317"/>
-      <c r="AH1" s="317"/>
-      <c r="AI1" s="317"/>
-      <c r="AJ1" s="317"/>
-      <c r="AK1" s="317"/>
-      <c r="AL1" s="318"/>
+      <c r="X1" s="308"/>
+      <c r="Y1" s="308"/>
+      <c r="Z1" s="308"/>
+      <c r="AA1" s="308"/>
+      <c r="AB1" s="308"/>
+      <c r="AC1" s="308"/>
+      <c r="AD1" s="308"/>
+      <c r="AE1" s="308"/>
+      <c r="AF1" s="308"/>
+      <c r="AG1" s="308"/>
+      <c r="AH1" s="308"/>
+      <c r="AI1" s="308"/>
+      <c r="AJ1" s="308"/>
+      <c r="AK1" s="308"/>
+      <c r="AL1" s="309"/>
     </row>
     <row r="2" spans="2:38" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="17" t="s">
@@ -4592,16 +4609,16 @@
       </c>
     </row>
     <row r="5" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B5" s="304" t="s">
+      <c r="B5" s="310" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="305"/>
-      <c r="D5" s="306"/>
-      <c r="F5" s="304" t="s">
+      <c r="C5" s="311"/>
+      <c r="D5" s="312"/>
+      <c r="F5" s="310" t="s">
         <v>193</v>
       </c>
-      <c r="G5" s="305"/>
-      <c r="H5" s="306"/>
+      <c r="G5" s="311"/>
+      <c r="H5" s="312"/>
       <c r="K5" s="27" t="s">
         <v>73</v>
       </c>
@@ -4709,10 +4726,10 @@
       <c r="F6" s="154" t="s">
         <v>194</v>
       </c>
-      <c r="G6" s="307" t="s">
+      <c r="G6" s="324" t="s">
         <v>284</v>
       </c>
-      <c r="H6" s="303"/>
+      <c r="H6" s="316"/>
       <c r="K6" s="27" t="s">
         <v>74</v>
       </c>
@@ -4816,10 +4833,10 @@
       <c r="F7" s="154" t="s">
         <v>283</v>
       </c>
-      <c r="G7" s="308">
+      <c r="G7" s="315">
         <v>2021</v>
       </c>
-      <c r="H7" s="303"/>
+      <c r="H7" s="316"/>
       <c r="K7" s="27"/>
       <c r="L7" s="55"/>
       <c r="M7" s="55"/>
@@ -4860,10 +4877,10 @@
       <c r="F8" s="154" t="s">
         <v>195</v>
       </c>
-      <c r="G8" s="308">
+      <c r="G8" s="315">
         <v>2004</v>
       </c>
-      <c r="H8" s="303"/>
+      <c r="H8" s="316"/>
       <c r="K8" s="27" t="s">
         <v>75</v>
       </c>
@@ -4959,11 +4976,11 @@
       <c r="F9" s="154" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="308">
+      <c r="G9" s="315">
         <f>AL4</f>
         <v>58.8</v>
       </c>
-      <c r="H9" s="303"/>
+      <c r="H9" s="316"/>
       <c r="K9" s="27" t="s">
         <v>77</v>
       </c>
@@ -5073,10 +5090,10 @@
       <c r="F10" s="154" t="s">
         <v>318</v>
       </c>
-      <c r="G10" s="309">
+      <c r="G10" s="325">
         <v>2128</v>
       </c>
-      <c r="H10" s="310"/>
+      <c r="H10" s="326"/>
       <c r="K10" s="27" t="s">
         <v>78</v>
       </c>
@@ -5218,10 +5235,10 @@
       <c r="F12" s="155" t="s">
         <v>196</v>
       </c>
-      <c r="G12" s="311" t="s">
+      <c r="G12" s="327" t="s">
         <v>197</v>
       </c>
-      <c r="H12" s="312"/>
+      <c r="H12" s="328"/>
       <c r="K12" s="27" t="s">
         <v>76</v>
       </c>
@@ -5493,16 +5510,16 @@
       </c>
     </row>
     <row r="15" spans="2:38" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="304" t="s">
+      <c r="B15" s="310" t="s">
         <v>130</v>
       </c>
-      <c r="C15" s="305"/>
-      <c r="D15" s="306"/>
-      <c r="F15" s="304" t="s">
+      <c r="C15" s="311"/>
+      <c r="D15" s="312"/>
+      <c r="F15" s="310" t="s">
         <v>203</v>
       </c>
-      <c r="G15" s="305"/>
-      <c r="H15" s="306"/>
+      <c r="G15" s="311"/>
+      <c r="H15" s="312"/>
       <c r="K15" s="27"/>
       <c r="L15" s="57"/>
       <c r="M15" s="57"/>
@@ -5519,18 +5536,18 @@
       <c r="B16" s="85" t="s">
         <v>132</v>
       </c>
-      <c r="C16" s="302" t="s">
+      <c r="C16" s="323" t="s">
         <v>131</v>
       </c>
-      <c r="D16" s="303"/>
+      <c r="D16" s="316"/>
       <c r="F16" s="154" t="s">
         <v>204</v>
       </c>
-      <c r="G16" s="325">
+      <c r="G16" s="317">
         <f>C6/'Financial Model'!N65</f>
         <v>77.403998131362243</v>
       </c>
-      <c r="H16" s="321"/>
+      <c r="H16" s="318"/>
       <c r="J16" s="30" t="s">
         <v>86</v>
       </c>
@@ -5616,18 +5633,18 @@
       <c r="B17" s="97" t="s">
         <v>164</v>
       </c>
-      <c r="C17" s="319" t="s">
+      <c r="C17" s="313" t="s">
         <v>165</v>
       </c>
-      <c r="D17" s="320"/>
+      <c r="D17" s="314"/>
       <c r="F17" s="154" t="s">
         <v>213</v>
       </c>
-      <c r="G17" s="325">
+      <c r="G17" s="317">
         <f>C8/SUM('Financial Model'!$K$3:$N$3)</f>
         <v>10.611405292999896</v>
       </c>
-      <c r="H17" s="321"/>
+      <c r="H17" s="318"/>
       <c r="K17" s="27" t="s">
         <v>84</v>
       </c>
@@ -5724,18 +5741,18 @@
       <c r="B18" s="85" t="s">
         <v>133</v>
       </c>
-      <c r="C18" s="302" t="s">
+      <c r="C18" s="323" t="s">
         <v>134</v>
       </c>
-      <c r="D18" s="303"/>
+      <c r="D18" s="316"/>
       <c r="F18" s="154" t="s">
         <v>214</v>
       </c>
-      <c r="G18" s="325">
+      <c r="G18" s="317">
         <f>C6/SUM('Financial Model'!K19:N19)</f>
         <v>-25.043163552931144</v>
       </c>
-      <c r="H18" s="321"/>
+      <c r="H18" s="318"/>
       <c r="K18" s="27" t="s">
         <v>85</v>
       </c>
@@ -5827,32 +5844,32 @@
     </row>
     <row r="19" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B19" s="83"/>
-      <c r="C19" s="308"/>
-      <c r="D19" s="303"/>
+      <c r="C19" s="315"/>
+      <c r="D19" s="316"/>
       <c r="F19" s="154" t="s">
         <v>218</v>
       </c>
-      <c r="G19" s="325">
+      <c r="G19" s="317">
         <f>C12/SUM('Financial Model'!K3:N3)</f>
         <v>9.7177228082759441</v>
       </c>
-      <c r="H19" s="321"/>
+      <c r="H19" s="318"/>
       <c r="K19" s="27"/>
       <c r="L19" s="57"/>
       <c r="M19" s="57"/>
     </row>
     <row r="20" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B20" s="84"/>
-      <c r="C20" s="322"/>
-      <c r="D20" s="323"/>
+      <c r="C20" s="321"/>
+      <c r="D20" s="322"/>
       <c r="F20" s="155" t="s">
         <v>320</v>
       </c>
-      <c r="G20" s="326">
+      <c r="G20" s="319">
         <f>C12/'Financial Model'!X34</f>
         <v>7.5281590226056059</v>
       </c>
-      <c r="H20" s="327"/>
+      <c r="H20" s="320"/>
       <c r="J20" s="30"/>
       <c r="K20" s="171" t="s">
         <v>212</v>
@@ -5883,14 +5900,14 @@
       </c>
     </row>
     <row r="23" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B23" s="304" t="s">
+      <c r="B23" s="310" t="s">
         <v>159</v>
       </c>
-      <c r="C23" s="305"/>
-      <c r="D23" s="305"/>
-      <c r="E23" s="305"/>
-      <c r="F23" s="305"/>
-      <c r="G23" s="306"/>
+      <c r="C23" s="311"/>
+      <c r="D23" s="311"/>
+      <c r="E23" s="311"/>
+      <c r="F23" s="311"/>
+      <c r="G23" s="312"/>
       <c r="K23" s="171" t="s">
         <v>209</v>
       </c>
@@ -6011,12 +6028,12 @@
       <c r="F31" s="94"/>
       <c r="G31" s="95"/>
       <c r="J31" s="7"/>
-      <c r="K31" s="304" t="s">
+      <c r="K31" s="310" t="s">
         <v>181</v>
       </c>
-      <c r="L31" s="305"/>
-      <c r="M31" s="305"/>
-      <c r="N31" s="306"/>
+      <c r="L31" s="311"/>
+      <c r="M31" s="311"/>
+      <c r="N31" s="312"/>
       <c r="P31" s="258" t="s">
         <v>290</v>
       </c>
@@ -6031,14 +6048,14 @@
       <c r="N32" s="89"/>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="304" t="s">
+      <c r="B33" s="310" t="s">
         <v>187</v>
       </c>
-      <c r="C33" s="305"/>
-      <c r="D33" s="305"/>
-      <c r="E33" s="305"/>
-      <c r="F33" s="305"/>
-      <c r="G33" s="306"/>
+      <c r="C33" s="311"/>
+      <c r="D33" s="311"/>
+      <c r="E33" s="311"/>
+      <c r="F33" s="311"/>
+      <c r="G33" s="312"/>
       <c r="J33" s="7"/>
       <c r="K33" s="147" t="s">
         <v>177</v>
@@ -6054,10 +6071,10 @@
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="179">
-        <v>44743</v>
-      </c>
-      <c r="C34" s="180" t="s">
-        <v>205</v>
+        <v>44986</v>
+      </c>
+      <c r="C34" s="329" t="s">
+        <v>321</v>
       </c>
       <c r="D34" s="88"/>
       <c r="E34" s="88"/>
@@ -6078,8 +6095,8 @@
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="141"/>
-      <c r="C35" s="181" t="s">
-        <v>206</v>
+      <c r="C35" s="330" t="s">
+        <v>322</v>
       </c>
       <c r="D35" s="88"/>
       <c r="E35" s="88"/>
@@ -6119,8 +6136,12 @@
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="141"/>
-      <c r="C37" s="88"/>
+      <c r="B37" s="179">
+        <v>44743</v>
+      </c>
+      <c r="C37" s="180" t="s">
+        <v>205</v>
+      </c>
       <c r="D37" s="88"/>
       <c r="E37" s="88"/>
       <c r="F37" s="88"/>
@@ -6138,7 +6159,9 @@
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="141"/>
-      <c r="C38" s="88"/>
+      <c r="C38" s="181" t="s">
+        <v>206</v>
+      </c>
       <c r="D38" s="88"/>
       <c r="E38" s="88"/>
       <c r="F38" s="88"/>
@@ -6569,6 +6592,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="L1:U1"/>
     <mergeCell ref="W1:AL1"/>
     <mergeCell ref="B33:G33"/>
@@ -6585,17 +6617,8 @@
     <mergeCell ref="B23:G23"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="G7:H7"/>
   </mergeCells>
-  <phoneticPr fontId="31" type="noConversion"/>
+  <phoneticPr fontId="32" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I67" r:id="rId1" xr:uid="{F79BC045-05D5-43FB-A051-BA2031CC85A7}"/>
     <hyperlink ref="I69" r:id="rId2" xr:uid="{58004FA9-9F7A-4B71-811E-FF4EE09F281F}"/>
@@ -6614,7 +6637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0FDCAC-3416-844A-BCBB-390EC350CF59}">
   <dimension ref="B1:BZ122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -10699,7 +10722,7 @@
         <f t="shared" ref="M35" si="98">M34/L34-1</f>
         <v>9.6574162918696915E-2</v>
       </c>
-      <c r="N35" s="328">
+      <c r="N35" s="303">
         <f>N34/M34-1</f>
         <v>0.28174433518597675</v>
       </c>
@@ -12362,12 +12385,12 @@
       <c r="P79" s="213"/>
     </row>
     <row r="80" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B80" s="324" t="s">
+      <c r="B80" s="302" t="s">
         <v>319</v>
       </c>
       <c r="F80" s="193"/>
       <c r="G80" s="193">
-        <f t="shared" ref="F80:M80" si="135">G73/SUM(D34:G34)</f>
+        <f t="shared" ref="G80:M80" si="135">G73/SUM(D34:G34)</f>
         <v>7.5570912427732031</v>
       </c>
       <c r="H80" s="193">
@@ -13601,7 +13624,7 @@
       <c r="B122" s="214"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="31" type="noConversion"/>
+  <phoneticPr fontId="32" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="L1" r:id="rId1" xr:uid="{F0F1B078-C7E3-AA47-9924-08C1D4511F24}"/>
     <hyperlink ref="M1" r:id="rId2" xr:uid="{9D82E829-DF9B-4456-A9EF-305989A97DF8}"/>
@@ -15007,7 +15030,7 @@
       <c r="S24" s="102"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="31" type="noConversion"/>
+  <phoneticPr fontId="32" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>